<commit_message>
Orga: Update Fahrplan (use real weeks)
</commit_message>
<xml_diff>
--- a/markdown/org/planung_pm.xlsx
+++ b/markdown/org/planung_pm.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1105" uniqueCount="279">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1106" uniqueCount="279">
   <si>
     <t>Thema</t>
   </si>
@@ -38459,7 +38459,9 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="44"/>
+      <c r="A2" s="44" t="s">
+        <v>133</v>
+      </c>
       <c r="B2" s="44">
         <v>14.0</v>
       </c>
@@ -38486,7 +38488,7 @@
     </row>
     <row r="3">
       <c r="A3" s="44" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="B3" s="44">
         <v>15.0</v>
@@ -38535,7 +38537,7 @@
     </row>
     <row r="4">
       <c r="A4" s="44" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="B4" s="44">
         <v>16.0</v>
@@ -38584,7 +38586,7 @@
     </row>
     <row r="5">
       <c r="A5" s="44" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="B5" s="44">
         <v>17.0</v>
@@ -38629,7 +38631,7 @@
     </row>
     <row r="6">
       <c r="A6" s="44" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="B6" s="44">
         <v>18.0</v>
@@ -38678,7 +38680,7 @@
     </row>
     <row r="7">
       <c r="A7" s="44" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="B7" s="44">
         <v>19.0</v>
@@ -38727,7 +38729,7 @@
     </row>
     <row r="8">
       <c r="A8" s="44" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="B8" s="44">
         <v>20.0</v>
@@ -38778,7 +38780,7 @@
     </row>
     <row r="9">
       <c r="A9" s="44" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="B9" s="44">
         <v>21.0</v>
@@ -38827,7 +38829,7 @@
     </row>
     <row r="10">
       <c r="A10" s="44" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="B10" s="44">
         <v>22.0</v>
@@ -38882,7 +38884,7 @@
     </row>
     <row r="11">
       <c r="A11" s="44" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="B11" s="44">
         <v>23.0</v>
@@ -38929,7 +38931,7 @@
     </row>
     <row r="12">
       <c r="A12" s="44" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="B12" s="44">
         <v>24.0</v>
@@ -38978,7 +38980,7 @@
     </row>
     <row r="13">
       <c r="A13" s="44" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="B13" s="44">
         <v>25.0</v>
@@ -39027,7 +39029,7 @@
     </row>
     <row r="14">
       <c r="A14" s="44" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="B14" s="44">
         <v>26.0</v>

</xml_diff>

<commit_message>
[Orga] Update Fahrplan - Zähle Vorlesungszeit-Wochen (#667)
* Orga: Update Fahrplan (use real weeks)

* Orga: Update Fahrplan (use real weeks)

* Orga: Update Fahrplan (use real weeks)
</commit_message>
<xml_diff>
--- a/markdown/org/planung_pm.xlsx
+++ b/markdown/org/planung_pm.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1105" uniqueCount="279">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1106" uniqueCount="279">
   <si>
     <t>Thema</t>
   </si>
@@ -38459,7 +38459,9 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="44"/>
+      <c r="A2" s="44" t="s">
+        <v>133</v>
+      </c>
       <c r="B2" s="44">
         <v>14.0</v>
       </c>
@@ -38486,7 +38488,7 @@
     </row>
     <row r="3">
       <c r="A3" s="44" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="B3" s="44">
         <v>15.0</v>
@@ -38535,7 +38537,7 @@
     </row>
     <row r="4">
       <c r="A4" s="44" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="B4" s="44">
         <v>16.0</v>
@@ -38584,7 +38586,7 @@
     </row>
     <row r="5">
       <c r="A5" s="44" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="B5" s="44">
         <v>17.0</v>
@@ -38629,7 +38631,7 @@
     </row>
     <row r="6">
       <c r="A6" s="44" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="B6" s="44">
         <v>18.0</v>
@@ -38678,7 +38680,7 @@
     </row>
     <row r="7">
       <c r="A7" s="44" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="B7" s="44">
         <v>19.0</v>
@@ -38727,7 +38729,7 @@
     </row>
     <row r="8">
       <c r="A8" s="44" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="B8" s="44">
         <v>20.0</v>
@@ -38778,7 +38780,7 @@
     </row>
     <row r="9">
       <c r="A9" s="44" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="B9" s="44">
         <v>21.0</v>
@@ -38827,7 +38829,7 @@
     </row>
     <row r="10">
       <c r="A10" s="44" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="B10" s="44">
         <v>22.0</v>
@@ -38882,7 +38884,7 @@
     </row>
     <row r="11">
       <c r="A11" s="44" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="B11" s="44">
         <v>23.0</v>
@@ -38929,7 +38931,7 @@
     </row>
     <row r="12">
       <c r="A12" s="44" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="B12" s="44">
         <v>24.0</v>
@@ -38978,7 +38980,7 @@
     </row>
     <row r="13">
       <c r="A13" s="44" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="B13" s="44">
         <v>25.0</v>
@@ -39027,7 +39029,7 @@
     </row>
     <row r="14">
       <c r="A14" s="44" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="B14" s="44">
         <v>26.0</v>

</xml_diff>

<commit_message>
Planung: Schiebe Optional nach vorn
</commit_message>
<xml_diff>
--- a/markdown/org/planung_pm.xlsx
+++ b/markdown/org/planung_pm.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1106" uniqueCount="279">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1107" uniqueCount="279">
   <si>
     <t>Thema</t>
   </si>
@@ -636,9 +636,6 @@
     <t>Karfreitag</t>
   </si>
   <si>
-    <t>ECS (Framework)</t>
-  </si>
-  <si>
     <t>Ostermontag</t>
   </si>
   <si>
@@ -646,19 +643,10 @@
 =&gt; Praktikum-Zeit (aber kein Praktikum)</t>
   </si>
   <si>
-    <t>Record-Klassen</t>
-  </si>
-  <si>
     <t>Zyklus 1: Konzept</t>
   </si>
   <si>
     <t>Zyklus 1: Code</t>
-  </si>
-  <si>
-    <t>Type-Object-Pattern</t>
-  </si>
-  <si>
-    <t>Zyklus 2: Konzept</t>
   </si>
   <si>
     <t>JUnit1: Intro</t>
@@ -673,7 +661,7 @@
     <t>JUnit4: Mocking (Mockito)</t>
   </si>
   <si>
-    <t>Zyklus 2: Code</t>
+    <t>Zyklus 2: Konzept</t>
   </si>
   <si>
     <t>Bad Smells</t>
@@ -682,11 +670,20 @@
     <t>Coding Rules und Metriken</t>
   </si>
   <si>
+    <t>Zyklus 2: Code</t>
+  </si>
+  <si>
     <t xml:space="preserve">Himmelfahrt
 </t>
   </si>
   <si>
     <t>Zyklus 3: Konzept</t>
+  </si>
+  <si>
+    <t>Serialisierung (equals, hashCode Wdhlg)</t>
+  </si>
+  <si>
+    <t>Record-Klassen</t>
   </si>
   <si>
     <t>Zyklus 3: Code</t>
@@ -734,9 +731,6 @@
     <t>Prüfungsphase</t>
   </si>
   <si>
-    <t>Serialisierung (equals, hashCode Wdhlg)</t>
-  </si>
-  <si>
     <t>Swing Basics</t>
   </si>
   <si>
@@ -752,7 +746,13 @@
     <t>Swing Tabellen</t>
   </si>
   <si>
+    <t>ECS (Framework)</t>
+  </si>
+  <si>
     <t>Build1: Ant</t>
+  </si>
+  <si>
+    <t>Type-Object-Pattern</t>
   </si>
   <si>
     <t>Einheit 8</t>
@@ -1223,7 +1223,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="98">
+  <cellXfs count="99">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
@@ -1380,12 +1380,6 @@
     <xf borderId="0" fillId="0" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
@@ -1401,14 +1395,14 @@
     <xf borderId="0" fillId="4" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
@@ -1417,6 +1411,9 @@
       <alignment horizontal="center" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="4" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -1439,9 +1436,6 @@
     </xf>
     <xf borderId="0" fillId="4" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="4" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
@@ -1469,6 +1463,15 @@
     </xf>
     <xf borderId="0" fillId="9" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="9" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
@@ -38509,11 +38512,11 @@
       <c r="H3" s="50">
         <v>25.0</v>
       </c>
-      <c r="I3" s="52" t="s">
-        <v>200</v>
-      </c>
-      <c r="J3" s="53">
-        <v>20.0</v>
+      <c r="I3" s="51" t="s">
+        <v>71</v>
+      </c>
+      <c r="J3" s="50">
+        <v>25.0</v>
       </c>
       <c r="K3" s="49" t="s">
         <v>54</v>
@@ -38526,13 +38529,13 @@
       <c r="O3" s="23"/>
       <c r="P3" s="22">
         <f t="shared" ref="P3:P14" si="1">SUM(D3,F3,H3,J3,L3,N3)</f>
-        <v>80</v>
-      </c>
-      <c r="R3" s="54" t="s">
+        <v>85</v>
+      </c>
+      <c r="R3" s="52" t="s">
+        <v>200</v>
+      </c>
+      <c r="S3" s="53" t="s">
         <v>201</v>
-      </c>
-      <c r="S3" s="55" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="4">
@@ -38542,34 +38545,34 @@
       <c r="B4" s="44">
         <v>16.0</v>
       </c>
-      <c r="C4" s="56" t="s">
+      <c r="C4" s="54" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="57">
+      <c r="D4" s="55">
         <v>25.0</v>
       </c>
-      <c r="E4" s="56" t="s">
+      <c r="E4" s="54" t="s">
         <v>21</v>
       </c>
-      <c r="F4" s="57">
+      <c r="F4" s="55">
         <v>15.0</v>
       </c>
-      <c r="G4" s="58" t="s">
+      <c r="G4" s="56" t="s">
         <v>98</v>
       </c>
-      <c r="H4" s="57">
+      <c r="H4" s="55">
         <v>20.0</v>
       </c>
-      <c r="I4" s="59" t="s">
-        <v>203</v>
-      </c>
-      <c r="J4" s="57">
-        <v>15.0</v>
-      </c>
-      <c r="K4" s="56" t="s">
+      <c r="I4" s="54" t="s">
+        <v>73</v>
+      </c>
+      <c r="J4" s="55">
+        <v>25.0</v>
+      </c>
+      <c r="K4" s="54" t="s">
         <v>35</v>
       </c>
-      <c r="L4" s="57">
+      <c r="L4" s="55">
         <v>10.0</v>
       </c>
       <c r="M4" s="27"/>
@@ -38577,11 +38580,11 @@
       <c r="O4" s="23"/>
       <c r="P4" s="22">
         <f t="shared" si="1"/>
-        <v>85</v>
+        <v>95</v>
       </c>
       <c r="R4" s="23"/>
-      <c r="S4" s="60" t="s">
-        <v>204</v>
+      <c r="S4" s="57" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="5">
@@ -38604,13 +38607,13 @@
         <v>20.0</v>
       </c>
       <c r="G5" s="51" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="H5" s="50">
-        <v>25.0</v>
+        <v>20.0</v>
       </c>
       <c r="I5" s="51" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="J5" s="50">
         <v>25.0</v>
@@ -38622,11 +38625,11 @@
       <c r="O5" s="23"/>
       <c r="P5" s="22">
         <f t="shared" si="1"/>
-        <v>95</v>
-      </c>
-      <c r="R5" s="61"/>
-      <c r="S5" s="60" t="s">
-        <v>205</v>
+        <v>90</v>
+      </c>
+      <c r="R5" s="58"/>
+      <c r="S5" s="57" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="6">
@@ -38637,31 +38640,35 @@
         <v>18.0</v>
       </c>
       <c r="C6" s="56" t="s">
-        <v>77</v>
-      </c>
-      <c r="D6" s="57">
-        <v>25.0</v>
-      </c>
-      <c r="E6" s="56" t="s">
-        <v>74</v>
-      </c>
-      <c r="F6" s="57">
+        <v>204</v>
+      </c>
+      <c r="D6" s="59">
         <v>20.0</v>
       </c>
-      <c r="G6" s="56" t="s">
+      <c r="E6" s="54" t="s">
+        <v>205</v>
+      </c>
+      <c r="F6" s="55">
+        <v>20.0</v>
+      </c>
+      <c r="G6" s="54" t="s">
+        <v>206</v>
+      </c>
+      <c r="H6" s="55">
+        <v>15.0</v>
+      </c>
+      <c r="I6" s="56" t="s">
+        <v>207</v>
+      </c>
+      <c r="J6" s="55">
+        <v>20.0</v>
+      </c>
+      <c r="K6" s="54" t="s">
         <v>52</v>
       </c>
-      <c r="H6" s="57">
+      <c r="L6" s="55">
         <v>20.0</v>
       </c>
-      <c r="I6" s="56" t="s">
-        <v>206</v>
-      </c>
-      <c r="J6" s="57">
-        <v>20.0</v>
-      </c>
-      <c r="K6" s="56"/>
-      <c r="L6" s="57"/>
       <c r="M6" s="27" t="s">
         <v>181</v>
       </c>
@@ -38671,11 +38678,11 @@
       <c r="O6" s="23"/>
       <c r="P6" s="22">
         <f t="shared" si="1"/>
-        <v>85</v>
+        <v>95</v>
       </c>
       <c r="R6" s="23"/>
-      <c r="S6" s="60" t="s">
-        <v>207</v>
+      <c r="S6" s="57" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="7">
@@ -38685,46 +38692,42 @@
       <c r="B7" s="44">
         <v>19.0</v>
       </c>
-      <c r="C7" s="49" t="s">
-        <v>208</v>
-      </c>
-      <c r="D7" s="48">
+      <c r="C7" s="51" t="s">
+        <v>209</v>
+      </c>
+      <c r="D7" s="50">
+        <v>30.0</v>
+      </c>
+      <c r="E7" s="51" t="s">
+        <v>210</v>
+      </c>
+      <c r="F7" s="50">
+        <v>30.0</v>
+      </c>
+      <c r="G7" s="51" t="s">
+        <v>56</v>
+      </c>
+      <c r="H7" s="50">
         <v>20.0</v>
       </c>
-      <c r="E7" s="51" t="s">
-        <v>209</v>
-      </c>
-      <c r="F7" s="50">
-        <v>20.0</v>
-      </c>
-      <c r="G7" s="51" t="s">
-        <v>210</v>
-      </c>
-      <c r="H7" s="50">
-        <v>15.0</v>
-      </c>
       <c r="I7" s="49" t="s">
-        <v>211</v>
+        <v>99</v>
       </c>
       <c r="J7" s="50">
-        <v>20.0</v>
-      </c>
-      <c r="K7" s="51" t="s">
-        <v>42</v>
-      </c>
-      <c r="L7" s="50">
-        <v>20.0</v>
-      </c>
-      <c r="M7" s="62"/>
-      <c r="N7" s="63"/>
+        <v>10.0</v>
+      </c>
+      <c r="K7" s="51"/>
+      <c r="L7" s="50"/>
+      <c r="M7" s="60"/>
+      <c r="N7" s="61"/>
       <c r="O7" s="23"/>
       <c r="P7" s="22">
         <f t="shared" si="1"/>
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="R7" s="23"/>
-      <c r="S7" s="60" t="s">
-        <v>212</v>
+      <c r="S7" s="57" t="s">
+        <v>211</v>
       </c>
     </row>
     <row r="8">
@@ -38734,32 +38737,36 @@
       <c r="B8" s="44">
         <v>20.0</v>
       </c>
-      <c r="C8" s="56" t="s">
-        <v>213</v>
-      </c>
-      <c r="D8" s="57">
-        <v>30.0</v>
-      </c>
-      <c r="E8" s="56" t="s">
-        <v>214</v>
-      </c>
-      <c r="F8" s="57">
-        <v>30.0</v>
+      <c r="C8" s="54" t="s">
+        <v>59</v>
+      </c>
+      <c r="D8" s="55">
+        <v>20.0</v>
+      </c>
+      <c r="E8" s="54" t="s">
+        <v>62</v>
+      </c>
+      <c r="F8" s="55">
+        <v>10.0</v>
       </c>
       <c r="G8" s="56" t="s">
-        <v>56</v>
-      </c>
-      <c r="H8" s="57">
-        <v>20.0</v>
-      </c>
-      <c r="I8" s="58" t="s">
-        <v>99</v>
-      </c>
-      <c r="J8" s="57">
-        <v>10.0</v>
-      </c>
-      <c r="K8" s="56"/>
-      <c r="L8" s="57"/>
+        <v>63</v>
+      </c>
+      <c r="H8" s="55">
+        <v>15.0</v>
+      </c>
+      <c r="I8" s="54" t="s">
+        <v>66</v>
+      </c>
+      <c r="J8" s="55">
+        <v>15.0</v>
+      </c>
+      <c r="K8" s="56" t="s">
+        <v>87</v>
+      </c>
+      <c r="L8" s="55">
+        <v>25.0</v>
+      </c>
       <c r="M8" s="27" t="s">
         <v>181</v>
       </c>
@@ -38769,13 +38776,13 @@
       <c r="O8" s="23"/>
       <c r="P8" s="22">
         <f t="shared" si="1"/>
-        <v>90</v>
-      </c>
-      <c r="R8" s="64" t="s">
-        <v>215</v>
-      </c>
-      <c r="S8" s="60" t="s">
-        <v>216</v>
+        <v>85</v>
+      </c>
+      <c r="R8" s="62" t="s">
+        <v>212</v>
+      </c>
+      <c r="S8" s="57" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="9">
@@ -38785,46 +38792,42 @@
       <c r="B9" s="44">
         <v>21.0</v>
       </c>
-      <c r="C9" s="51" t="s">
-        <v>59</v>
+      <c r="C9" s="49" t="s">
+        <v>214</v>
       </c>
       <c r="D9" s="50">
+        <v>15.0</v>
+      </c>
+      <c r="E9" s="63" t="s">
+        <v>215</v>
+      </c>
+      <c r="F9" s="50">
+        <v>15.0</v>
+      </c>
+      <c r="G9" s="51" t="s">
+        <v>42</v>
+      </c>
+      <c r="H9" s="50">
         <v>20.0</v>
       </c>
-      <c r="E9" s="51" t="s">
-        <v>62</v>
-      </c>
-      <c r="F9" s="50">
-        <v>10.0</v>
-      </c>
-      <c r="G9" s="49" t="s">
-        <v>63</v>
-      </c>
-      <c r="H9" s="50">
-        <v>15.0</v>
-      </c>
       <c r="I9" s="51" t="s">
-        <v>66</v>
+        <v>100</v>
       </c>
       <c r="J9" s="50">
-        <v>15.0</v>
-      </c>
-      <c r="K9" s="51" t="s">
-        <v>100</v>
-      </c>
-      <c r="L9" s="50">
         <v>35.0</v>
       </c>
+      <c r="K9" s="51"/>
+      <c r="L9" s="50"/>
       <c r="M9" s="51"/>
       <c r="N9" s="50"/>
       <c r="O9" s="23"/>
       <c r="P9" s="22">
         <f t="shared" si="1"/>
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="R9" s="23"/>
-      <c r="S9" s="60" t="s">
-        <v>217</v>
+      <c r="S9" s="57" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="10">
@@ -38834,34 +38837,34 @@
       <c r="B10" s="44">
         <v>22.0</v>
       </c>
-      <c r="C10" s="56" t="s">
+      <c r="C10" s="54" t="s">
         <v>68</v>
       </c>
-      <c r="D10" s="57">
+      <c r="D10" s="55">
         <v>15.0</v>
       </c>
-      <c r="E10" s="56" t="s">
+      <c r="E10" s="54" t="s">
         <v>79</v>
       </c>
-      <c r="F10" s="57">
+      <c r="F10" s="55">
         <v>35.0</v>
       </c>
-      <c r="G10" s="56" t="s">
+      <c r="G10" s="54" t="s">
         <v>29</v>
       </c>
-      <c r="H10" s="57">
+      <c r="H10" s="55">
         <v>20.0</v>
       </c>
-      <c r="I10" s="56" t="s">
+      <c r="I10" s="54" t="s">
         <v>32</v>
       </c>
-      <c r="J10" s="57">
+      <c r="J10" s="55">
         <v>15.0</v>
       </c>
-      <c r="K10" s="65" t="s">
-        <v>218</v>
-      </c>
-      <c r="L10" s="66">
+      <c r="K10" s="64" t="s">
+        <v>217</v>
+      </c>
+      <c r="L10" s="65">
         <v>10.0</v>
       </c>
       <c r="M10" s="27" t="s">
@@ -38875,11 +38878,11 @@
         <f t="shared" si="1"/>
         <v>95</v>
       </c>
-      <c r="R10" s="67" t="s">
+      <c r="R10" s="66" t="s">
+        <v>218</v>
+      </c>
+      <c r="S10" s="57" t="s">
         <v>219</v>
-      </c>
-      <c r="S10" s="60" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="11">
@@ -38908,7 +38911,7 @@
         <v>35.0</v>
       </c>
       <c r="I11" s="49" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="J11" s="50">
         <v>10.0</v>
@@ -38917,16 +38920,16 @@
       <c r="L11" s="50"/>
       <c r="M11" s="51"/>
       <c r="N11" s="50"/>
-      <c r="O11" s="63"/>
+      <c r="O11" s="61"/>
       <c r="P11" s="22">
         <f t="shared" si="1"/>
         <v>90</v>
       </c>
-      <c r="R11" s="64" t="s">
+      <c r="R11" s="62" t="s">
+        <v>221</v>
+      </c>
+      <c r="S11" s="57" t="s">
         <v>222</v>
-      </c>
-      <c r="S11" s="60" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="12">
@@ -38936,46 +38939,46 @@
       <c r="B12" s="44">
         <v>24.0</v>
       </c>
-      <c r="C12" s="58" t="s">
+      <c r="C12" s="56" t="s">
         <v>82</v>
       </c>
-      <c r="D12" s="57">
+      <c r="D12" s="55">
         <v>15.0</v>
       </c>
-      <c r="E12" s="58" t="s">
+      <c r="E12" s="56" t="s">
+        <v>223</v>
+      </c>
+      <c r="F12" s="55">
+        <v>25.0</v>
+      </c>
+      <c r="G12" s="37" t="s">
         <v>224</v>
-      </c>
-      <c r="F12" s="57">
-        <v>25.0</v>
-      </c>
-      <c r="G12" s="37" t="s">
-        <v>225</v>
       </c>
       <c r="H12" s="36">
         <v>15.0</v>
       </c>
-      <c r="I12" s="68" t="s">
+      <c r="I12" s="67" t="s">
+        <v>225</v>
+      </c>
+      <c r="J12" s="68">
+        <v>20.0</v>
+      </c>
+      <c r="K12" s="64" t="s">
         <v>226</v>
       </c>
-      <c r="J12" s="69">
-        <v>20.0</v>
-      </c>
-      <c r="K12" s="65" t="s">
-        <v>227</v>
-      </c>
-      <c r="L12" s="70">
+      <c r="L12" s="69">
         <v>15.0</v>
       </c>
-      <c r="M12" s="56"/>
-      <c r="N12" s="57"/>
+      <c r="M12" s="54"/>
+      <c r="N12" s="55"/>
       <c r="O12" s="23"/>
       <c r="P12" s="22">
         <f t="shared" si="1"/>
         <v>90</v>
       </c>
       <c r="R12" s="23"/>
-      <c r="S12" s="60" t="s">
-        <v>228</v>
+      <c r="S12" s="57" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="13">
@@ -39015,16 +39018,16 @@
       <c r="L13" s="50">
         <v>15.0</v>
       </c>
-      <c r="M13" s="62"/>
-      <c r="N13" s="63"/>
+      <c r="M13" s="60"/>
+      <c r="N13" s="61"/>
       <c r="O13" s="23"/>
       <c r="P13" s="22">
         <f t="shared" si="1"/>
         <v>85</v>
       </c>
       <c r="R13" s="23"/>
-      <c r="S13" s="60" t="s">
-        <v>229</v>
+      <c r="S13" s="57" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="14">
@@ -39034,30 +39037,30 @@
       <c r="B14" s="44">
         <v>26.0</v>
       </c>
-      <c r="C14" s="71" t="s">
+      <c r="C14" s="70" t="s">
         <v>13</v>
       </c>
-      <c r="D14" s="72"/>
-      <c r="E14" s="71" t="s">
+      <c r="D14" s="59"/>
+      <c r="E14" s="70" t="s">
         <v>14</v>
       </c>
-      <c r="F14" s="72"/>
-      <c r="G14" s="56"/>
-      <c r="H14" s="57"/>
-      <c r="I14" s="58"/>
-      <c r="J14" s="57"/>
-      <c r="K14" s="58"/>
-      <c r="L14" s="57"/>
-      <c r="M14" s="73"/>
-      <c r="N14" s="74"/>
+      <c r="F14" s="59"/>
+      <c r="G14" s="54"/>
+      <c r="H14" s="55"/>
+      <c r="I14" s="56"/>
+      <c r="J14" s="55"/>
+      <c r="K14" s="56"/>
+      <c r="L14" s="55"/>
+      <c r="M14" s="71"/>
+      <c r="N14" s="72"/>
       <c r="O14" s="23"/>
       <c r="P14" s="22">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R14" s="23"/>
-      <c r="S14" s="75" t="s">
-        <v>230</v>
+      <c r="S14" s="73" t="s">
+        <v>229</v>
       </c>
     </row>
     <row r="15">
@@ -39065,8 +39068,8 @@
       <c r="B15" s="44">
         <v>27.0</v>
       </c>
-      <c r="C15" s="76" t="s">
-        <v>231</v>
+      <c r="C15" s="74" t="s">
+        <v>230</v>
       </c>
       <c r="D15" s="29" t="s">
         <v>181</v>
@@ -39111,8 +39114,8 @@
       <c r="B16" s="44">
         <v>28.0</v>
       </c>
-      <c r="C16" s="76" t="s">
-        <v>231</v>
+      <c r="C16" s="74" t="s">
+        <v>230</v>
       </c>
       <c r="D16" s="29"/>
       <c r="E16" s="28" t="s">
@@ -39164,30 +39167,26 @@
     <row r="20">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
-      <c r="C20" s="58"/>
-      <c r="D20" s="57"/>
-      <c r="E20" s="58"/>
-      <c r="F20" s="57"/>
-      <c r="G20" s="58"/>
-      <c r="H20" s="57"/>
-      <c r="I20" s="56"/>
-      <c r="J20" s="57"/>
-      <c r="K20" s="58"/>
-      <c r="L20" s="57"/>
-      <c r="M20" s="58"/>
-      <c r="N20" s="57"/>
+      <c r="C20" s="56"/>
+      <c r="D20" s="55"/>
+      <c r="E20" s="56"/>
+      <c r="F20" s="55"/>
+      <c r="G20" s="56"/>
+      <c r="H20" s="55"/>
+      <c r="I20" s="54"/>
+      <c r="J20" s="55"/>
+      <c r="K20" s="56"/>
+      <c r="L20" s="55"/>
+      <c r="M20" s="56"/>
+      <c r="N20" s="55"/>
       <c r="O20" s="27"/>
       <c r="P20" s="27"/>
     </row>
     <row r="21">
       <c r="A21" s="4"/>
       <c r="B21" s="4"/>
-      <c r="C21" s="77" t="s">
-        <v>87</v>
-      </c>
-      <c r="D21" s="78">
-        <v>25.0</v>
-      </c>
+      <c r="C21" s="75"/>
+      <c r="D21" s="76"/>
       <c r="E21" s="49" t="s">
         <v>24</v>
       </c>
@@ -39200,70 +39199,66 @@
       <c r="H21" s="50">
         <v>15.0</v>
       </c>
-      <c r="I21" s="49" t="s">
-        <v>232</v>
-      </c>
-      <c r="J21" s="50">
-        <v>15.0</v>
-      </c>
+      <c r="I21" s="49"/>
+      <c r="J21" s="50"/>
       <c r="K21" s="49" t="s">
         <v>107</v>
       </c>
       <c r="L21" s="50">
         <v>15.0</v>
       </c>
-      <c r="M21" s="79" t="s">
+      <c r="M21" s="77" t="s">
         <v>181</v>
       </c>
-      <c r="N21" s="80" t="s">
+      <c r="N21" s="78" t="s">
         <v>181</v>
       </c>
-      <c r="O21" s="81"/>
+      <c r="O21" s="79"/>
       <c r="P21" s="22">
         <f t="shared" ref="P21:P24" si="2">SUM(D21,F21,H21,J21,L21,N21)</f>
-        <v>75</v>
+        <v>35</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
-      <c r="C22" s="58" t="s">
+      <c r="C22" s="56" t="s">
+        <v>231</v>
+      </c>
+      <c r="D22" s="55">
+        <v>10.0</v>
+      </c>
+      <c r="E22" s="56" t="s">
+        <v>232</v>
+      </c>
+      <c r="F22" s="55">
+        <v>10.0</v>
+      </c>
+      <c r="G22" s="56" t="s">
         <v>233</v>
       </c>
-      <c r="D22" s="57">
-        <v>10.0</v>
-      </c>
-      <c r="E22" s="58" t="s">
+      <c r="H22" s="55">
+        <v>15.0</v>
+      </c>
+      <c r="I22" s="56" t="s">
         <v>234</v>
       </c>
-      <c r="F22" s="57">
-        <v>10.0</v>
-      </c>
-      <c r="G22" s="58" t="s">
+      <c r="J22" s="55">
+        <v>15.0</v>
+      </c>
+      <c r="K22" s="56" t="s">
         <v>235</v>
       </c>
-      <c r="H22" s="57">
+      <c r="L22" s="55">
         <v>15.0</v>
       </c>
-      <c r="I22" s="58" t="s">
-        <v>236</v>
-      </c>
-      <c r="J22" s="57">
-        <v>15.0</v>
-      </c>
-      <c r="K22" s="58" t="s">
-        <v>237</v>
-      </c>
-      <c r="L22" s="57">
-        <v>15.0</v>
-      </c>
-      <c r="M22" s="58" t="s">
+      <c r="M22" s="56" t="s">
         <v>93</v>
       </c>
-      <c r="N22" s="57">
+      <c r="N22" s="55">
         <v>30.0</v>
       </c>
-      <c r="O22" s="74"/>
+      <c r="O22" s="72"/>
       <c r="P22" s="22">
         <f t="shared" si="2"/>
         <v>95</v>
@@ -39280,11 +39275,15 @@
       <c r="D23" s="50">
         <v>20.0</v>
       </c>
-      <c r="E23" s="51"/>
-      <c r="F23" s="50"/>
+      <c r="E23" s="80" t="s">
+        <v>236</v>
+      </c>
+      <c r="F23" s="81">
+        <v>20.0</v>
+      </c>
       <c r="G23" s="49"/>
       <c r="H23" s="50"/>
-      <c r="I23" s="49"/>
+      <c r="I23" s="51"/>
       <c r="J23" s="50"/>
       <c r="K23" s="49"/>
       <c r="L23" s="50"/>
@@ -39293,7 +39292,7 @@
       <c r="O23" s="23"/>
       <c r="P23" s="22">
         <f t="shared" si="2"/>
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="R23" s="23"/>
       <c r="S23" s="23"/>
@@ -39307,28 +39306,36 @@
       <c r="D24" s="36">
         <v>20.0</v>
       </c>
-      <c r="E24" s="58" t="s">
+      <c r="E24" s="56" t="s">
+        <v>237</v>
+      </c>
+      <c r="F24" s="55">
+        <v>25.0</v>
+      </c>
+      <c r="G24" s="56" t="s">
+        <v>97</v>
+      </c>
+      <c r="H24" s="55">
+        <v>20.0</v>
+      </c>
+      <c r="I24" s="82" t="s">
+        <v>215</v>
+      </c>
+      <c r="J24" s="55">
+        <v>15.0</v>
+      </c>
+      <c r="K24" s="54" t="s">
         <v>238</v>
       </c>
-      <c r="F24" s="57">
-        <v>25.0</v>
-      </c>
-      <c r="G24" s="58" t="s">
-        <v>97</v>
-      </c>
-      <c r="H24" s="57">
+      <c r="L24" s="55">
         <v>20.0</v>
       </c>
-      <c r="I24" s="58"/>
-      <c r="J24" s="57"/>
-      <c r="K24" s="65"/>
-      <c r="L24" s="70"/>
-      <c r="M24" s="58"/>
-      <c r="N24" s="57"/>
-      <c r="O24" s="74"/>
+      <c r="M24" s="56"/>
+      <c r="N24" s="55"/>
+      <c r="O24" s="72"/>
       <c r="P24" s="22">
         <f t="shared" si="2"/>
-        <v>65</v>
+        <v>100</v>
       </c>
       <c r="R24" s="23"/>
       <c r="S24" s="23"/>
@@ -39344,8 +39351,8 @@
       <c r="B26" s="3"/>
       <c r="E26" s="32"/>
       <c r="F26" s="33"/>
-      <c r="I26" s="77"/>
-      <c r="J26" s="78"/>
+      <c r="I26" s="75"/>
+      <c r="J26" s="76"/>
       <c r="R26" s="23"/>
       <c r="S26" s="23"/>
     </row>
@@ -42593,35 +42600,35 @@
       <c r="A2" s="4" t="s">
         <v>243</v>
       </c>
-      <c r="B2" s="82" t="s">
+      <c r="B2" s="83" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="83">
+      <c r="C2" s="84">
         <v>45.0</v>
       </c>
-      <c r="D2" s="82" t="s">
+      <c r="D2" s="83" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="83">
+      <c r="E2" s="84">
         <v>20.0</v>
       </c>
-      <c r="F2" s="82" t="s">
+      <c r="F2" s="83" t="s">
         <v>18</v>
       </c>
-      <c r="G2" s="83">
+      <c r="G2" s="84">
         <v>25.0</v>
       </c>
-      <c r="H2" s="84"/>
-      <c r="I2" s="85"/>
-      <c r="J2" s="84"/>
-      <c r="K2" s="85"/>
-      <c r="L2" s="84"/>
-      <c r="M2" s="85"/>
-      <c r="N2" s="84"/>
-      <c r="O2" s="85"/>
-      <c r="P2" s="81"/>
-      <c r="Q2" s="85"/>
-      <c r="R2" s="81"/>
+      <c r="H2" s="85"/>
+      <c r="I2" s="86"/>
+      <c r="J2" s="85"/>
+      <c r="K2" s="86"/>
+      <c r="L2" s="85"/>
+      <c r="M2" s="86"/>
+      <c r="N2" s="85"/>
+      <c r="O2" s="86"/>
+      <c r="P2" s="79"/>
+      <c r="Q2" s="86"/>
+      <c r="R2" s="79"/>
       <c r="S2" s="22">
         <f t="shared" ref="S2:S17" si="1">SUM(C2,E2,G2,I2,K2,M2,O2,Q2)</f>
         <v>90</v>
@@ -42641,43 +42648,43 @@
       <c r="A3" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="B3" s="82" t="s">
+      <c r="B3" s="83" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="83">
+      <c r="C3" s="84">
         <v>25.0</v>
       </c>
-      <c r="D3" s="82" t="s">
+      <c r="D3" s="83" t="s">
         <v>21</v>
       </c>
-      <c r="E3" s="83">
+      <c r="E3" s="84">
         <v>15.0</v>
       </c>
-      <c r="F3" s="82" t="s">
+      <c r="F3" s="83" t="s">
         <v>22</v>
       </c>
-      <c r="G3" s="83">
+      <c r="G3" s="84">
         <v>25.0</v>
       </c>
-      <c r="H3" s="82" t="s">
+      <c r="H3" s="83" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="83">
+      <c r="I3" s="84">
         <v>10.0</v>
       </c>
-      <c r="J3" s="82" t="s">
+      <c r="J3" s="83" t="s">
         <v>52</v>
       </c>
-      <c r="K3" s="83">
+      <c r="K3" s="84">
         <v>20.0</v>
       </c>
-      <c r="L3" s="81"/>
-      <c r="M3" s="85"/>
-      <c r="N3" s="81"/>
-      <c r="O3" s="85"/>
-      <c r="P3" s="81"/>
-      <c r="Q3" s="85"/>
-      <c r="R3" s="81"/>
+      <c r="L3" s="79"/>
+      <c r="M3" s="86"/>
+      <c r="N3" s="79"/>
+      <c r="O3" s="86"/>
+      <c r="P3" s="79"/>
+      <c r="Q3" s="86"/>
+      <c r="R3" s="79"/>
       <c r="S3" s="22">
         <f t="shared" si="1"/>
         <v>95</v>
@@ -42697,16 +42704,16 @@
       <c r="A4" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="B4" s="86" t="s">
+      <c r="B4" s="87" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="74">
+      <c r="C4" s="72">
         <v>20.0</v>
       </c>
-      <c r="D4" s="86" t="s">
+      <c r="D4" s="87" t="s">
         <v>54</v>
       </c>
-      <c r="E4" s="74">
+      <c r="E4" s="72">
         <v>15.0</v>
       </c>
       <c r="F4" s="35"/>
@@ -42739,10 +42746,10 @@
       <c r="U4" s="21">
         <v>15.0</v>
       </c>
-      <c r="V4" s="61" t="s">
+      <c r="V4" s="58" t="s">
         <v>136</v>
       </c>
-      <c r="W4" s="62" t="s">
+      <c r="W4" s="60" t="s">
         <v>246</v>
       </c>
     </row>
@@ -42750,53 +42757,53 @@
       <c r="A5" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="B5" s="82" t="s">
+      <c r="B5" s="83" t="s">
         <v>59</v>
       </c>
-      <c r="C5" s="83">
+      <c r="C5" s="84">
         <v>20.0</v>
       </c>
-      <c r="D5" s="82" t="s">
+      <c r="D5" s="83" t="s">
         <v>62</v>
       </c>
-      <c r="E5" s="83">
+      <c r="E5" s="84">
         <v>10.0</v>
       </c>
-      <c r="F5" s="82" t="s">
+      <c r="F5" s="83" t="s">
         <v>63</v>
       </c>
-      <c r="G5" s="83">
+      <c r="G5" s="84">
         <v>15.0</v>
       </c>
-      <c r="H5" s="82" t="s">
+      <c r="H5" s="83" t="s">
         <v>66</v>
       </c>
-      <c r="I5" s="83">
+      <c r="I5" s="84">
         <v>15.0</v>
       </c>
-      <c r="J5" s="82" t="s">
+      <c r="J5" s="83" t="s">
         <v>35</v>
       </c>
-      <c r="K5" s="83">
+      <c r="K5" s="84">
         <v>10.0</v>
       </c>
-      <c r="L5" s="81" t="s">
+      <c r="L5" s="79" t="s">
         <v>181</v>
       </c>
-      <c r="M5" s="85" t="s">
+      <c r="M5" s="86" t="s">
         <v>181</v>
       </c>
-      <c r="N5" s="81" t="s">
+      <c r="N5" s="79" t="s">
         <v>181</v>
       </c>
-      <c r="O5" s="85" t="s">
+      <c r="O5" s="86" t="s">
         <v>181</v>
       </c>
-      <c r="P5" s="81"/>
-      <c r="Q5" s="85" t="s">
+      <c r="P5" s="79"/>
+      <c r="Q5" s="86" t="s">
         <v>181</v>
       </c>
-      <c r="R5" s="81"/>
+      <c r="R5" s="79"/>
       <c r="S5" s="22">
         <f t="shared" si="1"/>
         <v>70</v>
@@ -42807,10 +42814,10 @@
       <c r="V5" s="23" t="s">
         <v>140</v>
       </c>
-      <c r="W5" s="62" t="s">
+      <c r="W5" s="60" t="s">
         <v>247</v>
       </c>
-      <c r="X5" s="62" t="s">
+      <c r="X5" s="60" t="s">
         <v>248</v>
       </c>
     </row>
@@ -42818,38 +42825,38 @@
       <c r="A6" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="B6" s="86" t="s">
+      <c r="B6" s="87" t="s">
         <v>98</v>
       </c>
-      <c r="C6" s="74">
+      <c r="C6" s="72">
         <v>20.0</v>
       </c>
-      <c r="D6" s="73" t="s">
+      <c r="D6" s="71" t="s">
         <v>99</v>
       </c>
-      <c r="E6" s="74">
+      <c r="E6" s="72">
         <v>10.0</v>
       </c>
-      <c r="F6" s="86" t="s">
-        <v>208</v>
-      </c>
-      <c r="G6" s="74">
+      <c r="F6" s="87" t="s">
+        <v>204</v>
+      </c>
+      <c r="G6" s="72">
         <v>25.0</v>
       </c>
-      <c r="H6" s="86" t="s">
-        <v>209</v>
-      </c>
-      <c r="I6" s="74">
+      <c r="H6" s="87" t="s">
+        <v>205</v>
+      </c>
+      <c r="I6" s="72">
         <v>20.0</v>
       </c>
-      <c r="J6" s="86" t="s">
-        <v>210</v>
-      </c>
-      <c r="K6" s="74">
+      <c r="J6" s="87" t="s">
+        <v>206</v>
+      </c>
+      <c r="K6" s="72">
         <v>15.0</v>
       </c>
-      <c r="L6" s="73"/>
-      <c r="M6" s="74"/>
+      <c r="L6" s="71"/>
+      <c r="M6" s="72"/>
       <c r="N6" s="27" t="s">
         <v>181</v>
       </c>
@@ -42869,10 +42876,10 @@
         <v>17.0</v>
       </c>
       <c r="V6" s="23"/>
-      <c r="W6" s="62" t="s">
+      <c r="W6" s="60" t="s">
         <v>249</v>
       </c>
-      <c r="X6" s="62" t="s">
+      <c r="X6" s="60" t="s">
         <v>250</v>
       </c>
     </row>
@@ -42880,49 +42887,49 @@
       <c r="A7" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="B7" s="82" t="s">
-        <v>213</v>
-      </c>
-      <c r="C7" s="83">
+      <c r="B7" s="83" t="s">
+        <v>209</v>
+      </c>
+      <c r="C7" s="84">
         <v>30.0</v>
       </c>
-      <c r="D7" s="82" t="s">
-        <v>214</v>
-      </c>
-      <c r="E7" s="83">
+      <c r="D7" s="83" t="s">
+        <v>210</v>
+      </c>
+      <c r="E7" s="84">
         <v>30.0</v>
       </c>
-      <c r="F7" s="82" t="s">
+      <c r="F7" s="83" t="s">
         <v>56</v>
       </c>
-      <c r="G7" s="83">
+      <c r="G7" s="84">
         <v>20.0</v>
       </c>
-      <c r="H7" s="87" t="s">
-        <v>211</v>
-      </c>
-      <c r="I7" s="83">
+      <c r="H7" s="88" t="s">
+        <v>207</v>
+      </c>
+      <c r="I7" s="84">
         <v>20.0</v>
       </c>
-      <c r="J7" s="87"/>
-      <c r="K7" s="83"/>
-      <c r="L7" s="81" t="s">
+      <c r="J7" s="88"/>
+      <c r="K7" s="84"/>
+      <c r="L7" s="79" t="s">
         <v>181</v>
       </c>
-      <c r="M7" s="85" t="s">
+      <c r="M7" s="86" t="s">
         <v>181</v>
       </c>
-      <c r="N7" s="81" t="s">
+      <c r="N7" s="79" t="s">
         <v>181</v>
       </c>
-      <c r="O7" s="85" t="s">
+      <c r="O7" s="86" t="s">
         <v>181</v>
       </c>
-      <c r="P7" s="81"/>
-      <c r="Q7" s="85" t="s">
+      <c r="P7" s="79"/>
+      <c r="Q7" s="86" t="s">
         <v>181</v>
       </c>
-      <c r="R7" s="81"/>
+      <c r="R7" s="79"/>
       <c r="S7" s="22">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -42931,10 +42938,10 @@
         <v>18.0</v>
       </c>
       <c r="V7" s="23"/>
-      <c r="W7" s="62" t="s">
+      <c r="W7" s="60" t="s">
         <v>251</v>
       </c>
-      <c r="X7" s="62" t="s">
+      <c r="X7" s="60" t="s">
         <v>252</v>
       </c>
     </row>
@@ -42942,50 +42949,50 @@
       <c r="A8" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="B8" s="73" t="s">
+      <c r="B8" s="71" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="74">
+      <c r="C8" s="72">
         <v>5.0</v>
       </c>
-      <c r="D8" s="73" t="s">
+      <c r="D8" s="71" t="s">
         <v>57</v>
       </c>
-      <c r="E8" s="74">
+      <c r="E8" s="72">
         <v>15.0</v>
       </c>
-      <c r="F8" s="86" t="s">
+      <c r="F8" s="87" t="s">
         <v>82</v>
       </c>
-      <c r="G8" s="74">
+      <c r="G8" s="72">
         <v>15.0</v>
       </c>
-      <c r="H8" s="86" t="s">
-        <v>221</v>
-      </c>
-      <c r="I8" s="74">
+      <c r="H8" s="87" t="s">
+        <v>220</v>
+      </c>
+      <c r="I8" s="72">
         <v>10.0</v>
       </c>
-      <c r="J8" s="73" t="s">
+      <c r="J8" s="71" t="s">
         <v>43</v>
       </c>
-      <c r="K8" s="74">
+      <c r="K8" s="72">
         <v>20.0</v>
       </c>
-      <c r="L8" s="73" t="s">
-        <v>206</v>
-      </c>
-      <c r="M8" s="74">
+      <c r="L8" s="71" t="s">
+        <v>238</v>
+      </c>
+      <c r="M8" s="72">
         <v>20.0</v>
       </c>
-      <c r="N8" s="86" t="s">
+      <c r="N8" s="87" t="s">
         <v>32</v>
       </c>
-      <c r="O8" s="74">
+      <c r="O8" s="72">
         <v>15.0</v>
       </c>
       <c r="P8" s="27"/>
-      <c r="Q8" s="74"/>
+      <c r="Q8" s="72"/>
       <c r="R8" s="27"/>
       <c r="S8" s="22">
         <f t="shared" si="1"/>
@@ -42995,10 +43002,10 @@
         <v>19.0</v>
       </c>
       <c r="V8" s="23"/>
-      <c r="W8" s="62" t="s">
+      <c r="W8" s="60" t="s">
         <v>187</v>
       </c>
-      <c r="X8" s="62" t="s">
+      <c r="X8" s="60" t="s">
         <v>253</v>
       </c>
     </row>
@@ -43006,53 +43013,53 @@
       <c r="A9" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="B9" s="82" t="s">
+      <c r="B9" s="83" t="s">
         <v>84</v>
       </c>
-      <c r="C9" s="83">
+      <c r="C9" s="84">
         <v>20.0</v>
       </c>
-      <c r="D9" s="87" t="s">
+      <c r="D9" s="88" t="s">
         <v>86</v>
       </c>
-      <c r="E9" s="83">
+      <c r="E9" s="84">
         <v>25.0</v>
       </c>
-      <c r="F9" s="82" t="s">
+      <c r="F9" s="83" t="s">
         <v>38</v>
       </c>
-      <c r="G9" s="83">
+      <c r="G9" s="84">
         <v>15.0</v>
       </c>
-      <c r="H9" s="82" t="s">
-        <v>232</v>
-      </c>
-      <c r="I9" s="83">
+      <c r="H9" s="83" t="s">
+        <v>214</v>
+      </c>
+      <c r="I9" s="84">
         <v>15.0</v>
       </c>
-      <c r="J9" s="81" t="s">
+      <c r="J9" s="79" t="s">
         <v>181</v>
       </c>
-      <c r="K9" s="85" t="s">
+      <c r="K9" s="86" t="s">
         <v>181</v>
       </c>
-      <c r="L9" s="81" t="s">
+      <c r="L9" s="79" t="s">
         <v>181</v>
       </c>
-      <c r="M9" s="85" t="s">
+      <c r="M9" s="86" t="s">
         <v>181</v>
       </c>
-      <c r="N9" s="81" t="s">
+      <c r="N9" s="79" t="s">
         <v>181</v>
       </c>
-      <c r="O9" s="85" t="s">
+      <c r="O9" s="86" t="s">
         <v>181</v>
       </c>
-      <c r="P9" s="81"/>
-      <c r="Q9" s="85" t="s">
+      <c r="P9" s="79"/>
+      <c r="Q9" s="86" t="s">
         <v>181</v>
       </c>
-      <c r="R9" s="81"/>
+      <c r="R9" s="79"/>
       <c r="S9" s="22">
         <f t="shared" si="1"/>
         <v>75</v>
@@ -43061,10 +43068,10 @@
         <v>20.0</v>
       </c>
       <c r="V9" s="23"/>
-      <c r="W9" s="62" t="s">
+      <c r="W9" s="60" t="s">
         <v>254</v>
       </c>
-      <c r="X9" s="62" t="s">
+      <c r="X9" s="60" t="s">
         <v>255</v>
       </c>
     </row>
@@ -43072,51 +43079,51 @@
       <c r="A10" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="B10" s="88" t="s">
+      <c r="B10" s="89" t="s">
         <v>110</v>
       </c>
-      <c r="C10" s="74">
+      <c r="C10" s="72">
         <v>45.0</v>
       </c>
-      <c r="D10" s="73" t="s">
+      <c r="D10" s="71" t="s">
+        <v>231</v>
+      </c>
+      <c r="E10" s="72">
+        <v>10.0</v>
+      </c>
+      <c r="F10" s="71" t="s">
+        <v>232</v>
+      </c>
+      <c r="G10" s="72">
+        <v>10.0</v>
+      </c>
+      <c r="H10" s="71" t="s">
         <v>233</v>
       </c>
-      <c r="E10" s="74">
-        <v>10.0</v>
-      </c>
-      <c r="F10" s="73" t="s">
+      <c r="I10" s="72">
+        <v>15.0</v>
+      </c>
+      <c r="J10" s="71" t="s">
         <v>234</v>
       </c>
-      <c r="G10" s="74">
-        <v>10.0</v>
-      </c>
-      <c r="H10" s="73" t="s">
+      <c r="K10" s="72">
+        <v>15.0</v>
+      </c>
+      <c r="L10" s="71" t="s">
         <v>235</v>
       </c>
-      <c r="I10" s="74">
+      <c r="M10" s="72">
         <v>15.0</v>
       </c>
-      <c r="J10" s="73" t="s">
-        <v>236</v>
-      </c>
-      <c r="K10" s="74">
-        <v>15.0</v>
-      </c>
-      <c r="L10" s="73" t="s">
-        <v>237</v>
-      </c>
-      <c r="M10" s="74">
-        <v>15.0</v>
-      </c>
-      <c r="N10" s="73" t="s">
+      <c r="N10" s="71" t="s">
         <v>93</v>
       </c>
-      <c r="O10" s="74">
+      <c r="O10" s="72">
         <v>30.0</v>
       </c>
-      <c r="P10" s="73"/>
-      <c r="Q10" s="74"/>
-      <c r="R10" s="74"/>
+      <c r="P10" s="71"/>
+      <c r="Q10" s="72"/>
+      <c r="R10" s="72"/>
       <c r="S10" s="22">
         <f t="shared" si="1"/>
         <v>140</v>
@@ -43138,45 +43145,45 @@
       <c r="A11" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="B11" s="82" t="s">
+      <c r="B11" s="83" t="s">
         <v>71</v>
       </c>
-      <c r="C11" s="83">
+      <c r="C11" s="84">
         <v>25.0</v>
       </c>
-      <c r="D11" s="82" t="s">
+      <c r="D11" s="83" t="s">
         <v>73</v>
       </c>
-      <c r="E11" s="83">
+      <c r="E11" s="84">
         <v>25.0</v>
       </c>
-      <c r="F11" s="82" t="s">
+      <c r="F11" s="83" t="s">
         <v>68</v>
       </c>
-      <c r="G11" s="83">
+      <c r="G11" s="84">
         <v>15.0</v>
       </c>
-      <c r="H11" s="82" t="s">
+      <c r="H11" s="83" t="s">
         <v>79</v>
       </c>
-      <c r="I11" s="83">
+      <c r="I11" s="84">
         <v>35.0</v>
       </c>
-      <c r="J11" s="89"/>
-      <c r="K11" s="90"/>
-      <c r="L11" s="91"/>
-      <c r="M11" s="92"/>
-      <c r="N11" s="81" t="s">
+      <c r="J11" s="90"/>
+      <c r="K11" s="91"/>
+      <c r="L11" s="92"/>
+      <c r="M11" s="93"/>
+      <c r="N11" s="79" t="s">
         <v>181</v>
       </c>
-      <c r="O11" s="85" t="s">
+      <c r="O11" s="86" t="s">
         <v>181</v>
       </c>
-      <c r="P11" s="81"/>
-      <c r="Q11" s="85" t="s">
+      <c r="P11" s="79"/>
+      <c r="Q11" s="86" t="s">
         <v>181</v>
       </c>
-      <c r="R11" s="81"/>
+      <c r="R11" s="79"/>
       <c r="S11" s="22">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -43185,10 +43192,10 @@
         <v>22.0</v>
       </c>
       <c r="V11" s="23"/>
-      <c r="W11" s="62" t="s">
+      <c r="W11" s="60" t="s">
         <v>256</v>
       </c>
-      <c r="X11" s="62" t="s">
+      <c r="X11" s="60" t="s">
         <v>257</v>
       </c>
     </row>
@@ -43196,38 +43203,38 @@
       <c r="A12" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="B12" s="73" t="s">
+      <c r="B12" s="71" t="s">
         <v>76</v>
       </c>
-      <c r="C12" s="74">
+      <c r="C12" s="72">
         <v>15.0</v>
       </c>
-      <c r="D12" s="73" t="s">
+      <c r="D12" s="71" t="s">
         <v>74</v>
       </c>
-      <c r="E12" s="74">
+      <c r="E12" s="72">
         <v>20.0</v>
       </c>
-      <c r="F12" s="73" t="s">
+      <c r="F12" s="71" t="s">
         <v>77</v>
       </c>
-      <c r="G12" s="74">
+      <c r="G12" s="72">
         <v>25.0</v>
       </c>
-      <c r="H12" s="73" t="s">
+      <c r="H12" s="71" t="s">
         <v>29</v>
       </c>
-      <c r="I12" s="74">
+      <c r="I12" s="72">
         <v>20.0</v>
       </c>
-      <c r="J12" s="73" t="s">
+      <c r="J12" s="71" t="s">
         <v>42</v>
       </c>
-      <c r="K12" s="74">
+      <c r="K12" s="72">
         <v>20.0</v>
       </c>
-      <c r="L12" s="73"/>
-      <c r="M12" s="74"/>
+      <c r="L12" s="71"/>
+      <c r="M12" s="72"/>
       <c r="N12" s="27" t="s">
         <v>181</v>
       </c>
@@ -43249,10 +43256,10 @@
       <c r="V12" s="23" t="s">
         <v>162</v>
       </c>
-      <c r="W12" s="62" t="s">
+      <c r="W12" s="60" t="s">
         <v>190</v>
       </c>
-      <c r="X12" s="62" t="s">
+      <c r="X12" s="60" t="s">
         <v>258</v>
       </c>
     </row>
@@ -43260,49 +43267,49 @@
       <c r="A13" s="4" t="s">
         <v>169</v>
       </c>
-      <c r="B13" s="87" t="s">
+      <c r="B13" s="88" t="s">
         <v>102</v>
       </c>
-      <c r="C13" s="83">
+      <c r="C13" s="84">
         <v>20.0</v>
       </c>
-      <c r="D13" s="87" t="s">
+      <c r="D13" s="88" t="s">
         <v>103</v>
       </c>
-      <c r="E13" s="83">
+      <c r="E13" s="84">
         <v>25.0</v>
       </c>
-      <c r="F13" s="87" t="s">
+      <c r="F13" s="88" t="s">
         <v>104</v>
       </c>
-      <c r="G13" s="83">
+      <c r="G13" s="84">
         <v>15.0</v>
       </c>
-      <c r="H13" s="87" t="s">
+      <c r="H13" s="88" t="s">
         <v>89</v>
       </c>
-      <c r="I13" s="83">
+      <c r="I13" s="84">
         <v>35.0</v>
       </c>
-      <c r="J13" s="87" t="s">
+      <c r="J13" s="88" t="s">
         <v>107</v>
       </c>
-      <c r="K13" s="83">
+      <c r="K13" s="84">
         <v>15.0</v>
       </c>
-      <c r="L13" s="89"/>
-      <c r="M13" s="90"/>
-      <c r="N13" s="81" t="s">
+      <c r="L13" s="90"/>
+      <c r="M13" s="91"/>
+      <c r="N13" s="79" t="s">
         <v>181</v>
       </c>
-      <c r="O13" s="85" t="s">
+      <c r="O13" s="86" t="s">
         <v>181</v>
       </c>
-      <c r="P13" s="81"/>
-      <c r="Q13" s="85" t="s">
+      <c r="P13" s="79"/>
+      <c r="Q13" s="86" t="s">
         <v>181</v>
       </c>
-      <c r="R13" s="81"/>
+      <c r="R13" s="79"/>
       <c r="S13" s="22">
         <f t="shared" si="1"/>
         <v>110</v>
@@ -43313,10 +43320,10 @@
       <c r="V13" s="23" t="s">
         <v>166</v>
       </c>
-      <c r="W13" s="62" t="s">
+      <c r="W13" s="60" t="s">
         <v>259</v>
       </c>
-      <c r="X13" s="62" t="s">
+      <c r="X13" s="60" t="s">
         <v>260</v>
       </c>
     </row>
@@ -43324,28 +43331,28 @@
       <c r="A14" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="B14" s="73" t="s">
-        <v>224</v>
-      </c>
-      <c r="C14" s="74">
+      <c r="B14" s="71" t="s">
+        <v>223</v>
+      </c>
+      <c r="C14" s="72">
         <v>25.0</v>
       </c>
-      <c r="D14" s="73" t="s">
-        <v>238</v>
-      </c>
-      <c r="E14" s="74">
+      <c r="D14" s="71" t="s">
+        <v>237</v>
+      </c>
+      <c r="E14" s="72">
         <v>25.0</v>
       </c>
-      <c r="F14" s="73" t="s">
+      <c r="F14" s="71" t="s">
         <v>97</v>
       </c>
-      <c r="G14" s="74">
+      <c r="G14" s="72">
         <v>20.0</v>
       </c>
-      <c r="H14" s="73" t="s">
+      <c r="H14" s="71" t="s">
         <v>100</v>
       </c>
-      <c r="I14" s="74">
+      <c r="I14" s="72">
         <v>35.0</v>
       </c>
       <c r="J14" s="37"/>
@@ -43375,10 +43382,10 @@
         <v>25.0</v>
       </c>
       <c r="V14" s="23"/>
-      <c r="W14" s="62" t="s">
+      <c r="W14" s="60" t="s">
         <v>261</v>
       </c>
-      <c r="X14" s="62" t="s">
+      <c r="X14" s="60" t="s">
         <v>262</v>
       </c>
     </row>
@@ -43386,51 +43393,51 @@
       <c r="A15" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="B15" s="87" t="s">
+      <c r="B15" s="88" t="s">
         <v>87</v>
       </c>
-      <c r="C15" s="83">
+      <c r="C15" s="84">
         <v>25.0</v>
       </c>
-      <c r="D15" s="82" t="s">
+      <c r="D15" s="83" t="s">
         <v>13</v>
       </c>
-      <c r="E15" s="83"/>
-      <c r="F15" s="82" t="s">
+      <c r="E15" s="84"/>
+      <c r="F15" s="83" t="s">
         <v>14</v>
       </c>
-      <c r="G15" s="83">
+      <c r="G15" s="84">
         <v>35.0</v>
       </c>
-      <c r="H15" s="81" t="s">
+      <c r="H15" s="79" t="s">
         <v>181</v>
       </c>
-      <c r="I15" s="85" t="s">
+      <c r="I15" s="86" t="s">
         <v>181</v>
       </c>
-      <c r="J15" s="81" t="s">
+      <c r="J15" s="79" t="s">
         <v>181</v>
       </c>
-      <c r="K15" s="85" t="s">
+      <c r="K15" s="86" t="s">
         <v>181</v>
       </c>
-      <c r="L15" s="81" t="s">
+      <c r="L15" s="79" t="s">
         <v>181</v>
       </c>
-      <c r="M15" s="85" t="s">
+      <c r="M15" s="86" t="s">
         <v>181</v>
       </c>
-      <c r="N15" s="81" t="s">
+      <c r="N15" s="79" t="s">
         <v>181</v>
       </c>
-      <c r="O15" s="85" t="s">
+      <c r="O15" s="86" t="s">
         <v>181</v>
       </c>
-      <c r="P15" s="81"/>
-      <c r="Q15" s="85" t="s">
+      <c r="P15" s="79"/>
+      <c r="Q15" s="86" t="s">
         <v>181</v>
       </c>
-      <c r="R15" s="81"/>
+      <c r="R15" s="79"/>
       <c r="S15" s="22">
         <f t="shared" si="1"/>
         <v>60</v>
@@ -43438,7 +43445,7 @@
       <c r="U15" s="21">
         <v>26.0</v>
       </c>
-      <c r="X15" s="62" t="s">
+      <c r="X15" s="60" t="s">
         <v>263</v>
       </c>
     </row>
@@ -43574,10 +43581,10 @@
     </row>
     <row r="20">
       <c r="A20" s="3"/>
-      <c r="D20" s="93" t="s">
+      <c r="D20" s="94" t="s">
         <v>53</v>
       </c>
-      <c r="E20" s="94">
+      <c r="E20" s="95">
         <v>15.0</v>
       </c>
       <c r="U20" s="23"/>
@@ -43592,10 +43599,10 @@
     </row>
     <row r="21">
       <c r="A21" s="3"/>
-      <c r="D21" s="93" t="s">
+      <c r="D21" s="94" t="s">
         <v>106</v>
       </c>
-      <c r="E21" s="94">
+      <c r="E21" s="95">
         <v>20.0</v>
       </c>
       <c r="U21" s="23"/>
@@ -43607,10 +43614,10 @@
     </row>
     <row r="22">
       <c r="A22" s="3"/>
-      <c r="D22" s="93" t="s">
-        <v>225</v>
-      </c>
-      <c r="E22" s="94">
+      <c r="D22" s="94" t="s">
+        <v>224</v>
+      </c>
+      <c r="E22" s="95">
         <v>15.0</v>
       </c>
       <c r="U22" s="23"/>
@@ -46093,33 +46100,33 @@
       <c r="A2" s="4" t="s">
         <v>243</v>
       </c>
-      <c r="B2" s="84" t="s">
+      <c r="B2" s="85" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="85">
+      <c r="C2" s="86">
         <v>40.0</v>
       </c>
-      <c r="D2" s="84" t="s">
+      <c r="D2" s="85" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="85">
+      <c r="E2" s="86">
         <v>20.0</v>
       </c>
-      <c r="F2" s="84" t="s">
+      <c r="F2" s="85" t="s">
         <v>18</v>
       </c>
-      <c r="G2" s="85">
+      <c r="G2" s="86">
         <v>25.0</v>
       </c>
-      <c r="H2" s="84"/>
-      <c r="I2" s="85"/>
-      <c r="J2" s="84"/>
-      <c r="K2" s="85"/>
-      <c r="L2" s="84"/>
-      <c r="M2" s="85"/>
-      <c r="N2" s="84"/>
-      <c r="O2" s="85"/>
-      <c r="P2" s="81"/>
+      <c r="H2" s="85"/>
+      <c r="I2" s="86"/>
+      <c r="J2" s="85"/>
+      <c r="K2" s="86"/>
+      <c r="L2" s="85"/>
+      <c r="M2" s="86"/>
+      <c r="N2" s="85"/>
+      <c r="O2" s="86"/>
+      <c r="P2" s="79"/>
       <c r="Q2" s="22">
         <f t="shared" ref="Q2:Q17" si="1">SUM(C2,E2,G2,I2,K2,M2,O2)</f>
         <v>85</v>
@@ -46139,37 +46146,37 @@
       <c r="A3" s="4" t="s">
         <v>266</v>
       </c>
-      <c r="B3" s="84" t="s">
+      <c r="B3" s="85" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="85">
+      <c r="C3" s="86">
         <v>25.0</v>
       </c>
-      <c r="D3" s="84" t="s">
+      <c r="D3" s="85" t="s">
         <v>21</v>
       </c>
-      <c r="E3" s="85">
+      <c r="E3" s="86">
         <v>15.0</v>
       </c>
-      <c r="F3" s="84" t="s">
+      <c r="F3" s="85" t="s">
         <v>22</v>
       </c>
-      <c r="G3" s="85">
+      <c r="G3" s="86">
         <v>25.0</v>
       </c>
-      <c r="H3" s="84" t="s">
+      <c r="H3" s="85" t="s">
         <v>23</v>
       </c>
-      <c r="I3" s="85">
+      <c r="I3" s="86">
         <v>20.0</v>
       </c>
-      <c r="J3" s="84"/>
-      <c r="K3" s="85"/>
-      <c r="L3" s="81"/>
-      <c r="M3" s="85"/>
-      <c r="N3" s="81"/>
-      <c r="O3" s="85"/>
-      <c r="P3" s="81"/>
+      <c r="J3" s="85"/>
+      <c r="K3" s="86"/>
+      <c r="L3" s="79"/>
+      <c r="M3" s="86"/>
+      <c r="N3" s="79"/>
+      <c r="O3" s="86"/>
+      <c r="P3" s="79"/>
       <c r="Q3" s="22">
         <f t="shared" si="1"/>
         <v>85</v>
@@ -46219,7 +46226,7 @@
       <c r="S4" s="21">
         <v>15.0</v>
       </c>
-      <c r="T4" s="61" t="s">
+      <c r="T4" s="58" t="s">
         <v>136</v>
       </c>
       <c r="U4" s="23" t="s">
@@ -46230,49 +46237,49 @@
       <c r="A5" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="B5" s="84" t="s">
+      <c r="B5" s="85" t="s">
         <v>59</v>
       </c>
-      <c r="C5" s="85">
+      <c r="C5" s="86">
         <v>20.0</v>
       </c>
-      <c r="D5" s="84" t="s">
+      <c r="D5" s="85" t="s">
         <v>62</v>
       </c>
-      <c r="E5" s="85">
+      <c r="E5" s="86">
         <v>10.0</v>
       </c>
-      <c r="F5" s="84" t="s">
+      <c r="F5" s="85" t="s">
         <v>52</v>
       </c>
-      <c r="G5" s="85">
+      <c r="G5" s="86">
         <v>15.0</v>
       </c>
-      <c r="H5" s="84" t="s">
+      <c r="H5" s="85" t="s">
         <v>26</v>
       </c>
-      <c r="I5" s="85">
+      <c r="I5" s="86">
         <v>10.0</v>
       </c>
-      <c r="J5" s="84" t="s">
+      <c r="J5" s="85" t="s">
         <v>98</v>
       </c>
-      <c r="K5" s="85">
+      <c r="K5" s="86">
         <v>15.0</v>
       </c>
-      <c r="L5" s="91" t="s">
+      <c r="L5" s="92" t="s">
         <v>54</v>
       </c>
-      <c r="M5" s="92">
+      <c r="M5" s="93">
         <v>10.0</v>
       </c>
-      <c r="N5" s="81" t="s">
+      <c r="N5" s="79" t="s">
         <v>181</v>
       </c>
-      <c r="O5" s="85" t="s">
+      <c r="O5" s="86" t="s">
         <v>181</v>
       </c>
-      <c r="P5" s="81"/>
+      <c r="P5" s="79"/>
       <c r="Q5" s="22">
         <f t="shared" si="1"/>
         <v>80</v>
@@ -46283,7 +46290,7 @@
       <c r="T5" s="23" t="s">
         <v>140</v>
       </c>
-      <c r="U5" s="95" t="s">
+      <c r="U5" s="96" t="s">
         <v>268</v>
       </c>
       <c r="V5" s="23" t="s">
@@ -46356,41 +46363,41 @@
       <c r="A7" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="B7" s="84" t="s">
+      <c r="B7" s="85" t="s">
         <v>55</v>
       </c>
-      <c r="C7" s="85">
+      <c r="C7" s="86">
         <v>35.0</v>
       </c>
-      <c r="D7" s="84" t="s">
+      <c r="D7" s="85" t="s">
         <v>56</v>
       </c>
-      <c r="E7" s="85">
+      <c r="E7" s="86">
         <v>35.0</v>
       </c>
-      <c r="F7" s="96" t="s">
+      <c r="F7" s="97" t="s">
         <v>49</v>
       </c>
-      <c r="G7" s="92">
+      <c r="G7" s="93">
         <v>20.0</v>
       </c>
-      <c r="H7" s="96"/>
-      <c r="I7" s="92"/>
-      <c r="J7" s="96"/>
-      <c r="K7" s="92"/>
-      <c r="L7" s="81" t="s">
+      <c r="H7" s="97"/>
+      <c r="I7" s="93"/>
+      <c r="J7" s="97"/>
+      <c r="K7" s="93"/>
+      <c r="L7" s="79" t="s">
         <v>181</v>
       </c>
-      <c r="M7" s="85" t="s">
+      <c r="M7" s="86" t="s">
         <v>181</v>
       </c>
-      <c r="N7" s="81" t="s">
+      <c r="N7" s="79" t="s">
         <v>181</v>
       </c>
-      <c r="O7" s="85" t="s">
+      <c r="O7" s="86" t="s">
         <v>181</v>
       </c>
-      <c r="P7" s="81"/>
+      <c r="P7" s="79"/>
       <c r="Q7" s="22">
         <f t="shared" si="1"/>
         <v>90</v>
@@ -46472,49 +46479,49 @@
       <c r="A9" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="B9" s="84" t="s">
+      <c r="B9" s="85" t="s">
         <v>84</v>
       </c>
-      <c r="C9" s="85">
+      <c r="C9" s="86">
         <v>30.0</v>
       </c>
-      <c r="D9" s="81" t="s">
+      <c r="D9" s="79" t="s">
         <v>86</v>
       </c>
-      <c r="E9" s="85">
+      <c r="E9" s="86">
         <v>30.0</v>
       </c>
-      <c r="F9" s="91" t="s">
+      <c r="F9" s="92" t="s">
         <v>38</v>
       </c>
-      <c r="G9" s="92">
+      <c r="G9" s="93">
         <v>15.0</v>
       </c>
-      <c r="H9" s="81" t="s">
+      <c r="H9" s="79" t="s">
         <v>181</v>
       </c>
-      <c r="I9" s="85" t="s">
+      <c r="I9" s="86" t="s">
         <v>181</v>
       </c>
-      <c r="J9" s="81" t="s">
+      <c r="J9" s="79" t="s">
         <v>181</v>
       </c>
-      <c r="K9" s="85" t="s">
+      <c r="K9" s="86" t="s">
         <v>181</v>
       </c>
-      <c r="L9" s="81" t="s">
+      <c r="L9" s="79" t="s">
         <v>181</v>
       </c>
-      <c r="M9" s="85" t="s">
+      <c r="M9" s="86" t="s">
         <v>181</v>
       </c>
-      <c r="N9" s="81" t="s">
+      <c r="N9" s="79" t="s">
         <v>181</v>
       </c>
-      <c r="O9" s="85" t="s">
+      <c r="O9" s="86" t="s">
         <v>181</v>
       </c>
-      <c r="P9" s="81"/>
+      <c r="P9" s="79"/>
       <c r="Q9" s="22">
         <f t="shared" si="1"/>
         <v>75</v>
@@ -46534,7 +46541,7 @@
       <c r="A10" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="B10" s="97" t="s">
+      <c r="B10" s="98" t="s">
         <v>110</v>
       </c>
       <c r="C10" s="26">
@@ -46598,41 +46605,41 @@
       <c r="A11" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="B11" s="84" t="s">
+      <c r="B11" s="85" t="s">
         <v>71</v>
       </c>
-      <c r="C11" s="85">
+      <c r="C11" s="86">
         <v>10.0</v>
       </c>
-      <c r="D11" s="84" t="s">
+      <c r="D11" s="85" t="s">
         <v>73</v>
       </c>
-      <c r="E11" s="85">
+      <c r="E11" s="86">
         <v>25.0</v>
       </c>
-      <c r="F11" s="84" t="s">
+      <c r="F11" s="85" t="s">
         <v>68</v>
       </c>
-      <c r="G11" s="85">
+      <c r="G11" s="86">
         <v>20.0</v>
       </c>
-      <c r="H11" s="84" t="s">
+      <c r="H11" s="85" t="s">
         <v>79</v>
       </c>
-      <c r="I11" s="85">
+      <c r="I11" s="86">
         <v>35.0</v>
       </c>
-      <c r="J11" s="96"/>
-      <c r="K11" s="92"/>
-      <c r="L11" s="91"/>
-      <c r="M11" s="92"/>
-      <c r="N11" s="81" t="s">
+      <c r="J11" s="97"/>
+      <c r="K11" s="93"/>
+      <c r="L11" s="92"/>
+      <c r="M11" s="93"/>
+      <c r="N11" s="79" t="s">
         <v>181</v>
       </c>
-      <c r="O11" s="85" t="s">
+      <c r="O11" s="86" t="s">
         <v>181</v>
       </c>
-      <c r="P11" s="81"/>
+      <c r="P11" s="79"/>
       <c r="Q11" s="22">
         <f t="shared" si="1"/>
         <v>90</v>
@@ -46716,49 +46723,49 @@
       <c r="A13" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="B13" s="81" t="s">
+      <c r="B13" s="79" t="s">
         <v>102</v>
       </c>
-      <c r="C13" s="85">
+      <c r="C13" s="86">
         <v>10.0</v>
       </c>
-      <c r="D13" s="81" t="s">
+      <c r="D13" s="79" t="s">
         <v>103</v>
       </c>
-      <c r="E13" s="85">
+      <c r="E13" s="86">
         <v>25.0</v>
       </c>
-      <c r="F13" s="81" t="s">
+      <c r="F13" s="79" t="s">
         <v>104</v>
       </c>
-      <c r="G13" s="85">
+      <c r="G13" s="86">
         <v>25.0</v>
       </c>
-      <c r="H13" s="84" t="s">
+      <c r="H13" s="85" t="s">
         <v>82</v>
       </c>
-      <c r="I13" s="85">
+      <c r="I13" s="86">
         <v>15.0</v>
       </c>
-      <c r="J13" s="96" t="s">
+      <c r="J13" s="97" t="s">
         <v>89</v>
       </c>
-      <c r="K13" s="92">
+      <c r="K13" s="93">
         <v>15.0</v>
       </c>
-      <c r="L13" s="81" t="s">
+      <c r="L13" s="79" t="s">
         <v>181</v>
       </c>
-      <c r="M13" s="85" t="s">
+      <c r="M13" s="86" t="s">
         <v>181</v>
       </c>
-      <c r="N13" s="81" t="s">
+      <c r="N13" s="79" t="s">
         <v>181</v>
       </c>
-      <c r="O13" s="85" t="s">
+      <c r="O13" s="86" t="s">
         <v>181</v>
       </c>
-      <c r="P13" s="81"/>
+      <c r="P13" s="79"/>
       <c r="Q13" s="22">
         <f t="shared" si="1"/>
         <v>90</v>
@@ -46838,49 +46845,49 @@
       <c r="A15" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="B15" s="84" t="s">
+      <c r="B15" s="85" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="85">
+      <c r="C15" s="86">
         <v>20.0</v>
       </c>
-      <c r="D15" s="84" t="s">
+      <c r="D15" s="85" t="s">
         <v>14</v>
       </c>
-      <c r="E15" s="85">
+      <c r="E15" s="86">
         <v>20.0</v>
       </c>
-      <c r="F15" s="81" t="s">
+      <c r="F15" s="79" t="s">
         <v>181</v>
       </c>
-      <c r="G15" s="85" t="s">
+      <c r="G15" s="86" t="s">
         <v>181</v>
       </c>
-      <c r="H15" s="81" t="s">
+      <c r="H15" s="79" t="s">
         <v>181</v>
       </c>
-      <c r="I15" s="85" t="s">
+      <c r="I15" s="86" t="s">
         <v>181</v>
       </c>
-      <c r="J15" s="81" t="s">
+      <c r="J15" s="79" t="s">
         <v>181</v>
       </c>
-      <c r="K15" s="85" t="s">
+      <c r="K15" s="86" t="s">
         <v>181</v>
       </c>
-      <c r="L15" s="81" t="s">
+      <c r="L15" s="79" t="s">
         <v>181</v>
       </c>
-      <c r="M15" s="85" t="s">
+      <c r="M15" s="86" t="s">
         <v>181</v>
       </c>
-      <c r="N15" s="81" t="s">
+      <c r="N15" s="79" t="s">
         <v>181</v>
       </c>
-      <c r="O15" s="85" t="s">
+      <c r="O15" s="86" t="s">
         <v>181</v>
       </c>
-      <c r="P15" s="81"/>
+      <c r="P15" s="79"/>
       <c r="Q15" s="22">
         <f t="shared" si="1"/>
         <v>40</v>
@@ -47019,10 +47026,10 @@
     </row>
     <row r="20">
       <c r="A20" s="3"/>
-      <c r="D20" s="93" t="s">
+      <c r="D20" s="94" t="s">
         <v>53</v>
       </c>
-      <c r="E20" s="94">
+      <c r="E20" s="95">
         <v>15.0</v>
       </c>
       <c r="S20" s="23"/>
@@ -47037,10 +47044,10 @@
     </row>
     <row r="21">
       <c r="A21" s="3"/>
-      <c r="D21" s="93" t="s">
+      <c r="D21" s="94" t="s">
         <v>106</v>
       </c>
-      <c r="E21" s="94">
+      <c r="E21" s="95">
         <v>20.0</v>
       </c>
       <c r="S21" s="23"/>
@@ -47052,16 +47059,16 @@
     </row>
     <row r="22">
       <c r="A22" s="3"/>
-      <c r="D22" s="93" t="s">
+      <c r="D22" s="94" t="s">
         <v>100</v>
       </c>
-      <c r="E22" s="94">
+      <c r="E22" s="95">
         <v>20.0</v>
       </c>
-      <c r="H22" s="81"/>
-      <c r="I22" s="85"/>
-      <c r="J22" s="81"/>
-      <c r="K22" s="85"/>
+      <c r="H22" s="79"/>
+      <c r="I22" s="86"/>
+      <c r="J22" s="79"/>
+      <c r="K22" s="86"/>
       <c r="S22" s="23"/>
       <c r="T22" s="23"/>
       <c r="U22" s="23"/>

</xml_diff>

<commit_message>
Planung: vertausche Woche 7 und 8 (Generics und Records)
</commit_message>
<xml_diff>
--- a/markdown/org/planung_pm.xlsx
+++ b/markdown/org/planung_pm.xlsx
@@ -14,7 +14,7 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId10" roundtripDataSignature="AMtx7mgbOalCEPwh+hcac8TBvw+RzQJMFQ=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId10" roundtripDataSignature="AMtx7mj5OVWkoZnkcVI3qairug7y+dFYUg=="/>
     </ext>
   </extLst>
 </workbook>
@@ -673,17 +673,17 @@
     <t>Zyklus 2: Code</t>
   </si>
   <si>
+    <t>Serialisierung (equals, hashCode Wdhlg)</t>
+  </si>
+  <si>
+    <t>Record-Klassen</t>
+  </si>
+  <si>
     <t xml:space="preserve">Himmelfahrt
 </t>
   </si>
   <si>
     <t>Zyklus 3: Konzept</t>
-  </si>
-  <si>
-    <t>Serialisierung (equals, hashCode Wdhlg)</t>
-  </si>
-  <si>
-    <t>Record-Klassen</t>
   </si>
   <si>
     <t>Zyklus 3: Code</t>
@@ -1223,7 +1223,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="99">
+  <cellXfs count="98">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
@@ -1410,10 +1410,10 @@
     <xf borderId="0" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="4" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="4" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -1469,9 +1469,6 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="9" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
@@ -38737,36 +38734,32 @@
       <c r="B8" s="44">
         <v>20.0</v>
       </c>
-      <c r="C8" s="54" t="s">
-        <v>59</v>
+      <c r="C8" s="56" t="s">
+        <v>212</v>
       </c>
       <c r="D8" s="55">
+        <v>15.0</v>
+      </c>
+      <c r="E8" s="62" t="s">
+        <v>213</v>
+      </c>
+      <c r="F8" s="55">
+        <v>15.0</v>
+      </c>
+      <c r="G8" s="54" t="s">
+        <v>42</v>
+      </c>
+      <c r="H8" s="55">
         <v>20.0</v>
       </c>
-      <c r="E8" s="54" t="s">
-        <v>62</v>
-      </c>
-      <c r="F8" s="55">
-        <v>10.0</v>
-      </c>
-      <c r="G8" s="56" t="s">
-        <v>63</v>
-      </c>
-      <c r="H8" s="55">
-        <v>15.0</v>
-      </c>
       <c r="I8" s="54" t="s">
-        <v>66</v>
+        <v>100</v>
       </c>
       <c r="J8" s="55">
-        <v>15.0</v>
-      </c>
-      <c r="K8" s="56" t="s">
-        <v>87</v>
-      </c>
-      <c r="L8" s="55">
-        <v>25.0</v>
-      </c>
+        <v>35.0</v>
+      </c>
+      <c r="K8" s="56"/>
+      <c r="L8" s="55"/>
       <c r="M8" s="27" t="s">
         <v>181</v>
       </c>
@@ -38778,11 +38771,11 @@
         <f t="shared" si="1"/>
         <v>85</v>
       </c>
-      <c r="R8" s="62" t="s">
-        <v>212</v>
+      <c r="R8" s="63" t="s">
+        <v>214</v>
       </c>
       <c r="S8" s="57" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
     </row>
     <row r="9">
@@ -38792,32 +38785,36 @@
       <c r="B9" s="44">
         <v>21.0</v>
       </c>
-      <c r="C9" s="49" t="s">
-        <v>214</v>
+      <c r="C9" s="51" t="s">
+        <v>59</v>
       </c>
       <c r="D9" s="50">
+        <v>20.0</v>
+      </c>
+      <c r="E9" s="51" t="s">
+        <v>62</v>
+      </c>
+      <c r="F9" s="50">
+        <v>10.0</v>
+      </c>
+      <c r="G9" s="49" t="s">
+        <v>63</v>
+      </c>
+      <c r="H9" s="50">
         <v>15.0</v>
       </c>
-      <c r="E9" s="63" t="s">
-        <v>215</v>
-      </c>
-      <c r="F9" s="50">
+      <c r="I9" s="51" t="s">
+        <v>66</v>
+      </c>
+      <c r="J9" s="50">
         <v>15.0</v>
       </c>
-      <c r="G9" s="51" t="s">
-        <v>42</v>
-      </c>
-      <c r="H9" s="50">
-        <v>20.0</v>
-      </c>
-      <c r="I9" s="51" t="s">
-        <v>100</v>
-      </c>
-      <c r="J9" s="50">
-        <v>35.0</v>
-      </c>
-      <c r="K9" s="51"/>
-      <c r="L9" s="50"/>
+      <c r="K9" s="49" t="s">
+        <v>87</v>
+      </c>
+      <c r="L9" s="50">
+        <v>25.0</v>
+      </c>
       <c r="M9" s="51"/>
       <c r="N9" s="50"/>
       <c r="O9" s="23"/>
@@ -38925,7 +38922,7 @@
         <f t="shared" si="1"/>
         <v>90</v>
       </c>
-      <c r="R11" s="62" t="s">
+      <c r="R11" s="63" t="s">
         <v>221</v>
       </c>
       <c r="S11" s="57" t="s">
@@ -39318,8 +39315,8 @@
       <c r="H24" s="55">
         <v>20.0</v>
       </c>
-      <c r="I24" s="82" t="s">
-        <v>215</v>
+      <c r="I24" s="62" t="s">
+        <v>213</v>
       </c>
       <c r="J24" s="55">
         <v>15.0</v>
@@ -39349,29 +39346,25 @@
     <row r="26">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
-      <c r="E26" s="32"/>
-      <c r="F26" s="33"/>
-      <c r="I26" s="75"/>
-      <c r="J26" s="76"/>
+      <c r="C26" s="51"/>
+      <c r="D26" s="50"/>
+      <c r="E26" s="51"/>
+      <c r="F26" s="50"/>
+      <c r="G26" s="51"/>
+      <c r="H26" s="50"/>
+      <c r="I26" s="49"/>
+      <c r="J26" s="50"/>
       <c r="R26" s="23"/>
       <c r="S26" s="23"/>
+      <c r="W26" s="23" t="s">
+        <v>193</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
-      <c r="C27" s="51"/>
-      <c r="D27" s="50"/>
-      <c r="E27" s="51"/>
-      <c r="F27" s="50"/>
-      <c r="G27" s="51"/>
-      <c r="H27" s="50"/>
       <c r="I27" s="49"/>
       <c r="J27" s="50"/>
-      <c r="R27" s="23"/>
-      <c r="S27" s="23"/>
-      <c r="W27" s="23" t="s">
-        <v>193</v>
-      </c>
     </row>
     <row r="28">
       <c r="A28" s="3"/>
@@ -39382,8 +39375,6 @@
     <row r="29">
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
-      <c r="I29" s="49"/>
-      <c r="J29" s="50"/>
     </row>
     <row r="30">
       <c r="A30" s="3"/>
@@ -42465,29 +42456,25 @@
       <c r="A799" s="3"/>
       <c r="B799" s="3"/>
     </row>
-    <row r="800">
-      <c r="A800" s="3"/>
-      <c r="B800" s="3"/>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="P3:P14 P17:P19 P21:P27">
+  <conditionalFormatting sqref="P3:P14 P17:P19 P21:P26">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="between">
       <formula>80</formula>
       <formula>95</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P3:P14 P17:P19 P21:P27">
+  <conditionalFormatting sqref="P3:P14 P17:P19 P21:P26">
     <cfRule type="cellIs" dxfId="3" priority="2" operator="greaterThan">
       <formula>105</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P3:P14 P17:P19 P21:P27">
+  <conditionalFormatting sqref="P3:P14 P17:P19 P21:P26">
     <cfRule type="cellIs" dxfId="4" priority="3" operator="between">
       <formula>95</formula>
       <formula>105</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P3:P14 P17:P19 P21:P27">
+  <conditionalFormatting sqref="P3:P14 P17:P19 P21:P26">
     <cfRule type="cellIs" dxfId="5" priority="4" operator="lessThan">
       <formula>80</formula>
     </cfRule>
@@ -42600,34 +42587,34 @@
       <c r="A2" s="4" t="s">
         <v>243</v>
       </c>
-      <c r="B2" s="83" t="s">
+      <c r="B2" s="82" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="84">
+      <c r="C2" s="83">
         <v>45.0</v>
       </c>
-      <c r="D2" s="83" t="s">
+      <c r="D2" s="82" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="84">
+      <c r="E2" s="83">
         <v>20.0</v>
       </c>
-      <c r="F2" s="83" t="s">
+      <c r="F2" s="82" t="s">
         <v>18</v>
       </c>
-      <c r="G2" s="84">
+      <c r="G2" s="83">
         <v>25.0</v>
       </c>
-      <c r="H2" s="85"/>
-      <c r="I2" s="86"/>
-      <c r="J2" s="85"/>
-      <c r="K2" s="86"/>
-      <c r="L2" s="85"/>
-      <c r="M2" s="86"/>
-      <c r="N2" s="85"/>
-      <c r="O2" s="86"/>
+      <c r="H2" s="84"/>
+      <c r="I2" s="85"/>
+      <c r="J2" s="84"/>
+      <c r="K2" s="85"/>
+      <c r="L2" s="84"/>
+      <c r="M2" s="85"/>
+      <c r="N2" s="84"/>
+      <c r="O2" s="85"/>
       <c r="P2" s="79"/>
-      <c r="Q2" s="86"/>
+      <c r="Q2" s="85"/>
       <c r="R2" s="79"/>
       <c r="S2" s="22">
         <f t="shared" ref="S2:S17" si="1">SUM(C2,E2,G2,I2,K2,M2,O2,Q2)</f>
@@ -42648,42 +42635,42 @@
       <c r="A3" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="B3" s="83" t="s">
+      <c r="B3" s="82" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="84">
+      <c r="C3" s="83">
         <v>25.0</v>
       </c>
-      <c r="D3" s="83" t="s">
+      <c r="D3" s="82" t="s">
         <v>21</v>
       </c>
-      <c r="E3" s="84">
+      <c r="E3" s="83">
         <v>15.0</v>
       </c>
-      <c r="F3" s="83" t="s">
+      <c r="F3" s="82" t="s">
         <v>22</v>
       </c>
-      <c r="G3" s="84">
+      <c r="G3" s="83">
         <v>25.0</v>
       </c>
-      <c r="H3" s="83" t="s">
+      <c r="H3" s="82" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="84">
+      <c r="I3" s="83">
         <v>10.0</v>
       </c>
-      <c r="J3" s="83" t="s">
+      <c r="J3" s="82" t="s">
         <v>52</v>
       </c>
-      <c r="K3" s="84">
+      <c r="K3" s="83">
         <v>20.0</v>
       </c>
       <c r="L3" s="79"/>
-      <c r="M3" s="86"/>
+      <c r="M3" s="85"/>
       <c r="N3" s="79"/>
-      <c r="O3" s="86"/>
+      <c r="O3" s="85"/>
       <c r="P3" s="79"/>
-      <c r="Q3" s="86"/>
+      <c r="Q3" s="85"/>
       <c r="R3" s="79"/>
       <c r="S3" s="22">
         <f t="shared" si="1"/>
@@ -42704,13 +42691,13 @@
       <c r="A4" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="B4" s="87" t="s">
+      <c r="B4" s="86" t="s">
         <v>23</v>
       </c>
       <c r="C4" s="72">
         <v>20.0</v>
       </c>
-      <c r="D4" s="87" t="s">
+      <c r="D4" s="86" t="s">
         <v>54</v>
       </c>
       <c r="E4" s="72">
@@ -42757,50 +42744,50 @@
       <c r="A5" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="B5" s="83" t="s">
+      <c r="B5" s="82" t="s">
         <v>59</v>
       </c>
-      <c r="C5" s="84">
+      <c r="C5" s="83">
         <v>20.0</v>
       </c>
-      <c r="D5" s="83" t="s">
+      <c r="D5" s="82" t="s">
         <v>62</v>
       </c>
-      <c r="E5" s="84">
+      <c r="E5" s="83">
         <v>10.0</v>
       </c>
-      <c r="F5" s="83" t="s">
+      <c r="F5" s="82" t="s">
         <v>63</v>
       </c>
-      <c r="G5" s="84">
+      <c r="G5" s="83">
         <v>15.0</v>
       </c>
-      <c r="H5" s="83" t="s">
+      <c r="H5" s="82" t="s">
         <v>66</v>
       </c>
-      <c r="I5" s="84">
+      <c r="I5" s="83">
         <v>15.0</v>
       </c>
-      <c r="J5" s="83" t="s">
+      <c r="J5" s="82" t="s">
         <v>35</v>
       </c>
-      <c r="K5" s="84">
+      <c r="K5" s="83">
         <v>10.0</v>
       </c>
       <c r="L5" s="79" t="s">
         <v>181</v>
       </c>
-      <c r="M5" s="86" t="s">
+      <c r="M5" s="85" t="s">
         <v>181</v>
       </c>
       <c r="N5" s="79" t="s">
         <v>181</v>
       </c>
-      <c r="O5" s="86" t="s">
+      <c r="O5" s="85" t="s">
         <v>181</v>
       </c>
       <c r="P5" s="79"/>
-      <c r="Q5" s="86" t="s">
+      <c r="Q5" s="85" t="s">
         <v>181</v>
       </c>
       <c r="R5" s="79"/>
@@ -42825,7 +42812,7 @@
       <c r="A6" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="B6" s="87" t="s">
+      <c r="B6" s="86" t="s">
         <v>98</v>
       </c>
       <c r="C6" s="72">
@@ -42837,19 +42824,19 @@
       <c r="E6" s="72">
         <v>10.0</v>
       </c>
-      <c r="F6" s="87" t="s">
+      <c r="F6" s="86" t="s">
         <v>204</v>
       </c>
       <c r="G6" s="72">
         <v>25.0</v>
       </c>
-      <c r="H6" s="87" t="s">
+      <c r="H6" s="86" t="s">
         <v>205</v>
       </c>
       <c r="I6" s="72">
         <v>20.0</v>
       </c>
-      <c r="J6" s="87" t="s">
+      <c r="J6" s="86" t="s">
         <v>206</v>
       </c>
       <c r="K6" s="72">
@@ -42887,46 +42874,46 @@
       <c r="A7" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="B7" s="83" t="s">
+      <c r="B7" s="82" t="s">
         <v>209</v>
       </c>
-      <c r="C7" s="84">
+      <c r="C7" s="83">
         <v>30.0</v>
       </c>
-      <c r="D7" s="83" t="s">
+      <c r="D7" s="82" t="s">
         <v>210</v>
       </c>
-      <c r="E7" s="84">
+      <c r="E7" s="83">
         <v>30.0</v>
       </c>
-      <c r="F7" s="83" t="s">
+      <c r="F7" s="82" t="s">
         <v>56</v>
       </c>
-      <c r="G7" s="84">
+      <c r="G7" s="83">
         <v>20.0</v>
       </c>
-      <c r="H7" s="88" t="s">
+      <c r="H7" s="87" t="s">
         <v>207</v>
       </c>
-      <c r="I7" s="84">
+      <c r="I7" s="83">
         <v>20.0</v>
       </c>
-      <c r="J7" s="88"/>
-      <c r="K7" s="84"/>
+      <c r="J7" s="87"/>
+      <c r="K7" s="83"/>
       <c r="L7" s="79" t="s">
         <v>181</v>
       </c>
-      <c r="M7" s="86" t="s">
+      <c r="M7" s="85" t="s">
         <v>181</v>
       </c>
       <c r="N7" s="79" t="s">
         <v>181</v>
       </c>
-      <c r="O7" s="86" t="s">
+      <c r="O7" s="85" t="s">
         <v>181</v>
       </c>
       <c r="P7" s="79"/>
-      <c r="Q7" s="86" t="s">
+      <c r="Q7" s="85" t="s">
         <v>181</v>
       </c>
       <c r="R7" s="79"/>
@@ -42961,13 +42948,13 @@
       <c r="E8" s="72">
         <v>15.0</v>
       </c>
-      <c r="F8" s="87" t="s">
+      <c r="F8" s="86" t="s">
         <v>82</v>
       </c>
       <c r="G8" s="72">
         <v>15.0</v>
       </c>
-      <c r="H8" s="87" t="s">
+      <c r="H8" s="86" t="s">
         <v>220</v>
       </c>
       <c r="I8" s="72">
@@ -42985,7 +42972,7 @@
       <c r="M8" s="72">
         <v>20.0</v>
       </c>
-      <c r="N8" s="87" t="s">
+      <c r="N8" s="86" t="s">
         <v>32</v>
       </c>
       <c r="O8" s="72">
@@ -43013,50 +43000,50 @@
       <c r="A9" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="B9" s="83" t="s">
+      <c r="B9" s="82" t="s">
         <v>84</v>
       </c>
-      <c r="C9" s="84">
+      <c r="C9" s="83">
         <v>20.0</v>
       </c>
-      <c r="D9" s="88" t="s">
+      <c r="D9" s="87" t="s">
         <v>86</v>
       </c>
-      <c r="E9" s="84">
+      <c r="E9" s="83">
         <v>25.0</v>
       </c>
-      <c r="F9" s="83" t="s">
+      <c r="F9" s="82" t="s">
         <v>38</v>
       </c>
-      <c r="G9" s="84">
+      <c r="G9" s="83">
         <v>15.0</v>
       </c>
-      <c r="H9" s="83" t="s">
-        <v>214</v>
-      </c>
-      <c r="I9" s="84">
+      <c r="H9" s="82" t="s">
+        <v>212</v>
+      </c>
+      <c r="I9" s="83">
         <v>15.0</v>
       </c>
       <c r="J9" s="79" t="s">
         <v>181</v>
       </c>
-      <c r="K9" s="86" t="s">
+      <c r="K9" s="85" t="s">
         <v>181</v>
       </c>
       <c r="L9" s="79" t="s">
         <v>181</v>
       </c>
-      <c r="M9" s="86" t="s">
+      <c r="M9" s="85" t="s">
         <v>181</v>
       </c>
       <c r="N9" s="79" t="s">
         <v>181</v>
       </c>
-      <c r="O9" s="86" t="s">
+      <c r="O9" s="85" t="s">
         <v>181</v>
       </c>
       <c r="P9" s="79"/>
-      <c r="Q9" s="86" t="s">
+      <c r="Q9" s="85" t="s">
         <v>181</v>
       </c>
       <c r="R9" s="79"/>
@@ -43079,7 +43066,7 @@
       <c r="A10" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="B10" s="89" t="s">
+      <c r="B10" s="88" t="s">
         <v>110</v>
       </c>
       <c r="C10" s="72">
@@ -43145,42 +43132,42 @@
       <c r="A11" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="B11" s="83" t="s">
+      <c r="B11" s="82" t="s">
         <v>71</v>
       </c>
-      <c r="C11" s="84">
+      <c r="C11" s="83">
         <v>25.0</v>
       </c>
-      <c r="D11" s="83" t="s">
+      <c r="D11" s="82" t="s">
         <v>73</v>
       </c>
-      <c r="E11" s="84">
+      <c r="E11" s="83">
         <v>25.0</v>
       </c>
-      <c r="F11" s="83" t="s">
+      <c r="F11" s="82" t="s">
         <v>68</v>
       </c>
-      <c r="G11" s="84">
+      <c r="G11" s="83">
         <v>15.0</v>
       </c>
-      <c r="H11" s="83" t="s">
+      <c r="H11" s="82" t="s">
         <v>79</v>
       </c>
-      <c r="I11" s="84">
+      <c r="I11" s="83">
         <v>35.0</v>
       </c>
-      <c r="J11" s="90"/>
-      <c r="K11" s="91"/>
-      <c r="L11" s="92"/>
-      <c r="M11" s="93"/>
+      <c r="J11" s="89"/>
+      <c r="K11" s="90"/>
+      <c r="L11" s="91"/>
+      <c r="M11" s="92"/>
       <c r="N11" s="79" t="s">
         <v>181</v>
       </c>
-      <c r="O11" s="86" t="s">
+      <c r="O11" s="85" t="s">
         <v>181</v>
       </c>
       <c r="P11" s="79"/>
-      <c r="Q11" s="86" t="s">
+      <c r="Q11" s="85" t="s">
         <v>181</v>
       </c>
       <c r="R11" s="79"/>
@@ -43267,46 +43254,46 @@
       <c r="A13" s="4" t="s">
         <v>169</v>
       </c>
-      <c r="B13" s="88" t="s">
+      <c r="B13" s="87" t="s">
         <v>102</v>
       </c>
-      <c r="C13" s="84">
+      <c r="C13" s="83">
         <v>20.0</v>
       </c>
-      <c r="D13" s="88" t="s">
+      <c r="D13" s="87" t="s">
         <v>103</v>
       </c>
-      <c r="E13" s="84">
+      <c r="E13" s="83">
         <v>25.0</v>
       </c>
-      <c r="F13" s="88" t="s">
+      <c r="F13" s="87" t="s">
         <v>104</v>
       </c>
-      <c r="G13" s="84">
+      <c r="G13" s="83">
         <v>15.0</v>
       </c>
-      <c r="H13" s="88" t="s">
+      <c r="H13" s="87" t="s">
         <v>89</v>
       </c>
-      <c r="I13" s="84">
+      <c r="I13" s="83">
         <v>35.0</v>
       </c>
-      <c r="J13" s="88" t="s">
+      <c r="J13" s="87" t="s">
         <v>107</v>
       </c>
-      <c r="K13" s="84">
+      <c r="K13" s="83">
         <v>15.0</v>
       </c>
-      <c r="L13" s="90"/>
-      <c r="M13" s="91"/>
+      <c r="L13" s="89"/>
+      <c r="M13" s="90"/>
       <c r="N13" s="79" t="s">
         <v>181</v>
       </c>
-      <c r="O13" s="86" t="s">
+      <c r="O13" s="85" t="s">
         <v>181</v>
       </c>
       <c r="P13" s="79"/>
-      <c r="Q13" s="86" t="s">
+      <c r="Q13" s="85" t="s">
         <v>181</v>
       </c>
       <c r="R13" s="79"/>
@@ -43393,48 +43380,48 @@
       <c r="A15" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="B15" s="88" t="s">
+      <c r="B15" s="87" t="s">
         <v>87</v>
       </c>
-      <c r="C15" s="84">
+      <c r="C15" s="83">
         <v>25.0</v>
       </c>
-      <c r="D15" s="83" t="s">
+      <c r="D15" s="82" t="s">
         <v>13</v>
       </c>
-      <c r="E15" s="84"/>
-      <c r="F15" s="83" t="s">
+      <c r="E15" s="83"/>
+      <c r="F15" s="82" t="s">
         <v>14</v>
       </c>
-      <c r="G15" s="84">
+      <c r="G15" s="83">
         <v>35.0</v>
       </c>
       <c r="H15" s="79" t="s">
         <v>181</v>
       </c>
-      <c r="I15" s="86" t="s">
+      <c r="I15" s="85" t="s">
         <v>181</v>
       </c>
       <c r="J15" s="79" t="s">
         <v>181</v>
       </c>
-      <c r="K15" s="86" t="s">
+      <c r="K15" s="85" t="s">
         <v>181</v>
       </c>
       <c r="L15" s="79" t="s">
         <v>181</v>
       </c>
-      <c r="M15" s="86" t="s">
+      <c r="M15" s="85" t="s">
         <v>181</v>
       </c>
       <c r="N15" s="79" t="s">
         <v>181</v>
       </c>
-      <c r="O15" s="86" t="s">
+      <c r="O15" s="85" t="s">
         <v>181</v>
       </c>
       <c r="P15" s="79"/>
-      <c r="Q15" s="86" t="s">
+      <c r="Q15" s="85" t="s">
         <v>181</v>
       </c>
       <c r="R15" s="79"/>
@@ -43581,10 +43568,10 @@
     </row>
     <row r="20">
       <c r="A20" s="3"/>
-      <c r="D20" s="94" t="s">
+      <c r="D20" s="93" t="s">
         <v>53</v>
       </c>
-      <c r="E20" s="95">
+      <c r="E20" s="94">
         <v>15.0</v>
       </c>
       <c r="U20" s="23"/>
@@ -43599,10 +43586,10 @@
     </row>
     <row r="21">
       <c r="A21" s="3"/>
-      <c r="D21" s="94" t="s">
+      <c r="D21" s="93" t="s">
         <v>106</v>
       </c>
-      <c r="E21" s="95">
+      <c r="E21" s="94">
         <v>20.0</v>
       </c>
       <c r="U21" s="23"/>
@@ -43614,10 +43601,10 @@
     </row>
     <row r="22">
       <c r="A22" s="3"/>
-      <c r="D22" s="94" t="s">
+      <c r="D22" s="93" t="s">
         <v>224</v>
       </c>
-      <c r="E22" s="95">
+      <c r="E22" s="94">
         <v>15.0</v>
       </c>
       <c r="U22" s="23"/>
@@ -46100,32 +46087,32 @@
       <c r="A2" s="4" t="s">
         <v>243</v>
       </c>
-      <c r="B2" s="85" t="s">
+      <c r="B2" s="84" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="86">
+      <c r="C2" s="85">
         <v>40.0</v>
       </c>
-      <c r="D2" s="85" t="s">
+      <c r="D2" s="84" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="86">
+      <c r="E2" s="85">
         <v>20.0</v>
       </c>
-      <c r="F2" s="85" t="s">
+      <c r="F2" s="84" t="s">
         <v>18</v>
       </c>
-      <c r="G2" s="86">
+      <c r="G2" s="85">
         <v>25.0</v>
       </c>
-      <c r="H2" s="85"/>
-      <c r="I2" s="86"/>
-      <c r="J2" s="85"/>
-      <c r="K2" s="86"/>
-      <c r="L2" s="85"/>
-      <c r="M2" s="86"/>
-      <c r="N2" s="85"/>
-      <c r="O2" s="86"/>
+      <c r="H2" s="84"/>
+      <c r="I2" s="85"/>
+      <c r="J2" s="84"/>
+      <c r="K2" s="85"/>
+      <c r="L2" s="84"/>
+      <c r="M2" s="85"/>
+      <c r="N2" s="84"/>
+      <c r="O2" s="85"/>
       <c r="P2" s="79"/>
       <c r="Q2" s="22">
         <f t="shared" ref="Q2:Q17" si="1">SUM(C2,E2,G2,I2,K2,M2,O2)</f>
@@ -46146,36 +46133,36 @@
       <c r="A3" s="4" t="s">
         <v>266</v>
       </c>
-      <c r="B3" s="85" t="s">
+      <c r="B3" s="84" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="86">
+      <c r="C3" s="85">
         <v>25.0</v>
       </c>
-      <c r="D3" s="85" t="s">
+      <c r="D3" s="84" t="s">
         <v>21</v>
       </c>
-      <c r="E3" s="86">
+      <c r="E3" s="85">
         <v>15.0</v>
       </c>
-      <c r="F3" s="85" t="s">
+      <c r="F3" s="84" t="s">
         <v>22</v>
       </c>
-      <c r="G3" s="86">
+      <c r="G3" s="85">
         <v>25.0</v>
       </c>
-      <c r="H3" s="85" t="s">
+      <c r="H3" s="84" t="s">
         <v>23</v>
       </c>
-      <c r="I3" s="86">
+      <c r="I3" s="85">
         <v>20.0</v>
       </c>
-      <c r="J3" s="85"/>
-      <c r="K3" s="86"/>
+      <c r="J3" s="84"/>
+      <c r="K3" s="85"/>
       <c r="L3" s="79"/>
-      <c r="M3" s="86"/>
+      <c r="M3" s="85"/>
       <c r="N3" s="79"/>
-      <c r="O3" s="86"/>
+      <c r="O3" s="85"/>
       <c r="P3" s="79"/>
       <c r="Q3" s="22">
         <f t="shared" si="1"/>
@@ -46237,46 +46224,46 @@
       <c r="A5" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="B5" s="85" t="s">
+      <c r="B5" s="84" t="s">
         <v>59</v>
       </c>
-      <c r="C5" s="86">
+      <c r="C5" s="85">
         <v>20.0</v>
       </c>
-      <c r="D5" s="85" t="s">
+      <c r="D5" s="84" t="s">
         <v>62</v>
       </c>
-      <c r="E5" s="86">
+      <c r="E5" s="85">
         <v>10.0</v>
       </c>
-      <c r="F5" s="85" t="s">
+      <c r="F5" s="84" t="s">
         <v>52</v>
       </c>
-      <c r="G5" s="86">
+      <c r="G5" s="85">
         <v>15.0</v>
       </c>
-      <c r="H5" s="85" t="s">
+      <c r="H5" s="84" t="s">
         <v>26</v>
       </c>
-      <c r="I5" s="86">
+      <c r="I5" s="85">
         <v>10.0</v>
       </c>
-      <c r="J5" s="85" t="s">
+      <c r="J5" s="84" t="s">
         <v>98</v>
       </c>
-      <c r="K5" s="86">
+      <c r="K5" s="85">
         <v>15.0</v>
       </c>
-      <c r="L5" s="92" t="s">
+      <c r="L5" s="91" t="s">
         <v>54</v>
       </c>
-      <c r="M5" s="93">
+      <c r="M5" s="92">
         <v>10.0</v>
       </c>
       <c r="N5" s="79" t="s">
         <v>181</v>
       </c>
-      <c r="O5" s="86" t="s">
+      <c r="O5" s="85" t="s">
         <v>181</v>
       </c>
       <c r="P5" s="79"/>
@@ -46290,7 +46277,7 @@
       <c r="T5" s="23" t="s">
         <v>140</v>
       </c>
-      <c r="U5" s="96" t="s">
+      <c r="U5" s="95" t="s">
         <v>268</v>
       </c>
       <c r="V5" s="23" t="s">
@@ -46363,38 +46350,38 @@
       <c r="A7" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="B7" s="85" t="s">
+      <c r="B7" s="84" t="s">
         <v>55</v>
       </c>
-      <c r="C7" s="86">
+      <c r="C7" s="85">
         <v>35.0</v>
       </c>
-      <c r="D7" s="85" t="s">
+      <c r="D7" s="84" t="s">
         <v>56</v>
       </c>
-      <c r="E7" s="86">
+      <c r="E7" s="85">
         <v>35.0</v>
       </c>
-      <c r="F7" s="97" t="s">
+      <c r="F7" s="96" t="s">
         <v>49</v>
       </c>
-      <c r="G7" s="93">
+      <c r="G7" s="92">
         <v>20.0</v>
       </c>
-      <c r="H7" s="97"/>
-      <c r="I7" s="93"/>
-      <c r="J7" s="97"/>
-      <c r="K7" s="93"/>
+      <c r="H7" s="96"/>
+      <c r="I7" s="92"/>
+      <c r="J7" s="96"/>
+      <c r="K7" s="92"/>
       <c r="L7" s="79" t="s">
         <v>181</v>
       </c>
-      <c r="M7" s="86" t="s">
+      <c r="M7" s="85" t="s">
         <v>181</v>
       </c>
       <c r="N7" s="79" t="s">
         <v>181</v>
       </c>
-      <c r="O7" s="86" t="s">
+      <c r="O7" s="85" t="s">
         <v>181</v>
       </c>
       <c r="P7" s="79"/>
@@ -46479,46 +46466,46 @@
       <c r="A9" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="B9" s="85" t="s">
+      <c r="B9" s="84" t="s">
         <v>84</v>
       </c>
-      <c r="C9" s="86">
+      <c r="C9" s="85">
         <v>30.0</v>
       </c>
       <c r="D9" s="79" t="s">
         <v>86</v>
       </c>
-      <c r="E9" s="86">
+      <c r="E9" s="85">
         <v>30.0</v>
       </c>
-      <c r="F9" s="92" t="s">
+      <c r="F9" s="91" t="s">
         <v>38</v>
       </c>
-      <c r="G9" s="93">
+      <c r="G9" s="92">
         <v>15.0</v>
       </c>
       <c r="H9" s="79" t="s">
         <v>181</v>
       </c>
-      <c r="I9" s="86" t="s">
+      <c r="I9" s="85" t="s">
         <v>181</v>
       </c>
       <c r="J9" s="79" t="s">
         <v>181</v>
       </c>
-      <c r="K9" s="86" t="s">
+      <c r="K9" s="85" t="s">
         <v>181</v>
       </c>
       <c r="L9" s="79" t="s">
         <v>181</v>
       </c>
-      <c r="M9" s="86" t="s">
+      <c r="M9" s="85" t="s">
         <v>181</v>
       </c>
       <c r="N9" s="79" t="s">
         <v>181</v>
       </c>
-      <c r="O9" s="86" t="s">
+      <c r="O9" s="85" t="s">
         <v>181</v>
       </c>
       <c r="P9" s="79"/>
@@ -46541,7 +46528,7 @@
       <c r="A10" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="B10" s="98" t="s">
+      <c r="B10" s="97" t="s">
         <v>110</v>
       </c>
       <c r="C10" s="26">
@@ -46605,38 +46592,38 @@
       <c r="A11" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="B11" s="85" t="s">
+      <c r="B11" s="84" t="s">
         <v>71</v>
       </c>
-      <c r="C11" s="86">
+      <c r="C11" s="85">
         <v>10.0</v>
       </c>
-      <c r="D11" s="85" t="s">
+      <c r="D11" s="84" t="s">
         <v>73</v>
       </c>
-      <c r="E11" s="86">
+      <c r="E11" s="85">
         <v>25.0</v>
       </c>
-      <c r="F11" s="85" t="s">
+      <c r="F11" s="84" t="s">
         <v>68</v>
       </c>
-      <c r="G11" s="86">
+      <c r="G11" s="85">
         <v>20.0</v>
       </c>
-      <c r="H11" s="85" t="s">
+      <c r="H11" s="84" t="s">
         <v>79</v>
       </c>
-      <c r="I11" s="86">
+      <c r="I11" s="85">
         <v>35.0</v>
       </c>
-      <c r="J11" s="97"/>
-      <c r="K11" s="93"/>
-      <c r="L11" s="92"/>
-      <c r="M11" s="93"/>
+      <c r="J11" s="96"/>
+      <c r="K11" s="92"/>
+      <c r="L11" s="91"/>
+      <c r="M11" s="92"/>
       <c r="N11" s="79" t="s">
         <v>181</v>
       </c>
-      <c r="O11" s="86" t="s">
+      <c r="O11" s="85" t="s">
         <v>181</v>
       </c>
       <c r="P11" s="79"/>
@@ -46726,43 +46713,43 @@
       <c r="B13" s="79" t="s">
         <v>102</v>
       </c>
-      <c r="C13" s="86">
+      <c r="C13" s="85">
         <v>10.0</v>
       </c>
       <c r="D13" s="79" t="s">
         <v>103</v>
       </c>
-      <c r="E13" s="86">
+      <c r="E13" s="85">
         <v>25.0</v>
       </c>
       <c r="F13" s="79" t="s">
         <v>104</v>
       </c>
-      <c r="G13" s="86">
+      <c r="G13" s="85">
         <v>25.0</v>
       </c>
-      <c r="H13" s="85" t="s">
+      <c r="H13" s="84" t="s">
         <v>82</v>
       </c>
-      <c r="I13" s="86">
+      <c r="I13" s="85">
         <v>15.0</v>
       </c>
-      <c r="J13" s="97" t="s">
+      <c r="J13" s="96" t="s">
         <v>89</v>
       </c>
-      <c r="K13" s="93">
+      <c r="K13" s="92">
         <v>15.0</v>
       </c>
       <c r="L13" s="79" t="s">
         <v>181</v>
       </c>
-      <c r="M13" s="86" t="s">
+      <c r="M13" s="85" t="s">
         <v>181</v>
       </c>
       <c r="N13" s="79" t="s">
         <v>181</v>
       </c>
-      <c r="O13" s="86" t="s">
+      <c r="O13" s="85" t="s">
         <v>181</v>
       </c>
       <c r="P13" s="79"/>
@@ -46845,46 +46832,46 @@
       <c r="A15" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="B15" s="85" t="s">
+      <c r="B15" s="84" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="86">
+      <c r="C15" s="85">
         <v>20.0</v>
       </c>
-      <c r="D15" s="85" t="s">
+      <c r="D15" s="84" t="s">
         <v>14</v>
       </c>
-      <c r="E15" s="86">
+      <c r="E15" s="85">
         <v>20.0</v>
       </c>
       <c r="F15" s="79" t="s">
         <v>181</v>
       </c>
-      <c r="G15" s="86" t="s">
+      <c r="G15" s="85" t="s">
         <v>181</v>
       </c>
       <c r="H15" s="79" t="s">
         <v>181</v>
       </c>
-      <c r="I15" s="86" t="s">
+      <c r="I15" s="85" t="s">
         <v>181</v>
       </c>
       <c r="J15" s="79" t="s">
         <v>181</v>
       </c>
-      <c r="K15" s="86" t="s">
+      <c r="K15" s="85" t="s">
         <v>181</v>
       </c>
       <c r="L15" s="79" t="s">
         <v>181</v>
       </c>
-      <c r="M15" s="86" t="s">
+      <c r="M15" s="85" t="s">
         <v>181</v>
       </c>
       <c r="N15" s="79" t="s">
         <v>181</v>
       </c>
-      <c r="O15" s="86" t="s">
+      <c r="O15" s="85" t="s">
         <v>181</v>
       </c>
       <c r="P15" s="79"/>
@@ -47026,10 +47013,10 @@
     </row>
     <row r="20">
       <c r="A20" s="3"/>
-      <c r="D20" s="94" t="s">
+      <c r="D20" s="93" t="s">
         <v>53</v>
       </c>
-      <c r="E20" s="95">
+      <c r="E20" s="94">
         <v>15.0</v>
       </c>
       <c r="S20" s="23"/>
@@ -47044,10 +47031,10 @@
     </row>
     <row r="21">
       <c r="A21" s="3"/>
-      <c r="D21" s="94" t="s">
+      <c r="D21" s="93" t="s">
         <v>106</v>
       </c>
-      <c r="E21" s="95">
+      <c r="E21" s="94">
         <v>20.0</v>
       </c>
       <c r="S21" s="23"/>
@@ -47059,16 +47046,16 @@
     </row>
     <row r="22">
       <c r="A22" s="3"/>
-      <c r="D22" s="94" t="s">
+      <c r="D22" s="93" t="s">
         <v>100</v>
       </c>
-      <c r="E22" s="95">
+      <c r="E22" s="94">
         <v>20.0</v>
       </c>
       <c r="H22" s="79"/>
-      <c r="I22" s="86"/>
+      <c r="I22" s="85"/>
       <c r="J22" s="79"/>
-      <c r="K22" s="86"/>
+      <c r="K22" s="85"/>
       <c r="S22" s="23"/>
       <c r="T22" s="23"/>
       <c r="U22" s="23"/>

</xml_diff>

<commit_message>
Planung: tausche Default-Methoden mit Command-Pattern
</commit_message>
<xml_diff>
--- a/markdown/org/planung_pm.xlsx
+++ b/markdown/org/planung_pm.xlsx
@@ -14,7 +14,7 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId10" roundtripDataSignature="AMtx7mj5OVWkoZnkcVI3qairug7y+dFYUg=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId10" roundtripDataSignature="AMtx7mgpprjPrtLG+vVO1MoZrEP6WqD1uQ=="/>
     </ext>
   </extLst>
 </workbook>
@@ -679,6 +679,9 @@
     <t>Record-Klassen</t>
   </si>
   <si>
+    <t>Git Worktree</t>
+  </si>
+  <si>
     <t xml:space="preserve">Himmelfahrt
 </t>
   </si>
@@ -687,9 +690,6 @@
   </si>
   <si>
     <t>Zyklus 3: Code</t>
-  </si>
-  <si>
-    <t>Git Worktree</t>
   </si>
   <si>
     <t>Pfingstmontag</t>
@@ -1413,14 +1413,14 @@
     <xf borderId="0" fillId="4" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
     <xf borderId="0" fillId="4" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="4" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="9" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
@@ -38640,7 +38640,7 @@
         <v>204</v>
       </c>
       <c r="D6" s="59">
-        <v>20.0</v>
+        <v>15.0</v>
       </c>
       <c r="E6" s="54" t="s">
         <v>205</v>
@@ -38675,7 +38675,7 @@
       <c r="O6" s="23"/>
       <c r="P6" s="22">
         <f t="shared" si="1"/>
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="R6" s="23"/>
       <c r="S6" s="57" t="s">
@@ -38747,10 +38747,10 @@
         <v>15.0</v>
       </c>
       <c r="G8" s="54" t="s">
-        <v>42</v>
+        <v>68</v>
       </c>
       <c r="H8" s="55">
-        <v>20.0</v>
+        <v>15.0</v>
       </c>
       <c r="I8" s="54" t="s">
         <v>100</v>
@@ -38758,8 +38758,12 @@
       <c r="J8" s="55">
         <v>35.0</v>
       </c>
-      <c r="K8" s="56"/>
-      <c r="L8" s="55"/>
+      <c r="K8" s="63" t="s">
+        <v>214</v>
+      </c>
+      <c r="L8" s="64">
+        <v>10.0</v>
+      </c>
       <c r="M8" s="27" t="s">
         <v>181</v>
       </c>
@@ -38769,13 +38773,13 @@
       <c r="O8" s="23"/>
       <c r="P8" s="22">
         <f t="shared" si="1"/>
-        <v>85</v>
-      </c>
-      <c r="R8" s="63" t="s">
-        <v>214</v>
+        <v>90</v>
+      </c>
+      <c r="R8" s="65" t="s">
+        <v>215</v>
       </c>
       <c r="S8" s="57" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="9">
@@ -38824,7 +38828,7 @@
       </c>
       <c r="R9" s="23"/>
       <c r="S9" s="57" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="10">
@@ -38835,35 +38839,31 @@
         <v>22.0</v>
       </c>
       <c r="C10" s="54" t="s">
-        <v>68</v>
+        <v>79</v>
       </c>
       <c r="D10" s="55">
+        <v>35.0</v>
+      </c>
+      <c r="E10" s="54" t="s">
+        <v>29</v>
+      </c>
+      <c r="F10" s="55">
+        <v>20.0</v>
+      </c>
+      <c r="G10" s="54" t="s">
+        <v>32</v>
+      </c>
+      <c r="H10" s="55">
         <v>15.0</v>
       </c>
-      <c r="E10" s="54" t="s">
-        <v>79</v>
-      </c>
-      <c r="F10" s="55">
-        <v>35.0</v>
-      </c>
-      <c r="G10" s="54" t="s">
-        <v>29</v>
-      </c>
-      <c r="H10" s="55">
+      <c r="I10" s="54" t="s">
+        <v>42</v>
+      </c>
+      <c r="J10" s="55">
         <v>20.0</v>
       </c>
-      <c r="I10" s="54" t="s">
-        <v>32</v>
-      </c>
-      <c r="J10" s="55">
-        <v>15.0</v>
-      </c>
-      <c r="K10" s="64" t="s">
-        <v>217</v>
-      </c>
-      <c r="L10" s="65">
-        <v>10.0</v>
-      </c>
+      <c r="K10" s="63"/>
+      <c r="L10" s="64"/>
       <c r="M10" s="27" t="s">
         <v>181</v>
       </c>
@@ -38873,7 +38873,7 @@
       <c r="O10" s="23"/>
       <c r="P10" s="22">
         <f t="shared" si="1"/>
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="R10" s="66" t="s">
         <v>218</v>
@@ -38922,7 +38922,7 @@
         <f t="shared" si="1"/>
         <v>90</v>
       </c>
-      <c r="R11" s="63" t="s">
+      <c r="R11" s="65" t="s">
         <v>221</v>
       </c>
       <c r="S11" s="57" t="s">
@@ -38960,7 +38960,7 @@
       <c r="J12" s="68">
         <v>20.0</v>
       </c>
-      <c r="K12" s="64" t="s">
+      <c r="K12" s="63" t="s">
         <v>226</v>
       </c>
       <c r="L12" s="69">
@@ -39369,8 +39369,6 @@
     <row r="28">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
-      <c r="I28" s="49"/>
-      <c r="J28" s="50"/>
     </row>
     <row r="29">
       <c r="A29" s="3"/>
@@ -42451,10 +42449,6 @@
     <row r="798">
       <c r="A798" s="3"/>
       <c r="B798" s="3"/>
-    </row>
-    <row r="799">
-      <c r="A799" s="3"/>
-      <c r="B799" s="3"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="P3:P14 P17:P19 P21:P26">

</xml_diff>

<commit_message>
[Org] Schiebe Optional weiter nach vorn im Semesterplan (#685)
* Planung: Schiebe Optional nach vorn

* Planung: Passe Screenshot an

* Planung: Passe Schedule an

* Planung: vertausche Woche 7 und 8 (Generics und Records)

* Planung: tausche Default-Methoden mit Command-Pattern
</commit_message>
<xml_diff>
--- a/markdown/org/planung_pm.xlsx
+++ b/markdown/org/planung_pm.xlsx
@@ -14,14 +14,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId10" roundtripDataSignature="AMtx7mgbOalCEPwh+hcac8TBvw+RzQJMFQ=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId10" roundtripDataSignature="AMtx7mgpprjPrtLG+vVO1MoZrEP6WqD1uQ=="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1106" uniqueCount="279">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1107" uniqueCount="279">
   <si>
     <t>Thema</t>
   </si>
@@ -636,9 +636,6 @@
     <t>Karfreitag</t>
   </si>
   <si>
-    <t>ECS (Framework)</t>
-  </si>
-  <si>
     <t>Ostermontag</t>
   </si>
   <si>
@@ -646,19 +643,10 @@
 =&gt; Praktikum-Zeit (aber kein Praktikum)</t>
   </si>
   <si>
-    <t>Record-Klassen</t>
-  </si>
-  <si>
     <t>Zyklus 1: Konzept</t>
   </si>
   <si>
     <t>Zyklus 1: Code</t>
-  </si>
-  <si>
-    <t>Type-Object-Pattern</t>
-  </si>
-  <si>
-    <t>Zyklus 2: Konzept</t>
   </si>
   <si>
     <t>JUnit1: Intro</t>
@@ -673,13 +661,25 @@
     <t>JUnit4: Mocking (Mockito)</t>
   </si>
   <si>
-    <t>Zyklus 2: Code</t>
+    <t>Zyklus 2: Konzept</t>
   </si>
   <si>
     <t>Bad Smells</t>
   </si>
   <si>
     <t>Coding Rules und Metriken</t>
+  </si>
+  <si>
+    <t>Zyklus 2: Code</t>
+  </si>
+  <si>
+    <t>Serialisierung (equals, hashCode Wdhlg)</t>
+  </si>
+  <si>
+    <t>Record-Klassen</t>
+  </si>
+  <si>
+    <t>Git Worktree</t>
   </si>
   <si>
     <t xml:space="preserve">Himmelfahrt
@@ -690,9 +690,6 @@
   </si>
   <si>
     <t>Zyklus 3: Code</t>
-  </si>
-  <si>
-    <t>Git Worktree</t>
   </si>
   <si>
     <t>Pfingstmontag</t>
@@ -734,9 +731,6 @@
     <t>Prüfungsphase</t>
   </si>
   <si>
-    <t>Serialisierung (equals, hashCode Wdhlg)</t>
-  </si>
-  <si>
     <t>Swing Basics</t>
   </si>
   <si>
@@ -752,7 +746,13 @@
     <t>Swing Tabellen</t>
   </si>
   <si>
+    <t>ECS (Framework)</t>
+  </si>
+  <si>
     <t>Build1: Ant</t>
+  </si>
+  <si>
+    <t>Type-Object-Pattern</t>
   </si>
   <si>
     <t>Einheit 8</t>
@@ -1380,12 +1380,6 @@
     <xf borderId="0" fillId="0" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
@@ -1401,14 +1395,14 @@
     <xf borderId="0" fillId="4" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
@@ -1416,7 +1410,7 @@
     <xf borderId="0" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="4" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="4" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -1424,6 +1418,9 @@
     </xf>
     <xf borderId="0" fillId="4" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="9" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
@@ -1439,9 +1436,6 @@
     </xf>
     <xf borderId="0" fillId="4" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="4" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
@@ -1469,6 +1463,12 @@
     </xf>
     <xf borderId="0" fillId="9" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="9" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
@@ -38509,11 +38509,11 @@
       <c r="H3" s="50">
         <v>25.0</v>
       </c>
-      <c r="I3" s="52" t="s">
-        <v>200</v>
-      </c>
-      <c r="J3" s="53">
-        <v>20.0</v>
+      <c r="I3" s="51" t="s">
+        <v>71</v>
+      </c>
+      <c r="J3" s="50">
+        <v>25.0</v>
       </c>
       <c r="K3" s="49" t="s">
         <v>54</v>
@@ -38526,13 +38526,13 @@
       <c r="O3" s="23"/>
       <c r="P3" s="22">
         <f t="shared" ref="P3:P14" si="1">SUM(D3,F3,H3,J3,L3,N3)</f>
-        <v>80</v>
-      </c>
-      <c r="R3" s="54" t="s">
+        <v>85</v>
+      </c>
+      <c r="R3" s="52" t="s">
+        <v>200</v>
+      </c>
+      <c r="S3" s="53" t="s">
         <v>201</v>
-      </c>
-      <c r="S3" s="55" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="4">
@@ -38542,34 +38542,34 @@
       <c r="B4" s="44">
         <v>16.0</v>
       </c>
-      <c r="C4" s="56" t="s">
+      <c r="C4" s="54" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="57">
+      <c r="D4" s="55">
         <v>25.0</v>
       </c>
-      <c r="E4" s="56" t="s">
+      <c r="E4" s="54" t="s">
         <v>21</v>
       </c>
-      <c r="F4" s="57">
+      <c r="F4" s="55">
         <v>15.0</v>
       </c>
-      <c r="G4" s="58" t="s">
+      <c r="G4" s="56" t="s">
         <v>98</v>
       </c>
-      <c r="H4" s="57">
+      <c r="H4" s="55">
         <v>20.0</v>
       </c>
-      <c r="I4" s="59" t="s">
-        <v>203</v>
-      </c>
-      <c r="J4" s="57">
-        <v>15.0</v>
-      </c>
-      <c r="K4" s="56" t="s">
+      <c r="I4" s="54" t="s">
+        <v>73</v>
+      </c>
+      <c r="J4" s="55">
+        <v>25.0</v>
+      </c>
+      <c r="K4" s="54" t="s">
         <v>35</v>
       </c>
-      <c r="L4" s="57">
+      <c r="L4" s="55">
         <v>10.0</v>
       </c>
       <c r="M4" s="27"/>
@@ -38577,11 +38577,11 @@
       <c r="O4" s="23"/>
       <c r="P4" s="22">
         <f t="shared" si="1"/>
-        <v>85</v>
+        <v>95</v>
       </c>
       <c r="R4" s="23"/>
-      <c r="S4" s="60" t="s">
-        <v>204</v>
+      <c r="S4" s="57" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="5">
@@ -38604,13 +38604,13 @@
         <v>20.0</v>
       </c>
       <c r="G5" s="51" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="H5" s="50">
-        <v>25.0</v>
+        <v>20.0</v>
       </c>
       <c r="I5" s="51" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="J5" s="50">
         <v>25.0</v>
@@ -38622,11 +38622,11 @@
       <c r="O5" s="23"/>
       <c r="P5" s="22">
         <f t="shared" si="1"/>
-        <v>95</v>
-      </c>
-      <c r="R5" s="61"/>
-      <c r="S5" s="60" t="s">
-        <v>205</v>
+        <v>90</v>
+      </c>
+      <c r="R5" s="58"/>
+      <c r="S5" s="57" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="6">
@@ -38637,31 +38637,35 @@
         <v>18.0</v>
       </c>
       <c r="C6" s="56" t="s">
-        <v>77</v>
-      </c>
-      <c r="D6" s="57">
-        <v>25.0</v>
-      </c>
-      <c r="E6" s="56" t="s">
-        <v>74</v>
-      </c>
-      <c r="F6" s="57">
+        <v>204</v>
+      </c>
+      <c r="D6" s="59">
+        <v>15.0</v>
+      </c>
+      <c r="E6" s="54" t="s">
+        <v>205</v>
+      </c>
+      <c r="F6" s="55">
         <v>20.0</v>
       </c>
-      <c r="G6" s="56" t="s">
+      <c r="G6" s="54" t="s">
+        <v>206</v>
+      </c>
+      <c r="H6" s="55">
+        <v>15.0</v>
+      </c>
+      <c r="I6" s="56" t="s">
+        <v>207</v>
+      </c>
+      <c r="J6" s="55">
+        <v>20.0</v>
+      </c>
+      <c r="K6" s="54" t="s">
         <v>52</v>
       </c>
-      <c r="H6" s="57">
+      <c r="L6" s="55">
         <v>20.0</v>
       </c>
-      <c r="I6" s="56" t="s">
-        <v>206</v>
-      </c>
-      <c r="J6" s="57">
-        <v>20.0</v>
-      </c>
-      <c r="K6" s="56"/>
-      <c r="L6" s="57"/>
       <c r="M6" s="27" t="s">
         <v>181</v>
       </c>
@@ -38671,11 +38675,11 @@
       <c r="O6" s="23"/>
       <c r="P6" s="22">
         <f t="shared" si="1"/>
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="R6" s="23"/>
-      <c r="S6" s="60" t="s">
-        <v>207</v>
+      <c r="S6" s="57" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="7">
@@ -38685,46 +38689,42 @@
       <c r="B7" s="44">
         <v>19.0</v>
       </c>
-      <c r="C7" s="49" t="s">
-        <v>208</v>
-      </c>
-      <c r="D7" s="48">
+      <c r="C7" s="51" t="s">
+        <v>209</v>
+      </c>
+      <c r="D7" s="50">
+        <v>30.0</v>
+      </c>
+      <c r="E7" s="51" t="s">
+        <v>210</v>
+      </c>
+      <c r="F7" s="50">
+        <v>30.0</v>
+      </c>
+      <c r="G7" s="51" t="s">
+        <v>56</v>
+      </c>
+      <c r="H7" s="50">
         <v>20.0</v>
       </c>
-      <c r="E7" s="51" t="s">
-        <v>209</v>
-      </c>
-      <c r="F7" s="50">
-        <v>20.0</v>
-      </c>
-      <c r="G7" s="51" t="s">
-        <v>210</v>
-      </c>
-      <c r="H7" s="50">
-        <v>15.0</v>
-      </c>
       <c r="I7" s="49" t="s">
-        <v>211</v>
+        <v>99</v>
       </c>
       <c r="J7" s="50">
-        <v>20.0</v>
-      </c>
-      <c r="K7" s="51" t="s">
-        <v>42</v>
-      </c>
-      <c r="L7" s="50">
-        <v>20.0</v>
-      </c>
-      <c r="M7" s="62"/>
-      <c r="N7" s="63"/>
+        <v>10.0</v>
+      </c>
+      <c r="K7" s="51"/>
+      <c r="L7" s="50"/>
+      <c r="M7" s="60"/>
+      <c r="N7" s="61"/>
       <c r="O7" s="23"/>
       <c r="P7" s="22">
         <f t="shared" si="1"/>
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="R7" s="23"/>
-      <c r="S7" s="60" t="s">
-        <v>212</v>
+      <c r="S7" s="57" t="s">
+        <v>211</v>
       </c>
     </row>
     <row r="8">
@@ -38735,31 +38735,35 @@
         <v>20.0</v>
       </c>
       <c r="C8" s="56" t="s">
+        <v>212</v>
+      </c>
+      <c r="D8" s="55">
+        <v>15.0</v>
+      </c>
+      <c r="E8" s="62" t="s">
         <v>213</v>
       </c>
-      <c r="D8" s="57">
-        <v>30.0</v>
-      </c>
-      <c r="E8" s="56" t="s">
+      <c r="F8" s="55">
+        <v>15.0</v>
+      </c>
+      <c r="G8" s="54" t="s">
+        <v>68</v>
+      </c>
+      <c r="H8" s="55">
+        <v>15.0</v>
+      </c>
+      <c r="I8" s="54" t="s">
+        <v>100</v>
+      </c>
+      <c r="J8" s="55">
+        <v>35.0</v>
+      </c>
+      <c r="K8" s="63" t="s">
         <v>214</v>
       </c>
-      <c r="F8" s="57">
-        <v>30.0</v>
-      </c>
-      <c r="G8" s="56" t="s">
-        <v>56</v>
-      </c>
-      <c r="H8" s="57">
-        <v>20.0</v>
-      </c>
-      <c r="I8" s="58" t="s">
-        <v>99</v>
-      </c>
-      <c r="J8" s="57">
+      <c r="L8" s="64">
         <v>10.0</v>
       </c>
-      <c r="K8" s="56"/>
-      <c r="L8" s="57"/>
       <c r="M8" s="27" t="s">
         <v>181</v>
       </c>
@@ -38771,10 +38775,10 @@
         <f t="shared" si="1"/>
         <v>90</v>
       </c>
-      <c r="R8" s="64" t="s">
+      <c r="R8" s="65" t="s">
         <v>215</v>
       </c>
-      <c r="S8" s="60" t="s">
+      <c r="S8" s="57" t="s">
         <v>216</v>
       </c>
     </row>
@@ -38809,21 +38813,21 @@
       <c r="J9" s="50">
         <v>15.0</v>
       </c>
-      <c r="K9" s="51" t="s">
-        <v>100</v>
+      <c r="K9" s="49" t="s">
+        <v>87</v>
       </c>
       <c r="L9" s="50">
-        <v>35.0</v>
+        <v>25.0</v>
       </c>
       <c r="M9" s="51"/>
       <c r="N9" s="50"/>
       <c r="O9" s="23"/>
       <c r="P9" s="22">
         <f t="shared" si="1"/>
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="R9" s="23"/>
-      <c r="S9" s="60" t="s">
+      <c r="S9" s="57" t="s">
         <v>217</v>
       </c>
     </row>
@@ -38834,36 +38838,32 @@
       <c r="B10" s="44">
         <v>22.0</v>
       </c>
-      <c r="C10" s="56" t="s">
-        <v>68</v>
-      </c>
-      <c r="D10" s="57">
+      <c r="C10" s="54" t="s">
+        <v>79</v>
+      </c>
+      <c r="D10" s="55">
+        <v>35.0</v>
+      </c>
+      <c r="E10" s="54" t="s">
+        <v>29</v>
+      </c>
+      <c r="F10" s="55">
+        <v>20.0</v>
+      </c>
+      <c r="G10" s="54" t="s">
+        <v>32</v>
+      </c>
+      <c r="H10" s="55">
         <v>15.0</v>
       </c>
-      <c r="E10" s="56" t="s">
-        <v>79</v>
-      </c>
-      <c r="F10" s="57">
-        <v>35.0</v>
-      </c>
-      <c r="G10" s="56" t="s">
-        <v>29</v>
-      </c>
-      <c r="H10" s="57">
+      <c r="I10" s="54" t="s">
+        <v>42</v>
+      </c>
+      <c r="J10" s="55">
         <v>20.0</v>
       </c>
-      <c r="I10" s="56" t="s">
-        <v>32</v>
-      </c>
-      <c r="J10" s="57">
-        <v>15.0</v>
-      </c>
-      <c r="K10" s="65" t="s">
-        <v>218</v>
-      </c>
-      <c r="L10" s="66">
-        <v>10.0</v>
-      </c>
+      <c r="K10" s="63"/>
+      <c r="L10" s="64"/>
       <c r="M10" s="27" t="s">
         <v>181</v>
       </c>
@@ -38873,13 +38873,13 @@
       <c r="O10" s="23"/>
       <c r="P10" s="22">
         <f t="shared" si="1"/>
-        <v>95</v>
-      </c>
-      <c r="R10" s="67" t="s">
+        <v>90</v>
+      </c>
+      <c r="R10" s="66" t="s">
+        <v>218</v>
+      </c>
+      <c r="S10" s="57" t="s">
         <v>219</v>
-      </c>
-      <c r="S10" s="60" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="11">
@@ -38908,7 +38908,7 @@
         <v>35.0</v>
       </c>
       <c r="I11" s="49" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="J11" s="50">
         <v>10.0</v>
@@ -38917,16 +38917,16 @@
       <c r="L11" s="50"/>
       <c r="M11" s="51"/>
       <c r="N11" s="50"/>
-      <c r="O11" s="63"/>
+      <c r="O11" s="61"/>
       <c r="P11" s="22">
         <f t="shared" si="1"/>
         <v>90</v>
       </c>
-      <c r="R11" s="64" t="s">
+      <c r="R11" s="65" t="s">
+        <v>221</v>
+      </c>
+      <c r="S11" s="57" t="s">
         <v>222</v>
-      </c>
-      <c r="S11" s="60" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="12">
@@ -38936,46 +38936,46 @@
       <c r="B12" s="44">
         <v>24.0</v>
       </c>
-      <c r="C12" s="58" t="s">
+      <c r="C12" s="56" t="s">
         <v>82</v>
       </c>
-      <c r="D12" s="57">
+      <c r="D12" s="55">
         <v>15.0</v>
       </c>
-      <c r="E12" s="58" t="s">
+      <c r="E12" s="56" t="s">
+        <v>223</v>
+      </c>
+      <c r="F12" s="55">
+        <v>25.0</v>
+      </c>
+      <c r="G12" s="37" t="s">
         <v>224</v>
-      </c>
-      <c r="F12" s="57">
-        <v>25.0</v>
-      </c>
-      <c r="G12" s="37" t="s">
-        <v>225</v>
       </c>
       <c r="H12" s="36">
         <v>15.0</v>
       </c>
-      <c r="I12" s="68" t="s">
+      <c r="I12" s="67" t="s">
+        <v>225</v>
+      </c>
+      <c r="J12" s="68">
+        <v>20.0</v>
+      </c>
+      <c r="K12" s="63" t="s">
         <v>226</v>
       </c>
-      <c r="J12" s="69">
-        <v>20.0</v>
-      </c>
-      <c r="K12" s="65" t="s">
-        <v>227</v>
-      </c>
-      <c r="L12" s="70">
+      <c r="L12" s="69">
         <v>15.0</v>
       </c>
-      <c r="M12" s="56"/>
-      <c r="N12" s="57"/>
+      <c r="M12" s="54"/>
+      <c r="N12" s="55"/>
       <c r="O12" s="23"/>
       <c r="P12" s="22">
         <f t="shared" si="1"/>
         <v>90</v>
       </c>
       <c r="R12" s="23"/>
-      <c r="S12" s="60" t="s">
-        <v>228</v>
+      <c r="S12" s="57" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="13">
@@ -39015,16 +39015,16 @@
       <c r="L13" s="50">
         <v>15.0</v>
       </c>
-      <c r="M13" s="62"/>
-      <c r="N13" s="63"/>
+      <c r="M13" s="60"/>
+      <c r="N13" s="61"/>
       <c r="O13" s="23"/>
       <c r="P13" s="22">
         <f t="shared" si="1"/>
         <v>85</v>
       </c>
       <c r="R13" s="23"/>
-      <c r="S13" s="60" t="s">
-        <v>229</v>
+      <c r="S13" s="57" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="14">
@@ -39034,30 +39034,30 @@
       <c r="B14" s="44">
         <v>26.0</v>
       </c>
-      <c r="C14" s="71" t="s">
+      <c r="C14" s="70" t="s">
         <v>13</v>
       </c>
-      <c r="D14" s="72"/>
-      <c r="E14" s="71" t="s">
+      <c r="D14" s="59"/>
+      <c r="E14" s="70" t="s">
         <v>14</v>
       </c>
-      <c r="F14" s="72"/>
-      <c r="G14" s="56"/>
-      <c r="H14" s="57"/>
-      <c r="I14" s="58"/>
-      <c r="J14" s="57"/>
-      <c r="K14" s="58"/>
-      <c r="L14" s="57"/>
-      <c r="M14" s="73"/>
-      <c r="N14" s="74"/>
+      <c r="F14" s="59"/>
+      <c r="G14" s="54"/>
+      <c r="H14" s="55"/>
+      <c r="I14" s="56"/>
+      <c r="J14" s="55"/>
+      <c r="K14" s="56"/>
+      <c r="L14" s="55"/>
+      <c r="M14" s="71"/>
+      <c r="N14" s="72"/>
       <c r="O14" s="23"/>
       <c r="P14" s="22">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R14" s="23"/>
-      <c r="S14" s="75" t="s">
-        <v>230</v>
+      <c r="S14" s="73" t="s">
+        <v>229</v>
       </c>
     </row>
     <row r="15">
@@ -39065,8 +39065,8 @@
       <c r="B15" s="44">
         <v>27.0</v>
       </c>
-      <c r="C15" s="76" t="s">
-        <v>231</v>
+      <c r="C15" s="74" t="s">
+        <v>230</v>
       </c>
       <c r="D15" s="29" t="s">
         <v>181</v>
@@ -39111,8 +39111,8 @@
       <c r="B16" s="44">
         <v>28.0</v>
       </c>
-      <c r="C16" s="76" t="s">
-        <v>231</v>
+      <c r="C16" s="74" t="s">
+        <v>230</v>
       </c>
       <c r="D16" s="29"/>
       <c r="E16" s="28" t="s">
@@ -39164,30 +39164,26 @@
     <row r="20">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
-      <c r="C20" s="58"/>
-      <c r="D20" s="57"/>
-      <c r="E20" s="58"/>
-      <c r="F20" s="57"/>
-      <c r="G20" s="58"/>
-      <c r="H20" s="57"/>
-      <c r="I20" s="56"/>
-      <c r="J20" s="57"/>
-      <c r="K20" s="58"/>
-      <c r="L20" s="57"/>
-      <c r="M20" s="58"/>
-      <c r="N20" s="57"/>
+      <c r="C20" s="56"/>
+      <c r="D20" s="55"/>
+      <c r="E20" s="56"/>
+      <c r="F20" s="55"/>
+      <c r="G20" s="56"/>
+      <c r="H20" s="55"/>
+      <c r="I20" s="54"/>
+      <c r="J20" s="55"/>
+      <c r="K20" s="56"/>
+      <c r="L20" s="55"/>
+      <c r="M20" s="56"/>
+      <c r="N20" s="55"/>
       <c r="O20" s="27"/>
       <c r="P20" s="27"/>
     </row>
     <row r="21">
       <c r="A21" s="4"/>
       <c r="B21" s="4"/>
-      <c r="C21" s="77" t="s">
-        <v>87</v>
-      </c>
-      <c r="D21" s="78">
-        <v>25.0</v>
-      </c>
+      <c r="C21" s="75"/>
+      <c r="D21" s="76"/>
       <c r="E21" s="49" t="s">
         <v>24</v>
       </c>
@@ -39200,70 +39196,66 @@
       <c r="H21" s="50">
         <v>15.0</v>
       </c>
-      <c r="I21" s="49" t="s">
-        <v>232</v>
-      </c>
-      <c r="J21" s="50">
-        <v>15.0</v>
-      </c>
+      <c r="I21" s="49"/>
+      <c r="J21" s="50"/>
       <c r="K21" s="49" t="s">
         <v>107</v>
       </c>
       <c r="L21" s="50">
         <v>15.0</v>
       </c>
-      <c r="M21" s="79" t="s">
+      <c r="M21" s="77" t="s">
         <v>181</v>
       </c>
-      <c r="N21" s="80" t="s">
+      <c r="N21" s="78" t="s">
         <v>181</v>
       </c>
-      <c r="O21" s="81"/>
+      <c r="O21" s="79"/>
       <c r="P21" s="22">
         <f t="shared" ref="P21:P24" si="2">SUM(D21,F21,H21,J21,L21,N21)</f>
-        <v>75</v>
+        <v>35</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
-      <c r="C22" s="58" t="s">
+      <c r="C22" s="56" t="s">
+        <v>231</v>
+      </c>
+      <c r="D22" s="55">
+        <v>10.0</v>
+      </c>
+      <c r="E22" s="56" t="s">
+        <v>232</v>
+      </c>
+      <c r="F22" s="55">
+        <v>10.0</v>
+      </c>
+      <c r="G22" s="56" t="s">
         <v>233</v>
       </c>
-      <c r="D22" s="57">
-        <v>10.0</v>
-      </c>
-      <c r="E22" s="58" t="s">
+      <c r="H22" s="55">
+        <v>15.0</v>
+      </c>
+      <c r="I22" s="56" t="s">
         <v>234</v>
       </c>
-      <c r="F22" s="57">
-        <v>10.0</v>
-      </c>
-      <c r="G22" s="58" t="s">
+      <c r="J22" s="55">
+        <v>15.0</v>
+      </c>
+      <c r="K22" s="56" t="s">
         <v>235</v>
       </c>
-      <c r="H22" s="57">
+      <c r="L22" s="55">
         <v>15.0</v>
       </c>
-      <c r="I22" s="58" t="s">
-        <v>236</v>
-      </c>
-      <c r="J22" s="57">
-        <v>15.0</v>
-      </c>
-      <c r="K22" s="58" t="s">
-        <v>237</v>
-      </c>
-      <c r="L22" s="57">
-        <v>15.0</v>
-      </c>
-      <c r="M22" s="58" t="s">
+      <c r="M22" s="56" t="s">
         <v>93</v>
       </c>
-      <c r="N22" s="57">
+      <c r="N22" s="55">
         <v>30.0</v>
       </c>
-      <c r="O22" s="74"/>
+      <c r="O22" s="72"/>
       <c r="P22" s="22">
         <f t="shared" si="2"/>
         <v>95</v>
@@ -39280,11 +39272,15 @@
       <c r="D23" s="50">
         <v>20.0</v>
       </c>
-      <c r="E23" s="51"/>
-      <c r="F23" s="50"/>
+      <c r="E23" s="80" t="s">
+        <v>236</v>
+      </c>
+      <c r="F23" s="81">
+        <v>20.0</v>
+      </c>
       <c r="G23" s="49"/>
       <c r="H23" s="50"/>
-      <c r="I23" s="49"/>
+      <c r="I23" s="51"/>
       <c r="J23" s="50"/>
       <c r="K23" s="49"/>
       <c r="L23" s="50"/>
@@ -39293,7 +39289,7 @@
       <c r="O23" s="23"/>
       <c r="P23" s="22">
         <f t="shared" si="2"/>
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="R23" s="23"/>
       <c r="S23" s="23"/>
@@ -39307,28 +39303,36 @@
       <c r="D24" s="36">
         <v>20.0</v>
       </c>
-      <c r="E24" s="58" t="s">
+      <c r="E24" s="56" t="s">
+        <v>237</v>
+      </c>
+      <c r="F24" s="55">
+        <v>25.0</v>
+      </c>
+      <c r="G24" s="56" t="s">
+        <v>97</v>
+      </c>
+      <c r="H24" s="55">
+        <v>20.0</v>
+      </c>
+      <c r="I24" s="62" t="s">
+        <v>213</v>
+      </c>
+      <c r="J24" s="55">
+        <v>15.0</v>
+      </c>
+      <c r="K24" s="54" t="s">
         <v>238</v>
       </c>
-      <c r="F24" s="57">
-        <v>25.0</v>
-      </c>
-      <c r="G24" s="58" t="s">
-        <v>97</v>
-      </c>
-      <c r="H24" s="57">
+      <c r="L24" s="55">
         <v>20.0</v>
       </c>
-      <c r="I24" s="58"/>
-      <c r="J24" s="57"/>
-      <c r="K24" s="65"/>
-      <c r="L24" s="70"/>
-      <c r="M24" s="58"/>
-      <c r="N24" s="57"/>
-      <c r="O24" s="74"/>
+      <c r="M24" s="56"/>
+      <c r="N24" s="55"/>
+      <c r="O24" s="72"/>
       <c r="P24" s="22">
         <f t="shared" si="2"/>
-        <v>65</v>
+        <v>100</v>
       </c>
       <c r="R24" s="23"/>
       <c r="S24" s="23"/>
@@ -39342,41 +39346,33 @@
     <row r="26">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
-      <c r="E26" s="32"/>
-      <c r="F26" s="33"/>
-      <c r="I26" s="77"/>
-      <c r="J26" s="78"/>
+      <c r="C26" s="51"/>
+      <c r="D26" s="50"/>
+      <c r="E26" s="51"/>
+      <c r="F26" s="50"/>
+      <c r="G26" s="51"/>
+      <c r="H26" s="50"/>
+      <c r="I26" s="49"/>
+      <c r="J26" s="50"/>
       <c r="R26" s="23"/>
       <c r="S26" s="23"/>
+      <c r="W26" s="23" t="s">
+        <v>193</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
-      <c r="C27" s="51"/>
-      <c r="D27" s="50"/>
-      <c r="E27" s="51"/>
-      <c r="F27" s="50"/>
-      <c r="G27" s="51"/>
-      <c r="H27" s="50"/>
       <c r="I27" s="49"/>
       <c r="J27" s="50"/>
-      <c r="R27" s="23"/>
-      <c r="S27" s="23"/>
-      <c r="W27" s="23" t="s">
-        <v>193</v>
-      </c>
     </row>
     <row r="28">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
-      <c r="I28" s="49"/>
-      <c r="J28" s="50"/>
     </row>
     <row r="29">
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
-      <c r="I29" s="49"/>
-      <c r="J29" s="50"/>
     </row>
     <row r="30">
       <c r="A30" s="3"/>
@@ -42454,33 +42450,25 @@
       <c r="A798" s="3"/>
       <c r="B798" s="3"/>
     </row>
-    <row r="799">
-      <c r="A799" s="3"/>
-      <c r="B799" s="3"/>
-    </row>
-    <row r="800">
-      <c r="A800" s="3"/>
-      <c r="B800" s="3"/>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="P3:P14 P17:P19 P21:P27">
+  <conditionalFormatting sqref="P3:P14 P17:P19 P21:P26">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="between">
       <formula>80</formula>
       <formula>95</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P3:P14 P17:P19 P21:P27">
+  <conditionalFormatting sqref="P3:P14 P17:P19 P21:P26">
     <cfRule type="cellIs" dxfId="3" priority="2" operator="greaterThan">
       <formula>105</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P3:P14 P17:P19 P21:P27">
+  <conditionalFormatting sqref="P3:P14 P17:P19 P21:P26">
     <cfRule type="cellIs" dxfId="4" priority="3" operator="between">
       <formula>95</formula>
       <formula>105</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P3:P14 P17:P19 P21:P27">
+  <conditionalFormatting sqref="P3:P14 P17:P19 P21:P26">
     <cfRule type="cellIs" dxfId="5" priority="4" operator="lessThan">
       <formula>80</formula>
     </cfRule>
@@ -42619,9 +42607,9 @@
       <c r="M2" s="85"/>
       <c r="N2" s="84"/>
       <c r="O2" s="85"/>
-      <c r="P2" s="81"/>
+      <c r="P2" s="79"/>
       <c r="Q2" s="85"/>
-      <c r="R2" s="81"/>
+      <c r="R2" s="79"/>
       <c r="S2" s="22">
         <f t="shared" ref="S2:S17" si="1">SUM(C2,E2,G2,I2,K2,M2,O2,Q2)</f>
         <v>90</v>
@@ -42671,13 +42659,13 @@
       <c r="K3" s="83">
         <v>20.0</v>
       </c>
-      <c r="L3" s="81"/>
+      <c r="L3" s="79"/>
       <c r="M3" s="85"/>
-      <c r="N3" s="81"/>
+      <c r="N3" s="79"/>
       <c r="O3" s="85"/>
-      <c r="P3" s="81"/>
+      <c r="P3" s="79"/>
       <c r="Q3" s="85"/>
-      <c r="R3" s="81"/>
+      <c r="R3" s="79"/>
       <c r="S3" s="22">
         <f t="shared" si="1"/>
         <v>95</v>
@@ -42700,13 +42688,13 @@
       <c r="B4" s="86" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="74">
+      <c r="C4" s="72">
         <v>20.0</v>
       </c>
       <c r="D4" s="86" t="s">
         <v>54</v>
       </c>
-      <c r="E4" s="74">
+      <c r="E4" s="72">
         <v>15.0</v>
       </c>
       <c r="F4" s="35"/>
@@ -42739,10 +42727,10 @@
       <c r="U4" s="21">
         <v>15.0</v>
       </c>
-      <c r="V4" s="61" t="s">
+      <c r="V4" s="58" t="s">
         <v>136</v>
       </c>
-      <c r="W4" s="62" t="s">
+      <c r="W4" s="60" t="s">
         <v>246</v>
       </c>
     </row>
@@ -42780,23 +42768,23 @@
       <c r="K5" s="83">
         <v>10.0</v>
       </c>
-      <c r="L5" s="81" t="s">
+      <c r="L5" s="79" t="s">
         <v>181</v>
       </c>
       <c r="M5" s="85" t="s">
         <v>181</v>
       </c>
-      <c r="N5" s="81" t="s">
+      <c r="N5" s="79" t="s">
         <v>181</v>
       </c>
       <c r="O5" s="85" t="s">
         <v>181</v>
       </c>
-      <c r="P5" s="81"/>
+      <c r="P5" s="79"/>
       <c r="Q5" s="85" t="s">
         <v>181</v>
       </c>
-      <c r="R5" s="81"/>
+      <c r="R5" s="79"/>
       <c r="S5" s="22">
         <f t="shared" si="1"/>
         <v>70</v>
@@ -42807,10 +42795,10 @@
       <c r="V5" s="23" t="s">
         <v>140</v>
       </c>
-      <c r="W5" s="62" t="s">
+      <c r="W5" s="60" t="s">
         <v>247</v>
       </c>
-      <c r="X5" s="62" t="s">
+      <c r="X5" s="60" t="s">
         <v>248</v>
       </c>
     </row>
@@ -42821,35 +42809,35 @@
       <c r="B6" s="86" t="s">
         <v>98</v>
       </c>
-      <c r="C6" s="74">
+      <c r="C6" s="72">
         <v>20.0</v>
       </c>
-      <c r="D6" s="73" t="s">
+      <c r="D6" s="71" t="s">
         <v>99</v>
       </c>
-      <c r="E6" s="74">
+      <c r="E6" s="72">
         <v>10.0</v>
       </c>
       <c r="F6" s="86" t="s">
-        <v>208</v>
-      </c>
-      <c r="G6" s="74">
+        <v>204</v>
+      </c>
+      <c r="G6" s="72">
         <v>25.0</v>
       </c>
       <c r="H6" s="86" t="s">
-        <v>209</v>
-      </c>
-      <c r="I6" s="74">
+        <v>205</v>
+      </c>
+      <c r="I6" s="72">
         <v>20.0</v>
       </c>
       <c r="J6" s="86" t="s">
-        <v>210</v>
-      </c>
-      <c r="K6" s="74">
+        <v>206</v>
+      </c>
+      <c r="K6" s="72">
         <v>15.0</v>
       </c>
-      <c r="L6" s="73"/>
-      <c r="M6" s="74"/>
+      <c r="L6" s="71"/>
+      <c r="M6" s="72"/>
       <c r="N6" s="27" t="s">
         <v>181</v>
       </c>
@@ -42869,10 +42857,10 @@
         <v>17.0</v>
       </c>
       <c r="V6" s="23"/>
-      <c r="W6" s="62" t="s">
+      <c r="W6" s="60" t="s">
         <v>249</v>
       </c>
-      <c r="X6" s="62" t="s">
+      <c r="X6" s="60" t="s">
         <v>250</v>
       </c>
     </row>
@@ -42881,13 +42869,13 @@
         <v>149</v>
       </c>
       <c r="B7" s="82" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="C7" s="83">
         <v>30.0</v>
       </c>
       <c r="D7" s="82" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="E7" s="83">
         <v>30.0</v>
@@ -42899,30 +42887,30 @@
         <v>20.0</v>
       </c>
       <c r="H7" s="87" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="I7" s="83">
         <v>20.0</v>
       </c>
       <c r="J7" s="87"/>
       <c r="K7" s="83"/>
-      <c r="L7" s="81" t="s">
+      <c r="L7" s="79" t="s">
         <v>181</v>
       </c>
       <c r="M7" s="85" t="s">
         <v>181</v>
       </c>
-      <c r="N7" s="81" t="s">
+      <c r="N7" s="79" t="s">
         <v>181</v>
       </c>
       <c r="O7" s="85" t="s">
         <v>181</v>
       </c>
-      <c r="P7" s="81"/>
+      <c r="P7" s="79"/>
       <c r="Q7" s="85" t="s">
         <v>181</v>
       </c>
-      <c r="R7" s="81"/>
+      <c r="R7" s="79"/>
       <c r="S7" s="22">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -42931,10 +42919,10 @@
         <v>18.0</v>
       </c>
       <c r="V7" s="23"/>
-      <c r="W7" s="62" t="s">
+      <c r="W7" s="60" t="s">
         <v>251</v>
       </c>
-      <c r="X7" s="62" t="s">
+      <c r="X7" s="60" t="s">
         <v>252</v>
       </c>
     </row>
@@ -42942,50 +42930,50 @@
       <c r="A8" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="B8" s="73" t="s">
+      <c r="B8" s="71" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="74">
+      <c r="C8" s="72">
         <v>5.0</v>
       </c>
-      <c r="D8" s="73" t="s">
+      <c r="D8" s="71" t="s">
         <v>57</v>
       </c>
-      <c r="E8" s="74">
+      <c r="E8" s="72">
         <v>15.0</v>
       </c>
       <c r="F8" s="86" t="s">
         <v>82</v>
       </c>
-      <c r="G8" s="74">
+      <c r="G8" s="72">
         <v>15.0</v>
       </c>
       <c r="H8" s="86" t="s">
-        <v>221</v>
-      </c>
-      <c r="I8" s="74">
+        <v>220</v>
+      </c>
+      <c r="I8" s="72">
         <v>10.0</v>
       </c>
-      <c r="J8" s="73" t="s">
+      <c r="J8" s="71" t="s">
         <v>43</v>
       </c>
-      <c r="K8" s="74">
+      <c r="K8" s="72">
         <v>20.0</v>
       </c>
-      <c r="L8" s="73" t="s">
-        <v>206</v>
-      </c>
-      <c r="M8" s="74">
+      <c r="L8" s="71" t="s">
+        <v>238</v>
+      </c>
+      <c r="M8" s="72">
         <v>20.0</v>
       </c>
       <c r="N8" s="86" t="s">
         <v>32</v>
       </c>
-      <c r="O8" s="74">
+      <c r="O8" s="72">
         <v>15.0</v>
       </c>
       <c r="P8" s="27"/>
-      <c r="Q8" s="74"/>
+      <c r="Q8" s="72"/>
       <c r="R8" s="27"/>
       <c r="S8" s="22">
         <f t="shared" si="1"/>
@@ -42995,10 +42983,10 @@
         <v>19.0</v>
       </c>
       <c r="V8" s="23"/>
-      <c r="W8" s="62" t="s">
+      <c r="W8" s="60" t="s">
         <v>187</v>
       </c>
-      <c r="X8" s="62" t="s">
+      <c r="X8" s="60" t="s">
         <v>253</v>
       </c>
     </row>
@@ -43025,34 +43013,34 @@
         <v>15.0</v>
       </c>
       <c r="H9" s="82" t="s">
-        <v>232</v>
+        <v>212</v>
       </c>
       <c r="I9" s="83">
         <v>15.0</v>
       </c>
-      <c r="J9" s="81" t="s">
+      <c r="J9" s="79" t="s">
         <v>181</v>
       </c>
       <c r="K9" s="85" t="s">
         <v>181</v>
       </c>
-      <c r="L9" s="81" t="s">
+      <c r="L9" s="79" t="s">
         <v>181</v>
       </c>
       <c r="M9" s="85" t="s">
         <v>181</v>
       </c>
-      <c r="N9" s="81" t="s">
+      <c r="N9" s="79" t="s">
         <v>181</v>
       </c>
       <c r="O9" s="85" t="s">
         <v>181</v>
       </c>
-      <c r="P9" s="81"/>
+      <c r="P9" s="79"/>
       <c r="Q9" s="85" t="s">
         <v>181</v>
       </c>
-      <c r="R9" s="81"/>
+      <c r="R9" s="79"/>
       <c r="S9" s="22">
         <f t="shared" si="1"/>
         <v>75</v>
@@ -43061,10 +43049,10 @@
         <v>20.0</v>
       </c>
       <c r="V9" s="23"/>
-      <c r="W9" s="62" t="s">
+      <c r="W9" s="60" t="s">
         <v>254</v>
       </c>
-      <c r="X9" s="62" t="s">
+      <c r="X9" s="60" t="s">
         <v>255</v>
       </c>
     </row>
@@ -43075,48 +43063,48 @@
       <c r="B10" s="88" t="s">
         <v>110</v>
       </c>
-      <c r="C10" s="74">
+      <c r="C10" s="72">
         <v>45.0</v>
       </c>
-      <c r="D10" s="73" t="s">
+      <c r="D10" s="71" t="s">
+        <v>231</v>
+      </c>
+      <c r="E10" s="72">
+        <v>10.0</v>
+      </c>
+      <c r="F10" s="71" t="s">
+        <v>232</v>
+      </c>
+      <c r="G10" s="72">
+        <v>10.0</v>
+      </c>
+      <c r="H10" s="71" t="s">
         <v>233</v>
       </c>
-      <c r="E10" s="74">
-        <v>10.0</v>
-      </c>
-      <c r="F10" s="73" t="s">
+      <c r="I10" s="72">
+        <v>15.0</v>
+      </c>
+      <c r="J10" s="71" t="s">
         <v>234</v>
       </c>
-      <c r="G10" s="74">
-        <v>10.0</v>
-      </c>
-      <c r="H10" s="73" t="s">
+      <c r="K10" s="72">
+        <v>15.0</v>
+      </c>
+      <c r="L10" s="71" t="s">
         <v>235</v>
       </c>
-      <c r="I10" s="74">
+      <c r="M10" s="72">
         <v>15.0</v>
       </c>
-      <c r="J10" s="73" t="s">
-        <v>236</v>
-      </c>
-      <c r="K10" s="74">
-        <v>15.0</v>
-      </c>
-      <c r="L10" s="73" t="s">
-        <v>237</v>
-      </c>
-      <c r="M10" s="74">
-        <v>15.0</v>
-      </c>
-      <c r="N10" s="73" t="s">
+      <c r="N10" s="71" t="s">
         <v>93</v>
       </c>
-      <c r="O10" s="74">
+      <c r="O10" s="72">
         <v>30.0</v>
       </c>
-      <c r="P10" s="73"/>
-      <c r="Q10" s="74"/>
-      <c r="R10" s="74"/>
+      <c r="P10" s="71"/>
+      <c r="Q10" s="72"/>
+      <c r="R10" s="72"/>
       <c r="S10" s="22">
         <f t="shared" si="1"/>
         <v>140</v>
@@ -43166,17 +43154,17 @@
       <c r="K11" s="90"/>
       <c r="L11" s="91"/>
       <c r="M11" s="92"/>
-      <c r="N11" s="81" t="s">
+      <c r="N11" s="79" t="s">
         <v>181</v>
       </c>
       <c r="O11" s="85" t="s">
         <v>181</v>
       </c>
-      <c r="P11" s="81"/>
+      <c r="P11" s="79"/>
       <c r="Q11" s="85" t="s">
         <v>181</v>
       </c>
-      <c r="R11" s="81"/>
+      <c r="R11" s="79"/>
       <c r="S11" s="22">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -43185,10 +43173,10 @@
         <v>22.0</v>
       </c>
       <c r="V11" s="23"/>
-      <c r="W11" s="62" t="s">
+      <c r="W11" s="60" t="s">
         <v>256</v>
       </c>
-      <c r="X11" s="62" t="s">
+      <c r="X11" s="60" t="s">
         <v>257</v>
       </c>
     </row>
@@ -43196,38 +43184,38 @@
       <c r="A12" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="B12" s="73" t="s">
+      <c r="B12" s="71" t="s">
         <v>76</v>
       </c>
-      <c r="C12" s="74">
+      <c r="C12" s="72">
         <v>15.0</v>
       </c>
-      <c r="D12" s="73" t="s">
+      <c r="D12" s="71" t="s">
         <v>74</v>
       </c>
-      <c r="E12" s="74">
+      <c r="E12" s="72">
         <v>20.0</v>
       </c>
-      <c r="F12" s="73" t="s">
+      <c r="F12" s="71" t="s">
         <v>77</v>
       </c>
-      <c r="G12" s="74">
+      <c r="G12" s="72">
         <v>25.0</v>
       </c>
-      <c r="H12" s="73" t="s">
+      <c r="H12" s="71" t="s">
         <v>29</v>
       </c>
-      <c r="I12" s="74">
+      <c r="I12" s="72">
         <v>20.0</v>
       </c>
-      <c r="J12" s="73" t="s">
+      <c r="J12" s="71" t="s">
         <v>42</v>
       </c>
-      <c r="K12" s="74">
+      <c r="K12" s="72">
         <v>20.0</v>
       </c>
-      <c r="L12" s="73"/>
-      <c r="M12" s="74"/>
+      <c r="L12" s="71"/>
+      <c r="M12" s="72"/>
       <c r="N12" s="27" t="s">
         <v>181</v>
       </c>
@@ -43249,10 +43237,10 @@
       <c r="V12" s="23" t="s">
         <v>162</v>
       </c>
-      <c r="W12" s="62" t="s">
+      <c r="W12" s="60" t="s">
         <v>190</v>
       </c>
-      <c r="X12" s="62" t="s">
+      <c r="X12" s="60" t="s">
         <v>258</v>
       </c>
     </row>
@@ -43292,17 +43280,17 @@
       </c>
       <c r="L13" s="89"/>
       <c r="M13" s="90"/>
-      <c r="N13" s="81" t="s">
+      <c r="N13" s="79" t="s">
         <v>181</v>
       </c>
       <c r="O13" s="85" t="s">
         <v>181</v>
       </c>
-      <c r="P13" s="81"/>
+      <c r="P13" s="79"/>
       <c r="Q13" s="85" t="s">
         <v>181</v>
       </c>
-      <c r="R13" s="81"/>
+      <c r="R13" s="79"/>
       <c r="S13" s="22">
         <f t="shared" si="1"/>
         <v>110</v>
@@ -43313,10 +43301,10 @@
       <c r="V13" s="23" t="s">
         <v>166</v>
       </c>
-      <c r="W13" s="62" t="s">
+      <c r="W13" s="60" t="s">
         <v>259</v>
       </c>
-      <c r="X13" s="62" t="s">
+      <c r="X13" s="60" t="s">
         <v>260</v>
       </c>
     </row>
@@ -43324,28 +43312,28 @@
       <c r="A14" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="B14" s="73" t="s">
-        <v>224</v>
-      </c>
-      <c r="C14" s="74">
+      <c r="B14" s="71" t="s">
+        <v>223</v>
+      </c>
+      <c r="C14" s="72">
         <v>25.0</v>
       </c>
-      <c r="D14" s="73" t="s">
-        <v>238</v>
-      </c>
-      <c r="E14" s="74">
+      <c r="D14" s="71" t="s">
+        <v>237</v>
+      </c>
+      <c r="E14" s="72">
         <v>25.0</v>
       </c>
-      <c r="F14" s="73" t="s">
+      <c r="F14" s="71" t="s">
         <v>97</v>
       </c>
-      <c r="G14" s="74">
+      <c r="G14" s="72">
         <v>20.0</v>
       </c>
-      <c r="H14" s="73" t="s">
+      <c r="H14" s="71" t="s">
         <v>100</v>
       </c>
-      <c r="I14" s="74">
+      <c r="I14" s="72">
         <v>35.0</v>
       </c>
       <c r="J14" s="37"/>
@@ -43375,10 +43363,10 @@
         <v>25.0</v>
       </c>
       <c r="V14" s="23"/>
-      <c r="W14" s="62" t="s">
+      <c r="W14" s="60" t="s">
         <v>261</v>
       </c>
-      <c r="X14" s="62" t="s">
+      <c r="X14" s="60" t="s">
         <v>262</v>
       </c>
     </row>
@@ -43402,35 +43390,35 @@
       <c r="G15" s="83">
         <v>35.0</v>
       </c>
-      <c r="H15" s="81" t="s">
+      <c r="H15" s="79" t="s">
         <v>181</v>
       </c>
       <c r="I15" s="85" t="s">
         <v>181</v>
       </c>
-      <c r="J15" s="81" t="s">
+      <c r="J15" s="79" t="s">
         <v>181</v>
       </c>
       <c r="K15" s="85" t="s">
         <v>181</v>
       </c>
-      <c r="L15" s="81" t="s">
+      <c r="L15" s="79" t="s">
         <v>181</v>
       </c>
       <c r="M15" s="85" t="s">
         <v>181</v>
       </c>
-      <c r="N15" s="81" t="s">
+      <c r="N15" s="79" t="s">
         <v>181</v>
       </c>
       <c r="O15" s="85" t="s">
         <v>181</v>
       </c>
-      <c r="P15" s="81"/>
+      <c r="P15" s="79"/>
       <c r="Q15" s="85" t="s">
         <v>181</v>
       </c>
-      <c r="R15" s="81"/>
+      <c r="R15" s="79"/>
       <c r="S15" s="22">
         <f t="shared" si="1"/>
         <v>60</v>
@@ -43438,7 +43426,7 @@
       <c r="U15" s="21">
         <v>26.0</v>
       </c>
-      <c r="X15" s="62" t="s">
+      <c r="X15" s="60" t="s">
         <v>263</v>
       </c>
     </row>
@@ -43608,7 +43596,7 @@
     <row r="22">
       <c r="A22" s="3"/>
       <c r="D22" s="93" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E22" s="94">
         <v>15.0</v>
@@ -46119,7 +46107,7 @@
       <c r="M2" s="85"/>
       <c r="N2" s="84"/>
       <c r="O2" s="85"/>
-      <c r="P2" s="81"/>
+      <c r="P2" s="79"/>
       <c r="Q2" s="22">
         <f t="shared" ref="Q2:Q17" si="1">SUM(C2,E2,G2,I2,K2,M2,O2)</f>
         <v>85</v>
@@ -46165,11 +46153,11 @@
       </c>
       <c r="J3" s="84"/>
       <c r="K3" s="85"/>
-      <c r="L3" s="81"/>
+      <c r="L3" s="79"/>
       <c r="M3" s="85"/>
-      <c r="N3" s="81"/>
+      <c r="N3" s="79"/>
       <c r="O3" s="85"/>
-      <c r="P3" s="81"/>
+      <c r="P3" s="79"/>
       <c r="Q3" s="22">
         <f t="shared" si="1"/>
         <v>85</v>
@@ -46219,7 +46207,7 @@
       <c r="S4" s="21">
         <v>15.0</v>
       </c>
-      <c r="T4" s="61" t="s">
+      <c r="T4" s="58" t="s">
         <v>136</v>
       </c>
       <c r="U4" s="23" t="s">
@@ -46266,13 +46254,13 @@
       <c r="M5" s="92">
         <v>10.0</v>
       </c>
-      <c r="N5" s="81" t="s">
+      <c r="N5" s="79" t="s">
         <v>181</v>
       </c>
       <c r="O5" s="85" t="s">
         <v>181</v>
       </c>
-      <c r="P5" s="81"/>
+      <c r="P5" s="79"/>
       <c r="Q5" s="22">
         <f t="shared" si="1"/>
         <v>80</v>
@@ -46378,19 +46366,19 @@
       <c r="I7" s="92"/>
       <c r="J7" s="96"/>
       <c r="K7" s="92"/>
-      <c r="L7" s="81" t="s">
+      <c r="L7" s="79" t="s">
         <v>181</v>
       </c>
       <c r="M7" s="85" t="s">
         <v>181</v>
       </c>
-      <c r="N7" s="81" t="s">
+      <c r="N7" s="79" t="s">
         <v>181</v>
       </c>
       <c r="O7" s="85" t="s">
         <v>181</v>
       </c>
-      <c r="P7" s="81"/>
+      <c r="P7" s="79"/>
       <c r="Q7" s="22">
         <f t="shared" si="1"/>
         <v>90</v>
@@ -46478,7 +46466,7 @@
       <c r="C9" s="85">
         <v>30.0</v>
       </c>
-      <c r="D9" s="81" t="s">
+      <c r="D9" s="79" t="s">
         <v>86</v>
       </c>
       <c r="E9" s="85">
@@ -46490,31 +46478,31 @@
       <c r="G9" s="92">
         <v>15.0</v>
       </c>
-      <c r="H9" s="81" t="s">
+      <c r="H9" s="79" t="s">
         <v>181</v>
       </c>
       <c r="I9" s="85" t="s">
         <v>181</v>
       </c>
-      <c r="J9" s="81" t="s">
+      <c r="J9" s="79" t="s">
         <v>181</v>
       </c>
       <c r="K9" s="85" t="s">
         <v>181</v>
       </c>
-      <c r="L9" s="81" t="s">
+      <c r="L9" s="79" t="s">
         <v>181</v>
       </c>
       <c r="M9" s="85" t="s">
         <v>181</v>
       </c>
-      <c r="N9" s="81" t="s">
+      <c r="N9" s="79" t="s">
         <v>181</v>
       </c>
       <c r="O9" s="85" t="s">
         <v>181</v>
       </c>
-      <c r="P9" s="81"/>
+      <c r="P9" s="79"/>
       <c r="Q9" s="22">
         <f t="shared" si="1"/>
         <v>75</v>
@@ -46626,13 +46614,13 @@
       <c r="K11" s="92"/>
       <c r="L11" s="91"/>
       <c r="M11" s="92"/>
-      <c r="N11" s="81" t="s">
+      <c r="N11" s="79" t="s">
         <v>181</v>
       </c>
       <c r="O11" s="85" t="s">
         <v>181</v>
       </c>
-      <c r="P11" s="81"/>
+      <c r="P11" s="79"/>
       <c r="Q11" s="22">
         <f t="shared" si="1"/>
         <v>90</v>
@@ -46716,19 +46704,19 @@
       <c r="A13" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="B13" s="81" t="s">
+      <c r="B13" s="79" t="s">
         <v>102</v>
       </c>
       <c r="C13" s="85">
         <v>10.0</v>
       </c>
-      <c r="D13" s="81" t="s">
+      <c r="D13" s="79" t="s">
         <v>103</v>
       </c>
       <c r="E13" s="85">
         <v>25.0</v>
       </c>
-      <c r="F13" s="81" t="s">
+      <c r="F13" s="79" t="s">
         <v>104</v>
       </c>
       <c r="G13" s="85">
@@ -46746,19 +46734,19 @@
       <c r="K13" s="92">
         <v>15.0</v>
       </c>
-      <c r="L13" s="81" t="s">
+      <c r="L13" s="79" t="s">
         <v>181</v>
       </c>
       <c r="M13" s="85" t="s">
         <v>181</v>
       </c>
-      <c r="N13" s="81" t="s">
+      <c r="N13" s="79" t="s">
         <v>181</v>
       </c>
       <c r="O13" s="85" t="s">
         <v>181</v>
       </c>
-      <c r="P13" s="81"/>
+      <c r="P13" s="79"/>
       <c r="Q13" s="22">
         <f t="shared" si="1"/>
         <v>90</v>
@@ -46850,37 +46838,37 @@
       <c r="E15" s="85">
         <v>20.0</v>
       </c>
-      <c r="F15" s="81" t="s">
+      <c r="F15" s="79" t="s">
         <v>181</v>
       </c>
       <c r="G15" s="85" t="s">
         <v>181</v>
       </c>
-      <c r="H15" s="81" t="s">
+      <c r="H15" s="79" t="s">
         <v>181</v>
       </c>
       <c r="I15" s="85" t="s">
         <v>181</v>
       </c>
-      <c r="J15" s="81" t="s">
+      <c r="J15" s="79" t="s">
         <v>181</v>
       </c>
       <c r="K15" s="85" t="s">
         <v>181</v>
       </c>
-      <c r="L15" s="81" t="s">
+      <c r="L15" s="79" t="s">
         <v>181</v>
       </c>
       <c r="M15" s="85" t="s">
         <v>181</v>
       </c>
-      <c r="N15" s="81" t="s">
+      <c r="N15" s="79" t="s">
         <v>181</v>
       </c>
       <c r="O15" s="85" t="s">
         <v>181</v>
       </c>
-      <c r="P15" s="81"/>
+      <c r="P15" s="79"/>
       <c r="Q15" s="22">
         <f t="shared" si="1"/>
         <v>40</v>
@@ -47058,9 +47046,9 @@
       <c r="E22" s="94">
         <v>20.0</v>
       </c>
-      <c r="H22" s="81"/>
+      <c r="H22" s="79"/>
       <c r="I22" s="85"/>
-      <c r="J22" s="81"/>
+      <c r="J22" s="79"/>
       <c r="K22" s="85"/>
       <c r="S22" s="23"/>
       <c r="T22" s="23"/>

</xml_diff>

<commit_message>
[ORG] Rescheduling: ziehe Maven+ANT und Factory-Method+Type-Object rein
</commit_message>
<xml_diff>
--- a/markdown/org/planung_pm.xlsx
+++ b/markdown/org/planung_pm.xlsx
@@ -13,15 +13,15 @@
   <definedNames/>
   <calcPr/>
   <extLst>
-    <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId10" roundtripDataSignature="AMtx7mgpprjPrtLG+vVO1MoZrEP6WqD1uQ=="/>
+    <ext uri="GoogleSheetsCustomDataVersion2">
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId10" roundtripDataChecksum="M/7pIkOR/hWOGpn0f3nEby9AnOLGNaXLB245mdCnM4I="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1107" uniqueCount="279">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1106" uniqueCount="279">
   <si>
     <t>Thema</t>
   </si>
@@ -710,16 +710,13 @@
     <t>Configuration</t>
   </si>
   <si>
-    <t>Testcoverage, BDD</t>
-  </si>
-  <si>
-    <t>Sealed Classes und Pattern Matching</t>
-  </si>
-  <si>
-    <t>Dependency Injection</t>
+    <t>Build1: Ant</t>
   </si>
   <si>
     <t>Zyklus 5: Konzept</t>
+  </si>
+  <si>
+    <t>Type-Object-Pattern</t>
   </si>
   <si>
     <t>Zyklus 5: Code</t>
@@ -749,10 +746,13 @@
     <t>ECS (Framework)</t>
   </si>
   <si>
-    <t>Build1: Ant</t>
+    <t>Testcoverage, BDD</t>
   </si>
   <si>
-    <t>Type-Object-Pattern</t>
+    <t>Sealed Classes und Pattern Matching</t>
+  </si>
+  <si>
+    <t>Dependency Injection</t>
   </si>
   <si>
     <t>Einheit 8</t>
@@ -1425,15 +1425,6 @@
     <xf borderId="0" fillId="9" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
     <xf borderId="0" fillId="4" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
@@ -1469,6 +1460,15 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="9" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
@@ -38948,23 +38948,23 @@
       <c r="F12" s="55">
         <v>25.0</v>
       </c>
-      <c r="G12" s="37" t="s">
+      <c r="G12" s="56" t="s">
         <v>224</v>
       </c>
-      <c r="H12" s="36">
+      <c r="H12" s="55">
+        <v>25.0</v>
+      </c>
+      <c r="I12" s="54" t="s">
+        <v>38</v>
+      </c>
+      <c r="J12" s="55">
         <v>15.0</v>
       </c>
-      <c r="I12" s="67" t="s">
-        <v>225</v>
-      </c>
-      <c r="J12" s="68">
-        <v>20.0</v>
-      </c>
-      <c r="K12" s="63" t="s">
-        <v>226</v>
-      </c>
-      <c r="L12" s="69">
-        <v>15.0</v>
+      <c r="K12" s="56" t="s">
+        <v>26</v>
+      </c>
+      <c r="L12" s="55">
+        <v>10.0</v>
       </c>
       <c r="M12" s="54"/>
       <c r="N12" s="55"/>
@@ -38975,7 +38975,7 @@
       </c>
       <c r="R12" s="23"/>
       <c r="S12" s="57" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="13">
@@ -39004,27 +39004,27 @@
         <v>15.0</v>
       </c>
       <c r="I13" s="49" t="s">
-        <v>26</v>
+        <v>97</v>
       </c>
       <c r="J13" s="50">
-        <v>10.0</v>
+        <v>20.0</v>
       </c>
       <c r="K13" s="51" t="s">
-        <v>38</v>
+        <v>226</v>
       </c>
       <c r="L13" s="50">
-        <v>15.0</v>
+        <v>20.0</v>
       </c>
       <c r="M13" s="60"/>
       <c r="N13" s="61"/>
       <c r="O13" s="23"/>
       <c r="P13" s="22">
         <f t="shared" si="1"/>
-        <v>85</v>
+        <v>100</v>
       </c>
       <c r="R13" s="23"/>
       <c r="S13" s="57" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="14">
@@ -39034,11 +39034,11 @@
       <c r="B14" s="44">
         <v>26.0</v>
       </c>
-      <c r="C14" s="70" t="s">
+      <c r="C14" s="67" t="s">
         <v>13</v>
       </c>
       <c r="D14" s="59"/>
-      <c r="E14" s="70" t="s">
+      <c r="E14" s="67" t="s">
         <v>14</v>
       </c>
       <c r="F14" s="59"/>
@@ -39048,16 +39048,16 @@
       <c r="J14" s="55"/>
       <c r="K14" s="56"/>
       <c r="L14" s="55"/>
-      <c r="M14" s="71"/>
-      <c r="N14" s="72"/>
+      <c r="M14" s="68"/>
+      <c r="N14" s="69"/>
       <c r="O14" s="23"/>
       <c r="P14" s="22">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R14" s="23"/>
-      <c r="S14" s="73" t="s">
-        <v>229</v>
+      <c r="S14" s="70" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="15">
@@ -39065,8 +39065,8 @@
       <c r="B15" s="44">
         <v>27.0</v>
       </c>
-      <c r="C15" s="74" t="s">
-        <v>230</v>
+      <c r="C15" s="71" t="s">
+        <v>229</v>
       </c>
       <c r="D15" s="29" t="s">
         <v>181</v>
@@ -39111,8 +39111,8 @@
       <c r="B16" s="44">
         <v>28.0</v>
       </c>
-      <c r="C16" s="74" t="s">
-        <v>230</v>
+      <c r="C16" s="71" t="s">
+        <v>229</v>
       </c>
       <c r="D16" s="29"/>
       <c r="E16" s="28" t="s">
@@ -39182,8 +39182,8 @@
     <row r="21">
       <c r="A21" s="4"/>
       <c r="B21" s="4"/>
-      <c r="C21" s="75"/>
-      <c r="D21" s="76"/>
+      <c r="C21" s="72"/>
+      <c r="D21" s="73"/>
       <c r="E21" s="49" t="s">
         <v>24</v>
       </c>
@@ -39204,13 +39204,13 @@
       <c r="L21" s="50">
         <v>15.0</v>
       </c>
-      <c r="M21" s="77" t="s">
+      <c r="M21" s="74" t="s">
         <v>181</v>
       </c>
-      <c r="N21" s="78" t="s">
+      <c r="N21" s="75" t="s">
         <v>181</v>
       </c>
-      <c r="O21" s="79"/>
+      <c r="O21" s="76"/>
       <c r="P21" s="22">
         <f t="shared" ref="P21:P24" si="2">SUM(D21,F21,H21,J21,L21,N21)</f>
         <v>35</v>
@@ -39220,31 +39220,31 @@
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
       <c r="C22" s="56" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D22" s="55">
         <v>10.0</v>
       </c>
       <c r="E22" s="56" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F22" s="55">
         <v>10.0</v>
       </c>
       <c r="G22" s="56" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="H22" s="55">
         <v>15.0</v>
       </c>
       <c r="I22" s="56" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="J22" s="55">
         <v>15.0</v>
       </c>
       <c r="K22" s="56" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="L22" s="55">
         <v>15.0</v>
@@ -39255,7 +39255,7 @@
       <c r="N22" s="55">
         <v>30.0</v>
       </c>
-      <c r="O22" s="72"/>
+      <c r="O22" s="69"/>
       <c r="P22" s="22">
         <f t="shared" si="2"/>
         <v>95</v>
@@ -39272,10 +39272,10 @@
       <c r="D23" s="50">
         <v>20.0</v>
       </c>
-      <c r="E23" s="80" t="s">
-        <v>236</v>
-      </c>
-      <c r="F23" s="81">
+      <c r="E23" s="77" t="s">
+        <v>235</v>
+      </c>
+      <c r="F23" s="78">
         <v>20.0</v>
       </c>
       <c r="G23" s="49"/>
@@ -39303,36 +39303,32 @@
       <c r="D24" s="36">
         <v>20.0</v>
       </c>
-      <c r="E24" s="56" t="s">
+      <c r="E24" s="37" t="s">
+        <v>236</v>
+      </c>
+      <c r="F24" s="36">
+        <v>15.0</v>
+      </c>
+      <c r="G24" s="79" t="s">
         <v>237</v>
       </c>
-      <c r="F24" s="55">
-        <v>25.0</v>
-      </c>
-      <c r="G24" s="56" t="s">
-        <v>97</v>
-      </c>
-      <c r="H24" s="55">
+      <c r="H24" s="80">
         <v>20.0</v>
       </c>
-      <c r="I24" s="62" t="s">
-        <v>213</v>
-      </c>
-      <c r="J24" s="55">
+      <c r="I24" s="63" t="s">
+        <v>238</v>
+      </c>
+      <c r="J24" s="81">
         <v>15.0</v>
       </c>
-      <c r="K24" s="54" t="s">
-        <v>238</v>
-      </c>
-      <c r="L24" s="55">
-        <v>20.0</v>
-      </c>
+      <c r="K24" s="54"/>
+      <c r="L24" s="55"/>
       <c r="M24" s="56"/>
       <c r="N24" s="55"/>
-      <c r="O24" s="72"/>
+      <c r="O24" s="69"/>
       <c r="P24" s="22">
         <f t="shared" si="2"/>
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="R24" s="23"/>
       <c r="S24" s="23"/>
@@ -39363,8 +39359,6 @@
     <row r="27">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
-      <c r="I27" s="49"/>
-      <c r="J27" s="50"/>
     </row>
     <row r="28">
       <c r="A28" s="3"/>
@@ -42441,14 +42435,6 @@
     <row r="796">
       <c r="A796" s="3"/>
       <c r="B796" s="3"/>
-    </row>
-    <row r="797">
-      <c r="A797" s="3"/>
-      <c r="B797" s="3"/>
-    </row>
-    <row r="798">
-      <c r="A798" s="3"/>
-      <c r="B798" s="3"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="P3:P14 P17:P19 P21:P26">
@@ -42607,9 +42593,9 @@
       <c r="M2" s="85"/>
       <c r="N2" s="84"/>
       <c r="O2" s="85"/>
-      <c r="P2" s="79"/>
+      <c r="P2" s="76"/>
       <c r="Q2" s="85"/>
-      <c r="R2" s="79"/>
+      <c r="R2" s="76"/>
       <c r="S2" s="22">
         <f t="shared" ref="S2:S17" si="1">SUM(C2,E2,G2,I2,K2,M2,O2,Q2)</f>
         <v>90</v>
@@ -42659,13 +42645,13 @@
       <c r="K3" s="83">
         <v>20.0</v>
       </c>
-      <c r="L3" s="79"/>
+      <c r="L3" s="76"/>
       <c r="M3" s="85"/>
-      <c r="N3" s="79"/>
+      <c r="N3" s="76"/>
       <c r="O3" s="85"/>
-      <c r="P3" s="79"/>
+      <c r="P3" s="76"/>
       <c r="Q3" s="85"/>
-      <c r="R3" s="79"/>
+      <c r="R3" s="76"/>
       <c r="S3" s="22">
         <f t="shared" si="1"/>
         <v>95</v>
@@ -42688,13 +42674,13 @@
       <c r="B4" s="86" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="72">
+      <c r="C4" s="69">
         <v>20.0</v>
       </c>
       <c r="D4" s="86" t="s">
         <v>54</v>
       </c>
-      <c r="E4" s="72">
+      <c r="E4" s="69">
         <v>15.0</v>
       </c>
       <c r="F4" s="35"/>
@@ -42768,23 +42754,23 @@
       <c r="K5" s="83">
         <v>10.0</v>
       </c>
-      <c r="L5" s="79" t="s">
+      <c r="L5" s="76" t="s">
         <v>181</v>
       </c>
       <c r="M5" s="85" t="s">
         <v>181</v>
       </c>
-      <c r="N5" s="79" t="s">
+      <c r="N5" s="76" t="s">
         <v>181</v>
       </c>
       <c r="O5" s="85" t="s">
         <v>181</v>
       </c>
-      <c r="P5" s="79"/>
+      <c r="P5" s="76"/>
       <c r="Q5" s="85" t="s">
         <v>181</v>
       </c>
-      <c r="R5" s="79"/>
+      <c r="R5" s="76"/>
       <c r="S5" s="22">
         <f t="shared" si="1"/>
         <v>70</v>
@@ -42809,35 +42795,35 @@
       <c r="B6" s="86" t="s">
         <v>98</v>
       </c>
-      <c r="C6" s="72">
+      <c r="C6" s="69">
         <v>20.0</v>
       </c>
-      <c r="D6" s="71" t="s">
+      <c r="D6" s="68" t="s">
         <v>99</v>
       </c>
-      <c r="E6" s="72">
+      <c r="E6" s="69">
         <v>10.0</v>
       </c>
       <c r="F6" s="86" t="s">
         <v>204</v>
       </c>
-      <c r="G6" s="72">
+      <c r="G6" s="69">
         <v>25.0</v>
       </c>
       <c r="H6" s="86" t="s">
         <v>205</v>
       </c>
-      <c r="I6" s="72">
+      <c r="I6" s="69">
         <v>20.0</v>
       </c>
       <c r="J6" s="86" t="s">
         <v>206</v>
       </c>
-      <c r="K6" s="72">
+      <c r="K6" s="69">
         <v>15.0</v>
       </c>
-      <c r="L6" s="71"/>
-      <c r="M6" s="72"/>
+      <c r="L6" s="68"/>
+      <c r="M6" s="69"/>
       <c r="N6" s="27" t="s">
         <v>181</v>
       </c>
@@ -42894,23 +42880,23 @@
       </c>
       <c r="J7" s="87"/>
       <c r="K7" s="83"/>
-      <c r="L7" s="79" t="s">
+      <c r="L7" s="76" t="s">
         <v>181</v>
       </c>
       <c r="M7" s="85" t="s">
         <v>181</v>
       </c>
-      <c r="N7" s="79" t="s">
+      <c r="N7" s="76" t="s">
         <v>181</v>
       </c>
       <c r="O7" s="85" t="s">
         <v>181</v>
       </c>
-      <c r="P7" s="79"/>
+      <c r="P7" s="76"/>
       <c r="Q7" s="85" t="s">
         <v>181</v>
       </c>
-      <c r="R7" s="79"/>
+      <c r="R7" s="76"/>
       <c r="S7" s="22">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -42930,50 +42916,50 @@
       <c r="A8" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="B8" s="71" t="s">
+      <c r="B8" s="68" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="72">
+      <c r="C8" s="69">
         <v>5.0</v>
       </c>
-      <c r="D8" s="71" t="s">
+      <c r="D8" s="68" t="s">
         <v>57</v>
       </c>
-      <c r="E8" s="72">
+      <c r="E8" s="69">
         <v>15.0</v>
       </c>
       <c r="F8" s="86" t="s">
         <v>82</v>
       </c>
-      <c r="G8" s="72">
+      <c r="G8" s="69">
         <v>15.0</v>
       </c>
       <c r="H8" s="86" t="s">
         <v>220</v>
       </c>
-      <c r="I8" s="72">
+      <c r="I8" s="69">
         <v>10.0</v>
       </c>
-      <c r="J8" s="71" t="s">
+      <c r="J8" s="68" t="s">
         <v>43</v>
       </c>
-      <c r="K8" s="72">
+      <c r="K8" s="69">
         <v>20.0</v>
       </c>
-      <c r="L8" s="71" t="s">
-        <v>238</v>
-      </c>
-      <c r="M8" s="72">
+      <c r="L8" s="68" t="s">
+        <v>226</v>
+      </c>
+      <c r="M8" s="69">
         <v>20.0</v>
       </c>
       <c r="N8" s="86" t="s">
         <v>32</v>
       </c>
-      <c r="O8" s="72">
+      <c r="O8" s="69">
         <v>15.0</v>
       </c>
       <c r="P8" s="27"/>
-      <c r="Q8" s="72"/>
+      <c r="Q8" s="69"/>
       <c r="R8" s="27"/>
       <c r="S8" s="22">
         <f t="shared" si="1"/>
@@ -43018,29 +43004,29 @@
       <c r="I9" s="83">
         <v>15.0</v>
       </c>
-      <c r="J9" s="79" t="s">
+      <c r="J9" s="76" t="s">
         <v>181</v>
       </c>
       <c r="K9" s="85" t="s">
         <v>181</v>
       </c>
-      <c r="L9" s="79" t="s">
+      <c r="L9" s="76" t="s">
         <v>181</v>
       </c>
       <c r="M9" s="85" t="s">
         <v>181</v>
       </c>
-      <c r="N9" s="79" t="s">
+      <c r="N9" s="76" t="s">
         <v>181</v>
       </c>
       <c r="O9" s="85" t="s">
         <v>181</v>
       </c>
-      <c r="P9" s="79"/>
+      <c r="P9" s="76"/>
       <c r="Q9" s="85" t="s">
         <v>181</v>
       </c>
-      <c r="R9" s="79"/>
+      <c r="R9" s="76"/>
       <c r="S9" s="22">
         <f t="shared" si="1"/>
         <v>75</v>
@@ -43063,48 +43049,48 @@
       <c r="B10" s="88" t="s">
         <v>110</v>
       </c>
-      <c r="C10" s="72">
+      <c r="C10" s="69">
         <v>45.0</v>
       </c>
-      <c r="D10" s="71" t="s">
+      <c r="D10" s="68" t="s">
+        <v>230</v>
+      </c>
+      <c r="E10" s="69">
+        <v>10.0</v>
+      </c>
+      <c r="F10" s="68" t="s">
         <v>231</v>
       </c>
-      <c r="E10" s="72">
+      <c r="G10" s="69">
         <v>10.0</v>
       </c>
-      <c r="F10" s="71" t="s">
+      <c r="H10" s="68" t="s">
         <v>232</v>
       </c>
-      <c r="G10" s="72">
-        <v>10.0</v>
-      </c>
-      <c r="H10" s="71" t="s">
+      <c r="I10" s="69">
+        <v>15.0</v>
+      </c>
+      <c r="J10" s="68" t="s">
         <v>233</v>
       </c>
-      <c r="I10" s="72">
+      <c r="K10" s="69">
         <v>15.0</v>
       </c>
-      <c r="J10" s="71" t="s">
+      <c r="L10" s="68" t="s">
         <v>234</v>
       </c>
-      <c r="K10" s="72">
+      <c r="M10" s="69">
         <v>15.0</v>
       </c>
-      <c r="L10" s="71" t="s">
-        <v>235</v>
-      </c>
-      <c r="M10" s="72">
-        <v>15.0</v>
-      </c>
-      <c r="N10" s="71" t="s">
+      <c r="N10" s="68" t="s">
         <v>93</v>
       </c>
-      <c r="O10" s="72">
+      <c r="O10" s="69">
         <v>30.0</v>
       </c>
-      <c r="P10" s="71"/>
-      <c r="Q10" s="72"/>
-      <c r="R10" s="72"/>
+      <c r="P10" s="68"/>
+      <c r="Q10" s="69"/>
+      <c r="R10" s="69"/>
       <c r="S10" s="22">
         <f t="shared" si="1"/>
         <v>140</v>
@@ -43154,17 +43140,17 @@
       <c r="K11" s="90"/>
       <c r="L11" s="91"/>
       <c r="M11" s="92"/>
-      <c r="N11" s="79" t="s">
+      <c r="N11" s="76" t="s">
         <v>181</v>
       </c>
       <c r="O11" s="85" t="s">
         <v>181</v>
       </c>
-      <c r="P11" s="79"/>
+      <c r="P11" s="76"/>
       <c r="Q11" s="85" t="s">
         <v>181</v>
       </c>
-      <c r="R11" s="79"/>
+      <c r="R11" s="76"/>
       <c r="S11" s="22">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -43184,38 +43170,38 @@
       <c r="A12" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="B12" s="71" t="s">
+      <c r="B12" s="68" t="s">
         <v>76</v>
       </c>
-      <c r="C12" s="72">
+      <c r="C12" s="69">
         <v>15.0</v>
       </c>
-      <c r="D12" s="71" t="s">
+      <c r="D12" s="68" t="s">
         <v>74</v>
       </c>
-      <c r="E12" s="72">
+      <c r="E12" s="69">
         <v>20.0</v>
       </c>
-      <c r="F12" s="71" t="s">
+      <c r="F12" s="68" t="s">
         <v>77</v>
       </c>
-      <c r="G12" s="72">
+      <c r="G12" s="69">
         <v>25.0</v>
       </c>
-      <c r="H12" s="71" t="s">
+      <c r="H12" s="68" t="s">
         <v>29</v>
       </c>
-      <c r="I12" s="72">
+      <c r="I12" s="69">
         <v>20.0</v>
       </c>
-      <c r="J12" s="71" t="s">
+      <c r="J12" s="68" t="s">
         <v>42</v>
       </c>
-      <c r="K12" s="72">
+      <c r="K12" s="69">
         <v>20.0</v>
       </c>
-      <c r="L12" s="71"/>
-      <c r="M12" s="72"/>
+      <c r="L12" s="68"/>
+      <c r="M12" s="69"/>
       <c r="N12" s="27" t="s">
         <v>181</v>
       </c>
@@ -43280,17 +43266,17 @@
       </c>
       <c r="L13" s="89"/>
       <c r="M13" s="90"/>
-      <c r="N13" s="79" t="s">
+      <c r="N13" s="76" t="s">
         <v>181</v>
       </c>
       <c r="O13" s="85" t="s">
         <v>181</v>
       </c>
-      <c r="P13" s="79"/>
+      <c r="P13" s="76"/>
       <c r="Q13" s="85" t="s">
         <v>181</v>
       </c>
-      <c r="R13" s="79"/>
+      <c r="R13" s="76"/>
       <c r="S13" s="22">
         <f t="shared" si="1"/>
         <v>110</v>
@@ -43312,28 +43298,28 @@
       <c r="A14" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="B14" s="71" t="s">
+      <c r="B14" s="68" t="s">
         <v>223</v>
       </c>
-      <c r="C14" s="72">
+      <c r="C14" s="69">
         <v>25.0</v>
       </c>
-      <c r="D14" s="71" t="s">
-        <v>237</v>
-      </c>
-      <c r="E14" s="72">
+      <c r="D14" s="68" t="s">
+        <v>224</v>
+      </c>
+      <c r="E14" s="69">
         <v>25.0</v>
       </c>
-      <c r="F14" s="71" t="s">
+      <c r="F14" s="68" t="s">
         <v>97</v>
       </c>
-      <c r="G14" s="72">
+      <c r="G14" s="69">
         <v>20.0</v>
       </c>
-      <c r="H14" s="71" t="s">
+      <c r="H14" s="68" t="s">
         <v>100</v>
       </c>
-      <c r="I14" s="72">
+      <c r="I14" s="69">
         <v>35.0</v>
       </c>
       <c r="J14" s="37"/>
@@ -43390,35 +43376,35 @@
       <c r="G15" s="83">
         <v>35.0</v>
       </c>
-      <c r="H15" s="79" t="s">
+      <c r="H15" s="76" t="s">
         <v>181</v>
       </c>
       <c r="I15" s="85" t="s">
         <v>181</v>
       </c>
-      <c r="J15" s="79" t="s">
+      <c r="J15" s="76" t="s">
         <v>181</v>
       </c>
       <c r="K15" s="85" t="s">
         <v>181</v>
       </c>
-      <c r="L15" s="79" t="s">
+      <c r="L15" s="76" t="s">
         <v>181</v>
       </c>
       <c r="M15" s="85" t="s">
         <v>181</v>
       </c>
-      <c r="N15" s="79" t="s">
+      <c r="N15" s="76" t="s">
         <v>181</v>
       </c>
       <c r="O15" s="85" t="s">
         <v>181</v>
       </c>
-      <c r="P15" s="79"/>
+      <c r="P15" s="76"/>
       <c r="Q15" s="85" t="s">
         <v>181</v>
       </c>
-      <c r="R15" s="79"/>
+      <c r="R15" s="76"/>
       <c r="S15" s="22">
         <f t="shared" si="1"/>
         <v>60</v>
@@ -43596,7 +43582,7 @@
     <row r="22">
       <c r="A22" s="3"/>
       <c r="D22" s="93" t="s">
-        <v>224</v>
+        <v>236</v>
       </c>
       <c r="E22" s="94">
         <v>15.0</v>
@@ -46107,7 +46093,7 @@
       <c r="M2" s="85"/>
       <c r="N2" s="84"/>
       <c r="O2" s="85"/>
-      <c r="P2" s="79"/>
+      <c r="P2" s="76"/>
       <c r="Q2" s="22">
         <f t="shared" ref="Q2:Q17" si="1">SUM(C2,E2,G2,I2,K2,M2,O2)</f>
         <v>85</v>
@@ -46153,11 +46139,11 @@
       </c>
       <c r="J3" s="84"/>
       <c r="K3" s="85"/>
-      <c r="L3" s="79"/>
+      <c r="L3" s="76"/>
       <c r="M3" s="85"/>
-      <c r="N3" s="79"/>
+      <c r="N3" s="76"/>
       <c r="O3" s="85"/>
-      <c r="P3" s="79"/>
+      <c r="P3" s="76"/>
       <c r="Q3" s="22">
         <f t="shared" si="1"/>
         <v>85</v>
@@ -46254,13 +46240,13 @@
       <c r="M5" s="92">
         <v>10.0</v>
       </c>
-      <c r="N5" s="79" t="s">
+      <c r="N5" s="76" t="s">
         <v>181</v>
       </c>
       <c r="O5" s="85" t="s">
         <v>181</v>
       </c>
-      <c r="P5" s="79"/>
+      <c r="P5" s="76"/>
       <c r="Q5" s="22">
         <f t="shared" si="1"/>
         <v>80</v>
@@ -46366,19 +46352,19 @@
       <c r="I7" s="92"/>
       <c r="J7" s="96"/>
       <c r="K7" s="92"/>
-      <c r="L7" s="79" t="s">
+      <c r="L7" s="76" t="s">
         <v>181</v>
       </c>
       <c r="M7" s="85" t="s">
         <v>181</v>
       </c>
-      <c r="N7" s="79" t="s">
+      <c r="N7" s="76" t="s">
         <v>181</v>
       </c>
       <c r="O7" s="85" t="s">
         <v>181</v>
       </c>
-      <c r="P7" s="79"/>
+      <c r="P7" s="76"/>
       <c r="Q7" s="22">
         <f t="shared" si="1"/>
         <v>90</v>
@@ -46466,7 +46452,7 @@
       <c r="C9" s="85">
         <v>30.0</v>
       </c>
-      <c r="D9" s="79" t="s">
+      <c r="D9" s="76" t="s">
         <v>86</v>
       </c>
       <c r="E9" s="85">
@@ -46478,31 +46464,31 @@
       <c r="G9" s="92">
         <v>15.0</v>
       </c>
-      <c r="H9" s="79" t="s">
+      <c r="H9" s="76" t="s">
         <v>181</v>
       </c>
       <c r="I9" s="85" t="s">
         <v>181</v>
       </c>
-      <c r="J9" s="79" t="s">
+      <c r="J9" s="76" t="s">
         <v>181</v>
       </c>
       <c r="K9" s="85" t="s">
         <v>181</v>
       </c>
-      <c r="L9" s="79" t="s">
+      <c r="L9" s="76" t="s">
         <v>181</v>
       </c>
       <c r="M9" s="85" t="s">
         <v>181</v>
       </c>
-      <c r="N9" s="79" t="s">
+      <c r="N9" s="76" t="s">
         <v>181</v>
       </c>
       <c r="O9" s="85" t="s">
         <v>181</v>
       </c>
-      <c r="P9" s="79"/>
+      <c r="P9" s="76"/>
       <c r="Q9" s="22">
         <f t="shared" si="1"/>
         <v>75</v>
@@ -46614,13 +46600,13 @@
       <c r="K11" s="92"/>
       <c r="L11" s="91"/>
       <c r="M11" s="92"/>
-      <c r="N11" s="79" t="s">
+      <c r="N11" s="76" t="s">
         <v>181</v>
       </c>
       <c r="O11" s="85" t="s">
         <v>181</v>
       </c>
-      <c r="P11" s="79"/>
+      <c r="P11" s="76"/>
       <c r="Q11" s="22">
         <f t="shared" si="1"/>
         <v>90</v>
@@ -46704,19 +46690,19 @@
       <c r="A13" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="B13" s="79" t="s">
+      <c r="B13" s="76" t="s">
         <v>102</v>
       </c>
       <c r="C13" s="85">
         <v>10.0</v>
       </c>
-      <c r="D13" s="79" t="s">
+      <c r="D13" s="76" t="s">
         <v>103</v>
       </c>
       <c r="E13" s="85">
         <v>25.0</v>
       </c>
-      <c r="F13" s="79" t="s">
+      <c r="F13" s="76" t="s">
         <v>104</v>
       </c>
       <c r="G13" s="85">
@@ -46734,19 +46720,19 @@
       <c r="K13" s="92">
         <v>15.0</v>
       </c>
-      <c r="L13" s="79" t="s">
+      <c r="L13" s="76" t="s">
         <v>181</v>
       </c>
       <c r="M13" s="85" t="s">
         <v>181</v>
       </c>
-      <c r="N13" s="79" t="s">
+      <c r="N13" s="76" t="s">
         <v>181</v>
       </c>
       <c r="O13" s="85" t="s">
         <v>181</v>
       </c>
-      <c r="P13" s="79"/>
+      <c r="P13" s="76"/>
       <c r="Q13" s="22">
         <f t="shared" si="1"/>
         <v>90</v>
@@ -46838,37 +46824,37 @@
       <c r="E15" s="85">
         <v>20.0</v>
       </c>
-      <c r="F15" s="79" t="s">
+      <c r="F15" s="76" t="s">
         <v>181</v>
       </c>
       <c r="G15" s="85" t="s">
         <v>181</v>
       </c>
-      <c r="H15" s="79" t="s">
+      <c r="H15" s="76" t="s">
         <v>181</v>
       </c>
       <c r="I15" s="85" t="s">
         <v>181</v>
       </c>
-      <c r="J15" s="79" t="s">
+      <c r="J15" s="76" t="s">
         <v>181</v>
       </c>
       <c r="K15" s="85" t="s">
         <v>181</v>
       </c>
-      <c r="L15" s="79" t="s">
+      <c r="L15" s="76" t="s">
         <v>181</v>
       </c>
       <c r="M15" s="85" t="s">
         <v>181</v>
       </c>
-      <c r="N15" s="79" t="s">
+      <c r="N15" s="76" t="s">
         <v>181</v>
       </c>
       <c r="O15" s="85" t="s">
         <v>181</v>
       </c>
-      <c r="P15" s="79"/>
+      <c r="P15" s="76"/>
       <c r="Q15" s="22">
         <f t="shared" si="1"/>
         <v>40</v>
@@ -47046,9 +47032,9 @@
       <c r="E22" s="94">
         <v>20.0</v>
       </c>
-      <c r="H22" s="79"/>
+      <c r="H22" s="76"/>
       <c r="I22" s="85"/>
-      <c r="J22" s="79"/>
+      <c r="J22" s="76"/>
       <c r="K22" s="85"/>
       <c r="S22" s="23"/>
       <c r="T22" s="23"/>

</xml_diff>

<commit_message>
[ORG] Rescheduling: ziehe Maven+ANT und Factory-Method+Type-Object rein (#726)
</commit_message>
<xml_diff>
--- a/markdown/org/planung_pm.xlsx
+++ b/markdown/org/planung_pm.xlsx
@@ -13,15 +13,15 @@
   <definedNames/>
   <calcPr/>
   <extLst>
-    <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId10" roundtripDataSignature="AMtx7mgpprjPrtLG+vVO1MoZrEP6WqD1uQ=="/>
+    <ext uri="GoogleSheetsCustomDataVersion2">
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId10" roundtripDataChecksum="M/7pIkOR/hWOGpn0f3nEby9AnOLGNaXLB245mdCnM4I="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1107" uniqueCount="279">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1106" uniqueCount="279">
   <si>
     <t>Thema</t>
   </si>
@@ -710,16 +710,13 @@
     <t>Configuration</t>
   </si>
   <si>
-    <t>Testcoverage, BDD</t>
-  </si>
-  <si>
-    <t>Sealed Classes und Pattern Matching</t>
-  </si>
-  <si>
-    <t>Dependency Injection</t>
+    <t>Build1: Ant</t>
   </si>
   <si>
     <t>Zyklus 5: Konzept</t>
+  </si>
+  <si>
+    <t>Type-Object-Pattern</t>
   </si>
   <si>
     <t>Zyklus 5: Code</t>
@@ -749,10 +746,13 @@
     <t>ECS (Framework)</t>
   </si>
   <si>
-    <t>Build1: Ant</t>
+    <t>Testcoverage, BDD</t>
   </si>
   <si>
-    <t>Type-Object-Pattern</t>
+    <t>Sealed Classes und Pattern Matching</t>
+  </si>
+  <si>
+    <t>Dependency Injection</t>
   </si>
   <si>
     <t>Einheit 8</t>
@@ -1425,15 +1425,6 @@
     <xf borderId="0" fillId="9" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
     <xf borderId="0" fillId="4" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
@@ -1469,6 +1460,15 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="9" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
@@ -38948,23 +38948,23 @@
       <c r="F12" s="55">
         <v>25.0</v>
       </c>
-      <c r="G12" s="37" t="s">
+      <c r="G12" s="56" t="s">
         <v>224</v>
       </c>
-      <c r="H12" s="36">
+      <c r="H12" s="55">
+        <v>25.0</v>
+      </c>
+      <c r="I12" s="54" t="s">
+        <v>38</v>
+      </c>
+      <c r="J12" s="55">
         <v>15.0</v>
       </c>
-      <c r="I12" s="67" t="s">
-        <v>225</v>
-      </c>
-      <c r="J12" s="68">
-        <v>20.0</v>
-      </c>
-      <c r="K12" s="63" t="s">
-        <v>226</v>
-      </c>
-      <c r="L12" s="69">
-        <v>15.0</v>
+      <c r="K12" s="56" t="s">
+        <v>26</v>
+      </c>
+      <c r="L12" s="55">
+        <v>10.0</v>
       </c>
       <c r="M12" s="54"/>
       <c r="N12" s="55"/>
@@ -38975,7 +38975,7 @@
       </c>
       <c r="R12" s="23"/>
       <c r="S12" s="57" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="13">
@@ -39004,27 +39004,27 @@
         <v>15.0</v>
       </c>
       <c r="I13" s="49" t="s">
-        <v>26</v>
+        <v>97</v>
       </c>
       <c r="J13" s="50">
-        <v>10.0</v>
+        <v>20.0</v>
       </c>
       <c r="K13" s="51" t="s">
-        <v>38</v>
+        <v>226</v>
       </c>
       <c r="L13" s="50">
-        <v>15.0</v>
+        <v>20.0</v>
       </c>
       <c r="M13" s="60"/>
       <c r="N13" s="61"/>
       <c r="O13" s="23"/>
       <c r="P13" s="22">
         <f t="shared" si="1"/>
-        <v>85</v>
+        <v>100</v>
       </c>
       <c r="R13" s="23"/>
       <c r="S13" s="57" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="14">
@@ -39034,11 +39034,11 @@
       <c r="B14" s="44">
         <v>26.0</v>
       </c>
-      <c r="C14" s="70" t="s">
+      <c r="C14" s="67" t="s">
         <v>13</v>
       </c>
       <c r="D14" s="59"/>
-      <c r="E14" s="70" t="s">
+      <c r="E14" s="67" t="s">
         <v>14</v>
       </c>
       <c r="F14" s="59"/>
@@ -39048,16 +39048,16 @@
       <c r="J14" s="55"/>
       <c r="K14" s="56"/>
       <c r="L14" s="55"/>
-      <c r="M14" s="71"/>
-      <c r="N14" s="72"/>
+      <c r="M14" s="68"/>
+      <c r="N14" s="69"/>
       <c r="O14" s="23"/>
       <c r="P14" s="22">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R14" s="23"/>
-      <c r="S14" s="73" t="s">
-        <v>229</v>
+      <c r="S14" s="70" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="15">
@@ -39065,8 +39065,8 @@
       <c r="B15" s="44">
         <v>27.0</v>
       </c>
-      <c r="C15" s="74" t="s">
-        <v>230</v>
+      <c r="C15" s="71" t="s">
+        <v>229</v>
       </c>
       <c r="D15" s="29" t="s">
         <v>181</v>
@@ -39111,8 +39111,8 @@
       <c r="B16" s="44">
         <v>28.0</v>
       </c>
-      <c r="C16" s="74" t="s">
-        <v>230</v>
+      <c r="C16" s="71" t="s">
+        <v>229</v>
       </c>
       <c r="D16" s="29"/>
       <c r="E16" s="28" t="s">
@@ -39182,8 +39182,8 @@
     <row r="21">
       <c r="A21" s="4"/>
       <c r="B21" s="4"/>
-      <c r="C21" s="75"/>
-      <c r="D21" s="76"/>
+      <c r="C21" s="72"/>
+      <c r="D21" s="73"/>
       <c r="E21" s="49" t="s">
         <v>24</v>
       </c>
@@ -39204,13 +39204,13 @@
       <c r="L21" s="50">
         <v>15.0</v>
       </c>
-      <c r="M21" s="77" t="s">
+      <c r="M21" s="74" t="s">
         <v>181</v>
       </c>
-      <c r="N21" s="78" t="s">
+      <c r="N21" s="75" t="s">
         <v>181</v>
       </c>
-      <c r="O21" s="79"/>
+      <c r="O21" s="76"/>
       <c r="P21" s="22">
         <f t="shared" ref="P21:P24" si="2">SUM(D21,F21,H21,J21,L21,N21)</f>
         <v>35</v>
@@ -39220,31 +39220,31 @@
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
       <c r="C22" s="56" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D22" s="55">
         <v>10.0</v>
       </c>
       <c r="E22" s="56" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F22" s="55">
         <v>10.0</v>
       </c>
       <c r="G22" s="56" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="H22" s="55">
         <v>15.0</v>
       </c>
       <c r="I22" s="56" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="J22" s="55">
         <v>15.0</v>
       </c>
       <c r="K22" s="56" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="L22" s="55">
         <v>15.0</v>
@@ -39255,7 +39255,7 @@
       <c r="N22" s="55">
         <v>30.0</v>
       </c>
-      <c r="O22" s="72"/>
+      <c r="O22" s="69"/>
       <c r="P22" s="22">
         <f t="shared" si="2"/>
         <v>95</v>
@@ -39272,10 +39272,10 @@
       <c r="D23" s="50">
         <v>20.0</v>
       </c>
-      <c r="E23" s="80" t="s">
-        <v>236</v>
-      </c>
-      <c r="F23" s="81">
+      <c r="E23" s="77" t="s">
+        <v>235</v>
+      </c>
+      <c r="F23" s="78">
         <v>20.0</v>
       </c>
       <c r="G23" s="49"/>
@@ -39303,36 +39303,32 @@
       <c r="D24" s="36">
         <v>20.0</v>
       </c>
-      <c r="E24" s="56" t="s">
+      <c r="E24" s="37" t="s">
+        <v>236</v>
+      </c>
+      <c r="F24" s="36">
+        <v>15.0</v>
+      </c>
+      <c r="G24" s="79" t="s">
         <v>237</v>
       </c>
-      <c r="F24" s="55">
-        <v>25.0</v>
-      </c>
-      <c r="G24" s="56" t="s">
-        <v>97</v>
-      </c>
-      <c r="H24" s="55">
+      <c r="H24" s="80">
         <v>20.0</v>
       </c>
-      <c r="I24" s="62" t="s">
-        <v>213</v>
-      </c>
-      <c r="J24" s="55">
+      <c r="I24" s="63" t="s">
+        <v>238</v>
+      </c>
+      <c r="J24" s="81">
         <v>15.0</v>
       </c>
-      <c r="K24" s="54" t="s">
-        <v>238</v>
-      </c>
-      <c r="L24" s="55">
-        <v>20.0</v>
-      </c>
+      <c r="K24" s="54"/>
+      <c r="L24" s="55"/>
       <c r="M24" s="56"/>
       <c r="N24" s="55"/>
-      <c r="O24" s="72"/>
+      <c r="O24" s="69"/>
       <c r="P24" s="22">
         <f t="shared" si="2"/>
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="R24" s="23"/>
       <c r="S24" s="23"/>
@@ -39363,8 +39359,6 @@
     <row r="27">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
-      <c r="I27" s="49"/>
-      <c r="J27" s="50"/>
     </row>
     <row r="28">
       <c r="A28" s="3"/>
@@ -42441,14 +42435,6 @@
     <row r="796">
       <c r="A796" s="3"/>
       <c r="B796" s="3"/>
-    </row>
-    <row r="797">
-      <c r="A797" s="3"/>
-      <c r="B797" s="3"/>
-    </row>
-    <row r="798">
-      <c r="A798" s="3"/>
-      <c r="B798" s="3"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="P3:P14 P17:P19 P21:P26">
@@ -42607,9 +42593,9 @@
       <c r="M2" s="85"/>
       <c r="N2" s="84"/>
       <c r="O2" s="85"/>
-      <c r="P2" s="79"/>
+      <c r="P2" s="76"/>
       <c r="Q2" s="85"/>
-      <c r="R2" s="79"/>
+      <c r="R2" s="76"/>
       <c r="S2" s="22">
         <f t="shared" ref="S2:S17" si="1">SUM(C2,E2,G2,I2,K2,M2,O2,Q2)</f>
         <v>90</v>
@@ -42659,13 +42645,13 @@
       <c r="K3" s="83">
         <v>20.0</v>
       </c>
-      <c r="L3" s="79"/>
+      <c r="L3" s="76"/>
       <c r="M3" s="85"/>
-      <c r="N3" s="79"/>
+      <c r="N3" s="76"/>
       <c r="O3" s="85"/>
-      <c r="P3" s="79"/>
+      <c r="P3" s="76"/>
       <c r="Q3" s="85"/>
-      <c r="R3" s="79"/>
+      <c r="R3" s="76"/>
       <c r="S3" s="22">
         <f t="shared" si="1"/>
         <v>95</v>
@@ -42688,13 +42674,13 @@
       <c r="B4" s="86" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="72">
+      <c r="C4" s="69">
         <v>20.0</v>
       </c>
       <c r="D4" s="86" t="s">
         <v>54</v>
       </c>
-      <c r="E4" s="72">
+      <c r="E4" s="69">
         <v>15.0</v>
       </c>
       <c r="F4" s="35"/>
@@ -42768,23 +42754,23 @@
       <c r="K5" s="83">
         <v>10.0</v>
       </c>
-      <c r="L5" s="79" t="s">
+      <c r="L5" s="76" t="s">
         <v>181</v>
       </c>
       <c r="M5" s="85" t="s">
         <v>181</v>
       </c>
-      <c r="N5" s="79" t="s">
+      <c r="N5" s="76" t="s">
         <v>181</v>
       </c>
       <c r="O5" s="85" t="s">
         <v>181</v>
       </c>
-      <c r="P5" s="79"/>
+      <c r="P5" s="76"/>
       <c r="Q5" s="85" t="s">
         <v>181</v>
       </c>
-      <c r="R5" s="79"/>
+      <c r="R5" s="76"/>
       <c r="S5" s="22">
         <f t="shared" si="1"/>
         <v>70</v>
@@ -42809,35 +42795,35 @@
       <c r="B6" s="86" t="s">
         <v>98</v>
       </c>
-      <c r="C6" s="72">
+      <c r="C6" s="69">
         <v>20.0</v>
       </c>
-      <c r="D6" s="71" t="s">
+      <c r="D6" s="68" t="s">
         <v>99</v>
       </c>
-      <c r="E6" s="72">
+      <c r="E6" s="69">
         <v>10.0</v>
       </c>
       <c r="F6" s="86" t="s">
         <v>204</v>
       </c>
-      <c r="G6" s="72">
+      <c r="G6" s="69">
         <v>25.0</v>
       </c>
       <c r="H6" s="86" t="s">
         <v>205</v>
       </c>
-      <c r="I6" s="72">
+      <c r="I6" s="69">
         <v>20.0</v>
       </c>
       <c r="J6" s="86" t="s">
         <v>206</v>
       </c>
-      <c r="K6" s="72">
+      <c r="K6" s="69">
         <v>15.0</v>
       </c>
-      <c r="L6" s="71"/>
-      <c r="M6" s="72"/>
+      <c r="L6" s="68"/>
+      <c r="M6" s="69"/>
       <c r="N6" s="27" t="s">
         <v>181</v>
       </c>
@@ -42894,23 +42880,23 @@
       </c>
       <c r="J7" s="87"/>
       <c r="K7" s="83"/>
-      <c r="L7" s="79" t="s">
+      <c r="L7" s="76" t="s">
         <v>181</v>
       </c>
       <c r="M7" s="85" t="s">
         <v>181</v>
       </c>
-      <c r="N7" s="79" t="s">
+      <c r="N7" s="76" t="s">
         <v>181</v>
       </c>
       <c r="O7" s="85" t="s">
         <v>181</v>
       </c>
-      <c r="P7" s="79"/>
+      <c r="P7" s="76"/>
       <c r="Q7" s="85" t="s">
         <v>181</v>
       </c>
-      <c r="R7" s="79"/>
+      <c r="R7" s="76"/>
       <c r="S7" s="22">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -42930,50 +42916,50 @@
       <c r="A8" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="B8" s="71" t="s">
+      <c r="B8" s="68" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="72">
+      <c r="C8" s="69">
         <v>5.0</v>
       </c>
-      <c r="D8" s="71" t="s">
+      <c r="D8" s="68" t="s">
         <v>57</v>
       </c>
-      <c r="E8" s="72">
+      <c r="E8" s="69">
         <v>15.0</v>
       </c>
       <c r="F8" s="86" t="s">
         <v>82</v>
       </c>
-      <c r="G8" s="72">
+      <c r="G8" s="69">
         <v>15.0</v>
       </c>
       <c r="H8" s="86" t="s">
         <v>220</v>
       </c>
-      <c r="I8" s="72">
+      <c r="I8" s="69">
         <v>10.0</v>
       </c>
-      <c r="J8" s="71" t="s">
+      <c r="J8" s="68" t="s">
         <v>43</v>
       </c>
-      <c r="K8" s="72">
+      <c r="K8" s="69">
         <v>20.0</v>
       </c>
-      <c r="L8" s="71" t="s">
-        <v>238</v>
-      </c>
-      <c r="M8" s="72">
+      <c r="L8" s="68" t="s">
+        <v>226</v>
+      </c>
+      <c r="M8" s="69">
         <v>20.0</v>
       </c>
       <c r="N8" s="86" t="s">
         <v>32</v>
       </c>
-      <c r="O8" s="72">
+      <c r="O8" s="69">
         <v>15.0</v>
       </c>
       <c r="P8" s="27"/>
-      <c r="Q8" s="72"/>
+      <c r="Q8" s="69"/>
       <c r="R8" s="27"/>
       <c r="S8" s="22">
         <f t="shared" si="1"/>
@@ -43018,29 +43004,29 @@
       <c r="I9" s="83">
         <v>15.0</v>
       </c>
-      <c r="J9" s="79" t="s">
+      <c r="J9" s="76" t="s">
         <v>181</v>
       </c>
       <c r="K9" s="85" t="s">
         <v>181</v>
       </c>
-      <c r="L9" s="79" t="s">
+      <c r="L9" s="76" t="s">
         <v>181</v>
       </c>
       <c r="M9" s="85" t="s">
         <v>181</v>
       </c>
-      <c r="N9" s="79" t="s">
+      <c r="N9" s="76" t="s">
         <v>181</v>
       </c>
       <c r="O9" s="85" t="s">
         <v>181</v>
       </c>
-      <c r="P9" s="79"/>
+      <c r="P9" s="76"/>
       <c r="Q9" s="85" t="s">
         <v>181</v>
       </c>
-      <c r="R9" s="79"/>
+      <c r="R9" s="76"/>
       <c r="S9" s="22">
         <f t="shared" si="1"/>
         <v>75</v>
@@ -43063,48 +43049,48 @@
       <c r="B10" s="88" t="s">
         <v>110</v>
       </c>
-      <c r="C10" s="72">
+      <c r="C10" s="69">
         <v>45.0</v>
       </c>
-      <c r="D10" s="71" t="s">
+      <c r="D10" s="68" t="s">
+        <v>230</v>
+      </c>
+      <c r="E10" s="69">
+        <v>10.0</v>
+      </c>
+      <c r="F10" s="68" t="s">
         <v>231</v>
       </c>
-      <c r="E10" s="72">
+      <c r="G10" s="69">
         <v>10.0</v>
       </c>
-      <c r="F10" s="71" t="s">
+      <c r="H10" s="68" t="s">
         <v>232</v>
       </c>
-      <c r="G10" s="72">
-        <v>10.0</v>
-      </c>
-      <c r="H10" s="71" t="s">
+      <c r="I10" s="69">
+        <v>15.0</v>
+      </c>
+      <c r="J10" s="68" t="s">
         <v>233</v>
       </c>
-      <c r="I10" s="72">
+      <c r="K10" s="69">
         <v>15.0</v>
       </c>
-      <c r="J10" s="71" t="s">
+      <c r="L10" s="68" t="s">
         <v>234</v>
       </c>
-      <c r="K10" s="72">
+      <c r="M10" s="69">
         <v>15.0</v>
       </c>
-      <c r="L10" s="71" t="s">
-        <v>235</v>
-      </c>
-      <c r="M10" s="72">
-        <v>15.0</v>
-      </c>
-      <c r="N10" s="71" t="s">
+      <c r="N10" s="68" t="s">
         <v>93</v>
       </c>
-      <c r="O10" s="72">
+      <c r="O10" s="69">
         <v>30.0</v>
       </c>
-      <c r="P10" s="71"/>
-      <c r="Q10" s="72"/>
-      <c r="R10" s="72"/>
+      <c r="P10" s="68"/>
+      <c r="Q10" s="69"/>
+      <c r="R10" s="69"/>
       <c r="S10" s="22">
         <f t="shared" si="1"/>
         <v>140</v>
@@ -43154,17 +43140,17 @@
       <c r="K11" s="90"/>
       <c r="L11" s="91"/>
       <c r="M11" s="92"/>
-      <c r="N11" s="79" t="s">
+      <c r="N11" s="76" t="s">
         <v>181</v>
       </c>
       <c r="O11" s="85" t="s">
         <v>181</v>
       </c>
-      <c r="P11" s="79"/>
+      <c r="P11" s="76"/>
       <c r="Q11" s="85" t="s">
         <v>181</v>
       </c>
-      <c r="R11" s="79"/>
+      <c r="R11" s="76"/>
       <c r="S11" s="22">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -43184,38 +43170,38 @@
       <c r="A12" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="B12" s="71" t="s">
+      <c r="B12" s="68" t="s">
         <v>76</v>
       </c>
-      <c r="C12" s="72">
+      <c r="C12" s="69">
         <v>15.0</v>
       </c>
-      <c r="D12" s="71" t="s">
+      <c r="D12" s="68" t="s">
         <v>74</v>
       </c>
-      <c r="E12" s="72">
+      <c r="E12" s="69">
         <v>20.0</v>
       </c>
-      <c r="F12" s="71" t="s">
+      <c r="F12" s="68" t="s">
         <v>77</v>
       </c>
-      <c r="G12" s="72">
+      <c r="G12" s="69">
         <v>25.0</v>
       </c>
-      <c r="H12" s="71" t="s">
+      <c r="H12" s="68" t="s">
         <v>29</v>
       </c>
-      <c r="I12" s="72">
+      <c r="I12" s="69">
         <v>20.0</v>
       </c>
-      <c r="J12" s="71" t="s">
+      <c r="J12" s="68" t="s">
         <v>42</v>
       </c>
-      <c r="K12" s="72">
+      <c r="K12" s="69">
         <v>20.0</v>
       </c>
-      <c r="L12" s="71"/>
-      <c r="M12" s="72"/>
+      <c r="L12" s="68"/>
+      <c r="M12" s="69"/>
       <c r="N12" s="27" t="s">
         <v>181</v>
       </c>
@@ -43280,17 +43266,17 @@
       </c>
       <c r="L13" s="89"/>
       <c r="M13" s="90"/>
-      <c r="N13" s="79" t="s">
+      <c r="N13" s="76" t="s">
         <v>181</v>
       </c>
       <c r="O13" s="85" t="s">
         <v>181</v>
       </c>
-      <c r="P13" s="79"/>
+      <c r="P13" s="76"/>
       <c r="Q13" s="85" t="s">
         <v>181</v>
       </c>
-      <c r="R13" s="79"/>
+      <c r="R13" s="76"/>
       <c r="S13" s="22">
         <f t="shared" si="1"/>
         <v>110</v>
@@ -43312,28 +43298,28 @@
       <c r="A14" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="B14" s="71" t="s">
+      <c r="B14" s="68" t="s">
         <v>223</v>
       </c>
-      <c r="C14" s="72">
+      <c r="C14" s="69">
         <v>25.0</v>
       </c>
-      <c r="D14" s="71" t="s">
-        <v>237</v>
-      </c>
-      <c r="E14" s="72">
+      <c r="D14" s="68" t="s">
+        <v>224</v>
+      </c>
+      <c r="E14" s="69">
         <v>25.0</v>
       </c>
-      <c r="F14" s="71" t="s">
+      <c r="F14" s="68" t="s">
         <v>97</v>
       </c>
-      <c r="G14" s="72">
+      <c r="G14" s="69">
         <v>20.0</v>
       </c>
-      <c r="H14" s="71" t="s">
+      <c r="H14" s="68" t="s">
         <v>100</v>
       </c>
-      <c r="I14" s="72">
+      <c r="I14" s="69">
         <v>35.0</v>
       </c>
       <c r="J14" s="37"/>
@@ -43390,35 +43376,35 @@
       <c r="G15" s="83">
         <v>35.0</v>
       </c>
-      <c r="H15" s="79" t="s">
+      <c r="H15" s="76" t="s">
         <v>181</v>
       </c>
       <c r="I15" s="85" t="s">
         <v>181</v>
       </c>
-      <c r="J15" s="79" t="s">
+      <c r="J15" s="76" t="s">
         <v>181</v>
       </c>
       <c r="K15" s="85" t="s">
         <v>181</v>
       </c>
-      <c r="L15" s="79" t="s">
+      <c r="L15" s="76" t="s">
         <v>181</v>
       </c>
       <c r="M15" s="85" t="s">
         <v>181</v>
       </c>
-      <c r="N15" s="79" t="s">
+      <c r="N15" s="76" t="s">
         <v>181</v>
       </c>
       <c r="O15" s="85" t="s">
         <v>181</v>
       </c>
-      <c r="P15" s="79"/>
+      <c r="P15" s="76"/>
       <c r="Q15" s="85" t="s">
         <v>181</v>
       </c>
-      <c r="R15" s="79"/>
+      <c r="R15" s="76"/>
       <c r="S15" s="22">
         <f t="shared" si="1"/>
         <v>60</v>
@@ -43596,7 +43582,7 @@
     <row r="22">
       <c r="A22" s="3"/>
       <c r="D22" s="93" t="s">
-        <v>224</v>
+        <v>236</v>
       </c>
       <c r="E22" s="94">
         <v>15.0</v>
@@ -46107,7 +46093,7 @@
       <c r="M2" s="85"/>
       <c r="N2" s="84"/>
       <c r="O2" s="85"/>
-      <c r="P2" s="79"/>
+      <c r="P2" s="76"/>
       <c r="Q2" s="22">
         <f t="shared" ref="Q2:Q17" si="1">SUM(C2,E2,G2,I2,K2,M2,O2)</f>
         <v>85</v>
@@ -46153,11 +46139,11 @@
       </c>
       <c r="J3" s="84"/>
       <c r="K3" s="85"/>
-      <c r="L3" s="79"/>
+      <c r="L3" s="76"/>
       <c r="M3" s="85"/>
-      <c r="N3" s="79"/>
+      <c r="N3" s="76"/>
       <c r="O3" s="85"/>
-      <c r="P3" s="79"/>
+      <c r="P3" s="76"/>
       <c r="Q3" s="22">
         <f t="shared" si="1"/>
         <v>85</v>
@@ -46254,13 +46240,13 @@
       <c r="M5" s="92">
         <v>10.0</v>
       </c>
-      <c r="N5" s="79" t="s">
+      <c r="N5" s="76" t="s">
         <v>181</v>
       </c>
       <c r="O5" s="85" t="s">
         <v>181</v>
       </c>
-      <c r="P5" s="79"/>
+      <c r="P5" s="76"/>
       <c r="Q5" s="22">
         <f t="shared" si="1"/>
         <v>80</v>
@@ -46366,19 +46352,19 @@
       <c r="I7" s="92"/>
       <c r="J7" s="96"/>
       <c r="K7" s="92"/>
-      <c r="L7" s="79" t="s">
+      <c r="L7" s="76" t="s">
         <v>181</v>
       </c>
       <c r="M7" s="85" t="s">
         <v>181</v>
       </c>
-      <c r="N7" s="79" t="s">
+      <c r="N7" s="76" t="s">
         <v>181</v>
       </c>
       <c r="O7" s="85" t="s">
         <v>181</v>
       </c>
-      <c r="P7" s="79"/>
+      <c r="P7" s="76"/>
       <c r="Q7" s="22">
         <f t="shared" si="1"/>
         <v>90</v>
@@ -46466,7 +46452,7 @@
       <c r="C9" s="85">
         <v>30.0</v>
       </c>
-      <c r="D9" s="79" t="s">
+      <c r="D9" s="76" t="s">
         <v>86</v>
       </c>
       <c r="E9" s="85">
@@ -46478,31 +46464,31 @@
       <c r="G9" s="92">
         <v>15.0</v>
       </c>
-      <c r="H9" s="79" t="s">
+      <c r="H9" s="76" t="s">
         <v>181</v>
       </c>
       <c r="I9" s="85" t="s">
         <v>181</v>
       </c>
-      <c r="J9" s="79" t="s">
+      <c r="J9" s="76" t="s">
         <v>181</v>
       </c>
       <c r="K9" s="85" t="s">
         <v>181</v>
       </c>
-      <c r="L9" s="79" t="s">
+      <c r="L9" s="76" t="s">
         <v>181</v>
       </c>
       <c r="M9" s="85" t="s">
         <v>181</v>
       </c>
-      <c r="N9" s="79" t="s">
+      <c r="N9" s="76" t="s">
         <v>181</v>
       </c>
       <c r="O9" s="85" t="s">
         <v>181</v>
       </c>
-      <c r="P9" s="79"/>
+      <c r="P9" s="76"/>
       <c r="Q9" s="22">
         <f t="shared" si="1"/>
         <v>75</v>
@@ -46614,13 +46600,13 @@
       <c r="K11" s="92"/>
       <c r="L11" s="91"/>
       <c r="M11" s="92"/>
-      <c r="N11" s="79" t="s">
+      <c r="N11" s="76" t="s">
         <v>181</v>
       </c>
       <c r="O11" s="85" t="s">
         <v>181</v>
       </c>
-      <c r="P11" s="79"/>
+      <c r="P11" s="76"/>
       <c r="Q11" s="22">
         <f t="shared" si="1"/>
         <v>90</v>
@@ -46704,19 +46690,19 @@
       <c r="A13" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="B13" s="79" t="s">
+      <c r="B13" s="76" t="s">
         <v>102</v>
       </c>
       <c r="C13" s="85">
         <v>10.0</v>
       </c>
-      <c r="D13" s="79" t="s">
+      <c r="D13" s="76" t="s">
         <v>103</v>
       </c>
       <c r="E13" s="85">
         <v>25.0</v>
       </c>
-      <c r="F13" s="79" t="s">
+      <c r="F13" s="76" t="s">
         <v>104</v>
       </c>
       <c r="G13" s="85">
@@ -46734,19 +46720,19 @@
       <c r="K13" s="92">
         <v>15.0</v>
       </c>
-      <c r="L13" s="79" t="s">
+      <c r="L13" s="76" t="s">
         <v>181</v>
       </c>
       <c r="M13" s="85" t="s">
         <v>181</v>
       </c>
-      <c r="N13" s="79" t="s">
+      <c r="N13" s="76" t="s">
         <v>181</v>
       </c>
       <c r="O13" s="85" t="s">
         <v>181</v>
       </c>
-      <c r="P13" s="79"/>
+      <c r="P13" s="76"/>
       <c r="Q13" s="22">
         <f t="shared" si="1"/>
         <v>90</v>
@@ -46838,37 +46824,37 @@
       <c r="E15" s="85">
         <v>20.0</v>
       </c>
-      <c r="F15" s="79" t="s">
+      <c r="F15" s="76" t="s">
         <v>181</v>
       </c>
       <c r="G15" s="85" t="s">
         <v>181</v>
       </c>
-      <c r="H15" s="79" t="s">
+      <c r="H15" s="76" t="s">
         <v>181</v>
       </c>
       <c r="I15" s="85" t="s">
         <v>181</v>
       </c>
-      <c r="J15" s="79" t="s">
+      <c r="J15" s="76" t="s">
         <v>181</v>
       </c>
       <c r="K15" s="85" t="s">
         <v>181</v>
       </c>
-      <c r="L15" s="79" t="s">
+      <c r="L15" s="76" t="s">
         <v>181</v>
       </c>
       <c r="M15" s="85" t="s">
         <v>181</v>
       </c>
-      <c r="N15" s="79" t="s">
+      <c r="N15" s="76" t="s">
         <v>181</v>
       </c>
       <c r="O15" s="85" t="s">
         <v>181</v>
       </c>
-      <c r="P15" s="79"/>
+      <c r="P15" s="76"/>
       <c r="Q15" s="22">
         <f t="shared" si="1"/>
         <v>40</v>
@@ -47046,9 +47032,9 @@
       <c r="E22" s="94">
         <v>20.0</v>
       </c>
-      <c r="H22" s="79"/>
+      <c r="H22" s="76"/>
       <c r="I22" s="85"/>
-      <c r="J22" s="79"/>
+      <c r="J22" s="76"/>
       <c r="K22" s="85"/>
       <c r="S22" s="23"/>
       <c r="T22" s="23"/>

</xml_diff>